<commit_message>
added utkonos to xlxs file for parcing
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mihail\PycharmProjects\parce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19EB7796-8DB9-4C37-9E5B-042E491E62E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD69EAF4-1E55-438A-BBE6-1757EC02771D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{FFE27364-2778-47AC-8397-2059D7069E9C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="257">
   <si>
     <t>Бренд</t>
   </si>
@@ -637,6 +637,174 @@
   </si>
   <si>
     <t>https://www.ozon.ru/product/syr-brest-litovsk-klassicheskiy-45-150-g-152141663/?asb=Tdv9tczfDa0PTKhltcp1Q6PBJg4kEMxiQyThzh5iKbU%253D&amp;asb2=gf9xWzcVUAeRvGgIa54q929unGEPpy48EadGcnul4r-wPb6gcWYx1GFdDzqUI3ln&amp;ectx=1&amp;keywords=%D0%91%D1%80%D0%B5%D1%81%D1%82+%D0%9B%D0%B8%D1%82%D0%BE%D0%B2%D1%81%D0%BA&amp;miniapp=supermarket&amp;sh=K5xV8Y4_HQ</t>
+  </si>
+  <si>
+    <t>Утконос</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3358100/pelmeni-cezar-gosudar-imperator-800-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3396163/pelmeni-cezar-carskoe-zastole-750-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3358133/pelmeni-cezar-gordost-sibiri-800-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3396159/pelmeni-cezar-sibirskie-800-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3372731/bliny-morozko-s-vetchinoj-i-syrom-zamorozhennye-420-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3057261/bliny-morozko-s-mjasom-zamorozhennye-420-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3063161/bliny-morozko-s-tvorogom-zamorozhennye-420-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3366065/picca-la-trattoria-vetchina-i-griby-zamorozhennaja-335-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3366068/picca-la-trattoria-pepperoni-zamorozhennaja-335-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3325035/griby-shampinony-morozko-green-rezanye-zamorozhennye-400-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3325041/kotlety-morozko-green-ovoshhnye-zamorozhennye</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3396152/kotlety-morozko-iz-govjadiny-zamorozhennye-330-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3396150/bifshteks-morozko-mjasnoj-zamorozhennyj-330-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3404645/kruassan-la-reine-bez-nachinki-zamorozhennye-6-shtuk-po-70-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3485105/vareniki-bratcy-vareniki-s-kartofelem-350-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3330439/vareniki-bratcy-vareniki-s-vishnej-350-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3330502/vareniki-bratcy-vareniki-s-tvorogom-350-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3403543/syr-tverdyj-kiprino-altajskij-50-250-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3403547/syr-tverdyj-kiprino-altajskij-narezka-50-125-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3403544/syr-polutverdyj-kiprino-rossijskij-50-250-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3403551/syr-polutverdyj-kiprino-rossijskij-narezka-50-125-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3403545/syr-tverdyj-kiprino-shvejcarskij-50-250-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3403548/syr-tverdyj-kiprino-shvejcarskij-narezka-50-125-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3303023/majonez-rjaba-provansal-olivkovyj-67-372-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3307178/sous-astoria-majoneznyj-syrnyj-42-233-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3307176/sous-astoria-majoneznyj-slivochno-chesnochnyj-42-233-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3412873/ketchup-astoria-tomatnyj-330-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3434057/ketchup-astoria-shashlychnyj-330-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3045260/voda-pitevaja-chernogolovka-negazirovannaja-5-l</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3481545/voda-detskaja-chernogolovka-oranzhevaja-korova-negazirovannaja-1-5-l</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3435254/napitok-chernogolovka-bajkal-silnogazirovannyj-1-25-l</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3382078/sous-sen-soy-soevyj-klassicheskij-220-ml</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3381718/lapsha-sen-soy-jaichnaja-egg-noodles-300-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3381717/lapsha-sen-soy-pshenichnaja-udon-300-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3381715/lapsha-sen-soy-grechnevaja-soba-300-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3127767/vermishel-sen-soy-funchoza-premium-200-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3381705/vermishel-sen-soy-funchoza-premium-pod-japonskim-sousom-terijaki-125-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3371208/makaronnye-izdelija-makfa-spagetti-500-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3351690/makaronnye-izdelija-makfa-vermishel-pautinka-400-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3357377/makaronnye-izdelija-makfa-spagetti-bez-gljutena-300-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3286457/gerkules-makfa-tradicionnyj-400-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3439292/khlopja-makfa-ovsjanye-bystrogo-prigotovlenija-350-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3105641/zubnaja-pasta-splat-professional-biokalcij-vosstanovlenie-emali-i-bezopasnoe-otbelivanie-100-ml</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3131886/zubnaja-pasta-splat-professional-lechebnye-travy-kompleksnaja-zashhita-100-ml</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3227951/stiralnyj-poroshok-biomio-bio-color-ekologichnyj-dlja-cvetnogo-belja-1-5-kg</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3224637/sredstvo-dlja-mytja-posudy-ovoshhej-i-fruktov-biomio-bio-care-bez-zapakha-450-ml</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3227930/sredstvo-dlja-mytja-posudy-v-posudomoechnoj-mashine-biomio-bio-total-7-v-1-s-efirnym-maslom-evkalipta-v-tabletkakh-30-shtuk</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3361973/sredstvo-dlja-mytja-stekol-zerkal-plastika-biomio-bio-glass-cleaner-bez-zapakha-sprej-500-ml</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3263798/krem-mylo-zhidkoe-detskoe-ushastyj-njan-zhidkoe-s-olivkovym-maslom-i-ekstraktom-aloe-vera-300-ml</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3288884/sredstvo-dlja-mytja-posudy-v-posudomoechnoj-mashine-ushastyj-njan-v-tabletkakh-20-shtuk</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3063096/stiralnyj-poroshok-ushastyj-njan-dlja-detskogo-belja-2-4-kg</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3062898/zubnaja-pasta-novyj-zhemchug-7-trav-ukhod-za-desnami-100-ml</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3189399/maslo-brest-litovsk-sladkoslivochnoe-nesolenoe-82-5-180-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3237864/syr-polutverdyj-brest-litovsk-klassicheskij-narezka-45-150-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3364427/syr-polutverdyj-brest-litovsk-slivochnyj-narezka-50-150-g</t>
   </si>
 </sst>
 </file>
@@ -799,7 +967,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -830,6 +998,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -1145,10 +1314,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF1A69E3-A9E5-424F-8F16-B76B324D2ACC}">
-  <dimension ref="D5:I95"/>
+  <dimension ref="D5:K95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I91" sqref="I91"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,10 +1328,11 @@
     <col min="7" max="7" width="255.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="129.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1181,8 +1351,14 @@
       <c r="I6" s="11" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="7" spans="4:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J6" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="4:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D7" s="4" t="s">
         <v>2</v>
       </c>
@@ -1195,8 +1371,14 @@
       <c r="G7" s="9" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="8" spans="4:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J7" t="s">
+        <v>202</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="4:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="4" t="s">
         <v>2</v>
       </c>
@@ -1207,8 +1389,14 @@
         <v>113</v>
       </c>
       <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="4:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J8" t="s">
+        <v>203</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="4:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D9" s="4" t="s">
         <v>2</v>
       </c>
@@ -1219,14 +1407,20 @@
         <v>115</v>
       </c>
       <c r="G9" s="9"/>
-      <c r="H9" t="s">
+      <c r="H9" s="9" t="s">
         <v>111</v>
       </c>
       <c r="I9" s="9" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="10" spans="4:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J9" t="s">
+        <v>204</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="4:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D10" s="4" t="s">
         <v>2</v>
       </c>
@@ -1240,8 +1434,14 @@
       <c r="I10" s="9" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="11" spans="4:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J10" t="s">
+        <v>205</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="4:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D11" s="4" t="s">
         <v>7</v>
       </c>
@@ -1258,8 +1458,14 @@
       <c r="I11" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="12" spans="4:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J11" t="s">
+        <v>206</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="4:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D12" s="4" t="s">
         <v>7</v>
       </c>
@@ -1272,8 +1478,14 @@
       <c r="G12" s="9" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="13" spans="4:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J12" t="s">
+        <v>207</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="4:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D13" s="4" t="s">
         <v>7</v>
       </c>
@@ -1284,8 +1496,14 @@
         <v>118</v>
       </c>
       <c r="G13" s="9"/>
-    </row>
-    <row r="14" spans="4:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J13" t="s">
+        <v>208</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="4:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D14" s="4" t="s">
         <v>11</v>
       </c>
@@ -1299,8 +1517,14 @@
       <c r="I14" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="15" spans="4:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J14" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="4:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D15" s="4" t="s">
         <v>11</v>
       </c>
@@ -1310,8 +1534,14 @@
       <c r="I15" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="16" spans="4:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J15" t="s">
+        <v>210</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="4:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D16" s="4" t="s">
         <v>14</v>
       </c>
@@ -1321,16 +1551,25 @@
       <c r="I16" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="17" spans="4:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K16" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="4:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D17" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="4:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J17" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="4:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D18" s="4" t="s">
         <v>14</v>
       </c>
@@ -1341,16 +1580,28 @@
         <v>109</v>
       </c>
       <c r="G18" s="9"/>
-    </row>
-    <row r="19" spans="4:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J18" t="s">
+        <v>212</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="4:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D19" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="4:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J19" t="s">
+        <v>213</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="4:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D20" s="4" t="s">
         <v>7</v>
       </c>
@@ -1361,16 +1612,25 @@
         <v>121</v>
       </c>
       <c r="G20" s="9"/>
-    </row>
-    <row r="21" spans="4:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J20" t="s">
+        <v>214</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="4:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D21" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="4:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K21" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="4:11" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D22" s="4" t="s">
         <v>21</v>
       </c>
@@ -1381,12 +1641,19 @@
         <v>122</v>
       </c>
       <c r="G22" s="9"/>
-    </row>
-    <row r="23" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J22" t="s">
+        <v>215</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D23" s="2"/>
       <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="4:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K23" s="3"/>
+    </row>
+    <row r="24" spans="4:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D24" s="4" t="s">
         <v>23</v>
       </c>
@@ -1398,16 +1665,28 @@
       <c r="I24" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="25" spans="4:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J24" t="s">
+        <v>216</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="4:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D25" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="4:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J25" t="s">
+        <v>217</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="4:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D26" s="4" t="s">
         <v>23</v>
       </c>
@@ -1418,40 +1697,58 @@
         <v>123</v>
       </c>
       <c r="G26" s="9"/>
-    </row>
-    <row r="27" spans="4:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J26" t="s">
+        <v>218</v>
+      </c>
+      <c r="K26" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="4:11" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D27" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="28" spans="4:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K27" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="4:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D28" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="29" spans="4:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K28" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="4:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D29" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="30" spans="4:9" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K29" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="4:11" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D30" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="31" spans="4:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K30" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="4:11" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D31" s="4" t="s">
         <v>31</v>
       </c>
@@ -1462,16 +1759,22 @@
         <v>124</v>
       </c>
       <c r="G31" s="9"/>
-    </row>
-    <row r="32" spans="4:9" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K31" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="4:11" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D32" s="7" t="s">
         <v>34</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="33" spans="4:9" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K32" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="4:11" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D33" s="4" t="s">
         <v>34</v>
       </c>
@@ -1482,24 +1785,33 @@
         <v>125</v>
       </c>
       <c r="G33" s="9"/>
-    </row>
-    <row r="34" spans="4:9" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K33" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="4:11" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D34" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="35" spans="4:9" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K34" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="4:11" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D35" s="4" t="s">
         <v>38</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="36" spans="4:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K35" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="4:11" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D36" s="4" t="s">
         <v>34</v>
       </c>
@@ -1509,12 +1821,16 @@
       <c r="I36" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="37" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K36" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D37" s="2"/>
       <c r="E37" s="3"/>
-    </row>
-    <row r="38" spans="4:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K37" s="3"/>
+    </row>
+    <row r="38" spans="4:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D38" s="4" t="s">
         <v>41</v>
       </c>
@@ -1525,8 +1841,14 @@
         <v>127</v>
       </c>
       <c r="G38" s="9"/>
-    </row>
-    <row r="39" spans="4:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J38" t="s">
+        <v>219</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="4:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D39" s="4" t="s">
         <v>41</v>
       </c>
@@ -1537,8 +1859,14 @@
         <v>126</v>
       </c>
       <c r="G39" s="9"/>
-    </row>
-    <row r="40" spans="4:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J39" t="s">
+        <v>220</v>
+      </c>
+      <c r="K39" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="4:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D40" s="4" t="s">
         <v>41</v>
       </c>
@@ -1551,24 +1879,42 @@
       <c r="G40" s="9" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="41" spans="4:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J40" t="s">
+        <v>223</v>
+      </c>
+      <c r="K40" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="4:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D41" s="4" t="s">
         <v>41</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="42" spans="4:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J41" t="s">
+        <v>224</v>
+      </c>
+      <c r="K41" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="4:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D42" s="4" t="s">
         <v>41</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="43" spans="4:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J42" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="K42" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="4:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D43" s="4" t="s">
         <v>41</v>
       </c>
@@ -1579,20 +1925,30 @@
         <v>129</v>
       </c>
       <c r="G43" s="9"/>
-    </row>
-    <row r="44" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J43" t="s">
+        <v>222</v>
+      </c>
+      <c r="K43" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D44" s="2"/>
       <c r="E44" s="3"/>
-    </row>
-    <row r="45" spans="4:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K44" s="3"/>
+    </row>
+    <row r="45" spans="4:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D45" s="4" t="s">
         <v>48</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="46" spans="4:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K45" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="4:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D46" s="4" t="s">
         <v>48</v>
       </c>
@@ -1603,8 +1959,14 @@
         <v>131</v>
       </c>
       <c r="G46" s="9"/>
-    </row>
-    <row r="47" spans="4:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J46" t="s">
+        <v>225</v>
+      </c>
+      <c r="K46" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="4:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D47" s="4" t="s">
         <v>48</v>
       </c>
@@ -1612,8 +1974,11 @@
         <v>51</v>
       </c>
       <c r="H47" s="9"/>
-    </row>
-    <row r="48" spans="4:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K47" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="4:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D48" s="4" t="s">
         <v>52</v>
       </c>
@@ -1630,8 +1995,14 @@
       <c r="I48" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="49" spans="4:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J48" t="s">
+        <v>226</v>
+      </c>
+      <c r="K48" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="49" spans="4:11" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D49" s="4" t="s">
         <v>52</v>
       </c>
@@ -1642,8 +2013,14 @@
         <v>133</v>
       </c>
       <c r="G49" s="9"/>
-    </row>
-    <row r="50" spans="4:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J49" t="s">
+        <v>227</v>
+      </c>
+      <c r="K49" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="50" spans="4:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D50" s="4" t="s">
         <v>52</v>
       </c>
@@ -1653,44 +2030,66 @@
       <c r="I50" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="51" spans="4:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J50" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="K50" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="4:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D51" s="4" t="s">
         <v>52</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="52" spans="4:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J51" t="s">
+        <v>229</v>
+      </c>
+      <c r="K51" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="52" spans="4:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D52" s="4" t="s">
         <v>57</v>
       </c>
       <c r="E52" s="5" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="53" spans="4:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K52" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53" spans="4:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D53" s="4" t="s">
         <v>57</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="54" spans="4:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K53" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54" spans="4:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D54" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="55" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K54" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="55" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D55" s="2"/>
       <c r="E55" s="3"/>
-    </row>
-    <row r="56" spans="4:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K55" s="3"/>
+    </row>
+    <row r="56" spans="4:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D56" s="4" t="s">
         <v>62</v>
       </c>
@@ -1704,16 +2103,28 @@
       <c r="I56" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="57" spans="4:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J56" t="s">
+        <v>230</v>
+      </c>
+      <c r="K56" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="57" spans="4:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="4" t="s">
         <v>62</v>
       </c>
       <c r="E57" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="58" spans="4:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J57" t="s">
+        <v>231</v>
+      </c>
+      <c r="K57" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="58" spans="4:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="4" t="s">
         <v>62</v>
       </c>
@@ -1726,15 +2137,22 @@
       <c r="I58" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="59" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J58" t="s">
+        <v>232</v>
+      </c>
+      <c r="K58" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="59" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D59" s="2"/>
       <c r="E59" s="3"/>
       <c r="I59" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="60" spans="4:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K59" s="3"/>
+    </row>
+    <row r="60" spans="4:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D60" s="4" t="s">
         <v>66</v>
       </c>
@@ -1748,16 +2166,28 @@
       <c r="I60" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="61" spans="4:9" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J60" t="s">
+        <v>233</v>
+      </c>
+      <c r="K60" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="61" spans="4:11" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D61" s="4" t="s">
         <v>66</v>
       </c>
       <c r="E61" s="5" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="62" spans="4:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J61" t="s">
+        <v>234</v>
+      </c>
+      <c r="K61" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="62" spans="4:11" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D62" s="4" t="s">
         <v>66</v>
       </c>
@@ -1767,8 +2197,14 @@
       <c r="I62" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="63" spans="4:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J62" t="s">
+        <v>235</v>
+      </c>
+      <c r="K62" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="63" spans="4:11" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D63" s="4" t="s">
         <v>66</v>
       </c>
@@ -1778,8 +2214,14 @@
       <c r="I63" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="64" spans="4:9" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J63" t="s">
+        <v>236</v>
+      </c>
+      <c r="K63" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="64" spans="4:11" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D64" s="4" t="s">
         <v>66</v>
       </c>
@@ -1792,8 +2234,14 @@
       <c r="I64" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="65" spans="4:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J64" t="s">
+        <v>237</v>
+      </c>
+      <c r="K64" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="65" spans="4:11" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D65" s="4" t="s">
         <v>66</v>
       </c>
@@ -1806,8 +2254,14 @@
       <c r="I65" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="66" spans="4:9" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J65" t="s">
+        <v>238</v>
+      </c>
+      <c r="K65" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="66" spans="4:11" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D66" s="4" t="s">
         <v>66</v>
       </c>
@@ -1820,15 +2274,19 @@
       <c r="I66" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="67" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K66" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="67" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D67" s="2"/>
       <c r="E67" s="3"/>
       <c r="I67" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="68" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K67" s="3"/>
+    </row>
+    <row r="68" spans="4:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D68" s="4" t="s">
         <v>74</v>
       </c>
@@ -1838,8 +2296,14 @@
       <c r="G68" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="69" spans="4:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J68" t="s">
+        <v>239</v>
+      </c>
+      <c r="K68" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="69" spans="4:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D69" s="4" t="s">
         <v>74</v>
       </c>
@@ -1852,8 +2316,14 @@
       <c r="G69" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="70" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J69" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="K69" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="70" spans="4:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D70" s="4" t="s">
         <v>74</v>
       </c>
@@ -1863,8 +2333,11 @@
       <c r="I70" s="9" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="71" spans="4:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K70" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="71" spans="4:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D71" s="4" t="s">
         <v>74</v>
       </c>
@@ -1880,8 +2353,14 @@
       <c r="I71" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="72" spans="4:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J71" t="s">
+        <v>241</v>
+      </c>
+      <c r="K71" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="72" spans="4:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D72" s="4" t="s">
         <v>74</v>
       </c>
@@ -1894,8 +2373,11 @@
       <c r="I72" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="73" spans="4:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K72" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="73" spans="4:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D73" s="4" t="s">
         <v>74</v>
       </c>
@@ -1905,8 +2387,14 @@
       <c r="I73" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="74" spans="4:9" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J73" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="K73" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="74" spans="4:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D74" s="4" t="s">
         <v>74</v>
       </c>
@@ -1916,15 +2404,22 @@
       <c r="H74" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="75" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J74" t="s">
+        <v>243</v>
+      </c>
+      <c r="K74" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="75" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D75" s="2"/>
       <c r="E75" s="3"/>
       <c r="I75" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="76" spans="4:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K75" s="3"/>
+    </row>
+    <row r="76" spans="4:11" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D76" s="4" t="s">
         <v>82</v>
       </c>
@@ -1937,8 +2432,14 @@
       <c r="G76" s="9" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="77" spans="4:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J76" t="s">
+        <v>244</v>
+      </c>
+      <c r="K76" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="77" spans="4:11" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D77" s="4" t="s">
         <v>82</v>
       </c>
@@ -1949,8 +2450,14 @@
         <v>140</v>
       </c>
       <c r="G77" s="9"/>
-    </row>
-    <row r="78" spans="4:9" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J77" t="s">
+        <v>245</v>
+      </c>
+      <c r="K77" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="78" spans="4:11" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D78" s="4" t="s">
         <v>85</v>
       </c>
@@ -1967,8 +2474,11 @@
       <c r="I78" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="79" spans="4:9" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K78" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="79" spans="4:11" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D79" s="4" t="s">
         <v>85</v>
       </c>
@@ -1982,8 +2492,14 @@
       <c r="H79" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="80" spans="4:9" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J79" t="s">
+        <v>246</v>
+      </c>
+      <c r="K79" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="80" spans="4:11" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D80" s="4" t="s">
         <v>85</v>
       </c>
@@ -1996,8 +2512,14 @@
       <c r="I80" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="81" spans="4:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J80" t="s">
+        <v>247</v>
+      </c>
+      <c r="K80" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="81" spans="4:11" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D81" s="4" t="s">
         <v>85</v>
       </c>
@@ -2010,8 +2532,14 @@
       <c r="I81" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="82" spans="4:9" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J81" t="s">
+        <v>248</v>
+      </c>
+      <c r="K81" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="82" spans="4:11" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D82" s="4" t="s">
         <v>85</v>
       </c>
@@ -2025,15 +2553,22 @@
       <c r="I82" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="83" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J82" t="s">
+        <v>249</v>
+      </c>
+      <c r="K82" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="83" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D83" s="2"/>
       <c r="E83" s="3"/>
       <c r="I83" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="84" spans="4:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K83" s="3"/>
+    </row>
+    <row r="84" spans="4:11" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D84" s="4" t="s">
         <v>91</v>
       </c>
@@ -2049,16 +2584,25 @@
       <c r="I84" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="85" spans="4:9" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J84" t="s">
+        <v>250</v>
+      </c>
+      <c r="K84" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="85" spans="4:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D85" s="4" t="s">
         <v>91</v>
       </c>
       <c r="E85" s="5" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="86" spans="4:9" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K85" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="86" spans="4:11" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D86" s="4" t="s">
         <v>91</v>
       </c>
@@ -2068,8 +2612,14 @@
       <c r="I86" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="87" spans="4:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J86" t="s">
+        <v>251</v>
+      </c>
+      <c r="K86" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="87" spans="4:11" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D87" s="4" t="s">
         <v>91</v>
       </c>
@@ -2079,16 +2629,25 @@
       <c r="I87" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="88" spans="4:9" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J87" t="s">
+        <v>252</v>
+      </c>
+      <c r="K87" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="88" spans="4:11" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D88" s="4" t="s">
         <v>96</v>
       </c>
       <c r="E88" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="89" spans="4:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K88" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="89" spans="4:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D89" s="4" t="s">
         <v>98</v>
       </c>
@@ -2098,15 +2657,22 @@
       <c r="I89" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="90" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J89" t="s">
+        <v>253</v>
+      </c>
+      <c r="K89" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="90" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D90" s="2"/>
       <c r="E90" s="3"/>
       <c r="I90" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="91" spans="4:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K90" s="3"/>
+    </row>
+    <row r="91" spans="4:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D91" s="4" t="s">
         <v>100</v>
       </c>
@@ -2116,16 +2682,25 @@
       <c r="I91" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="92" spans="4:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K91" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="92" spans="4:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D92" s="4" t="s">
         <v>100</v>
       </c>
       <c r="E92" s="5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="93" spans="4:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J92" t="s">
+        <v>254</v>
+      </c>
+      <c r="K92" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="93" spans="4:11" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D93" s="4" t="s">
         <v>100</v>
       </c>
@@ -2136,8 +2711,14 @@
       <c r="G93" s="9" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="94" spans="4:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J93" t="s">
+        <v>255</v>
+      </c>
+      <c r="K93" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="94" spans="4:11" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D94" s="4" t="s">
         <v>100</v>
       </c>
@@ -2147,8 +2728,14 @@
       <c r="I94" s="9" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="95" spans="4:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J94" t="s">
+        <v>256</v>
+      </c>
+      <c r="K94" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="95" spans="4:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D95" s="4" t="s">
         <v>100</v>
       </c>
@@ -2160,6 +2747,9 @@
       </c>
       <c r="I95" s="9" t="s">
         <v>200</v>
+      </c>
+      <c r="K95" s="5" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2198,8 +2788,17 @@
     <hyperlink ref="I10" r:id="rId31" xr:uid="{715D8978-E09F-4537-A640-856992E7F8CB}"/>
     <hyperlink ref="I95" r:id="rId32" display="https://www.ozon.ru/product/syr-brest-litovsk-klassicheskiy-45-150-g-152141663/?asb=Tdv9tczfDa0PTKhltcp1Q6PBJg4kEMxiQyThzh5iKbU%253D&amp;asb2=gf9xWzcVUAeRvGgIa54q929unGEPpy48EadGcnul4r-wPb6gcWYx1GFdDzqUI3ln&amp;ectx=1&amp;keywords=%D0%91%D1%80%D0%B5%D1%81%D1%82+%D0%9B%D0%B8%D1%82%D0%BE%D0%B2%D1%81%D0%BA&amp;miniapp=supermarket&amp;sh=K5xV8Y4_HQ" xr:uid="{EA030594-B44A-4F70-BE65-1EAA753D15CB}"/>
     <hyperlink ref="I94" r:id="rId33" display="https://www.ozon.ru/product/brest-litovsk-maslo-sladko-slivochnoe-nesolenoe-82-5-180-g-145923184/?asb=jIkcWaZ8F2DraHiq9EkWSqHPHpJGeby2dptq6D3zZMw%253D&amp;asb2=jU54E3oIkNKIgSViutQjlT_4Mgd1c3ms7hb00oP7TOiu8wiJapREib7WfJBxMz2F&amp;ectx=1&amp;keywords=%D0%91%D1%80%D0%B5%D1%81%D1%82+%D0%9B%D0%B8%D1%82%D0%BE%D0%B2%D1%81%D0%BA&amp;miniapp=supermarket&amp;sh=K5xV8Xe3Fg" xr:uid="{B8E2B196-F6B7-4B8D-B1DC-360FE9199845}"/>
+    <hyperlink ref="H9" r:id="rId34" xr:uid="{018BC0E8-7D36-4FDC-B01F-961CF1BAB866}"/>
+    <hyperlink ref="G7" r:id="rId35" display="https://lavka.yandex.ru/213/good/b01a29d7997948658686098667c64a1e000300010000?searchQuery=%D0%A6%D0%B5%D0%B7%D0%B0%D1%80%D1%8C%20%D0%B3%D0%BE%D1%81%D1%83%D0%B4%D0%B0%D1%80%D1%8C%20%D0%B8%D0%BC%D0%BF%D0%B5%D1%80%D0%B0%D1%82%D0%BE%D1%80%20800%20%D0%B3&amp;searchPosition=-1" xr:uid="{E1D5F1F2-7D41-4892-BB76-421E3FAE8527}"/>
+    <hyperlink ref="G12" r:id="rId36" xr:uid="{AF577DF4-4728-48AF-A65A-2285548B425E}"/>
+    <hyperlink ref="J14" r:id="rId37" xr:uid="{E3ADEC76-6366-47CD-B97C-D6EF83C1141B}"/>
+    <hyperlink ref="J17" r:id="rId38" xr:uid="{28F53E34-2BE7-45DE-A4C8-DE5703380BA0}"/>
+    <hyperlink ref="J42" r:id="rId39" xr:uid="{7B711258-2660-4291-8B28-70B42D0DCF9C}"/>
+    <hyperlink ref="J50" r:id="rId40" xr:uid="{C121E486-6DC5-4AB8-BDD6-D4F32794A3A4}"/>
+    <hyperlink ref="J69" r:id="rId41" xr:uid="{7F316388-2C20-4908-B372-14903C2E8EAA}"/>
+    <hyperlink ref="J73" r:id="rId42" xr:uid="{851CBC7D-F6E3-4C94-816D-5E4B54BC54F2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId34"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId43"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added auchan to db
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mihail\PycharmProjects\parce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD69EAF4-1E55-438A-BBE6-1757EC02771D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95EA9A6-25FF-4B3A-AB8E-1F6D89EE10F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{FFE27364-2778-47AC-8397-2059D7069E9C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="292">
   <si>
     <t>Бренд</t>
   </si>
@@ -805,6 +805,111 @@
   </si>
   <si>
     <t>https://www.utkonos.ru/item/3364427/syr-polutverdyj-brest-litovsk-slivochnyj-narezka-50-150-g</t>
+  </si>
+  <si>
+    <t>Ашан</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ru/product/pelmeni-cezar-gosudar-imperator-800-g/</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ru/product/pelmcarszastcezar_750gr/</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ru/product/pelmeni-cezar-gordost-sibiri-800-g/</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ru/product/pelmeni-cezar-sibirskie-gost-800-g/</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ru/product/blinys_vetsyr_morozko420gr/</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ru/product/bliny-morozko-s-myasom-molodyh-bychkov-420-g/</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ru/product/picca-la-trattoria-s-vetchinoy-i-gribami-335-g/</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ru/product/kotlety-morozko-kievskie-600-g/</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ru/product/kruassany-la-reine-bez-nachinki-420-g/</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ru/product/shnicel-sytoedov-s-kartofelnym-pyure-pod-krasnym-sousom-350-g/</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ru/product/chebureki-chebureche-s-govyadinoy-i-svininoy-280-g/</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ru/product/syr-tverdyy-kiprino-altayskiy-250-g/</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ru/product/syr-tverdyy-kiprino-altayskiy-narezka-50-125-g/</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ru/product/syr_shveycarskiy_50_narez125g/</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ru/product/mayonez-ryaba-provansal-olivkovyy-67-372-g/</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ru/product/mayonez-ryaba-provansal-67-400-g/</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ru/product/sous-mayoneznyy-astoria-syrnyy-42-233-ml/</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ru/product/sous-mayoneznyy-astoria-slivochno-chesnochnyy-42-233-g/</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ru/product/margarin-hozyayushka-nizhegorodskiy-slivochnyy-60-200-g/</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ru/product/voda-chernogolovskaya-bez-gaza-plastik-5-l/</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ru/product/chernogolovka_dyushes_125_pet/</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ru/product/sous-soevyy-sen-soy-premium-klassicheskiy-220-ml/</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ru/product/lapsha-sen-soy-soba-grechnevaya-300-g/</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ru/product/vermishel-sen-soy-funchoza-premium-200-g/</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ru/product/makarony-makfa-spagetti-vermishel-500-g/</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ru/product/makaronnye-izdeliya-makfa-pautinka-450-g/</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ru/product/muka-pshenichnaya-makfa-vysshtiy-sort-2-kg/</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ru/product/sredstvo-dlya-mytya-posudy-ovoshchey-i-fruktov-biomio-s-efirnym-maslom-mandarina-450-ml/</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ru/product/tabletki-dlya-posudomoechnoy-mashiny-ushastyy-nyan-20-sht/</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ru/product/stiralnyy-poroshok-dlya-detskogo-belya-ushastyy-nyan-2-4-kg/</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ru/product/maslo-brest-litovsk-sladko-slivochnoe-nesolenoe-82-5-180g/</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ru/product/syr-brest-litovsk-klassicheskiy-narezannyy-45-150-g/</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ru/product/syr-polutverdyy-brest-litovsk-50-slivochnyy-narezka-150-g/</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ru/product/syr-polutverdyy-brest-litovsk-rossiyskiy-50-narezka-150-g/</t>
   </si>
 </sst>
 </file>
@@ -866,7 +971,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -962,12 +1067,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -999,6 +1115,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -1314,10 +1433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF1A69E3-A9E5-424F-8F16-B76B324D2ACC}">
-  <dimension ref="D5:K95"/>
+  <dimension ref="D5:L95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="J88" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M95" sqref="M95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1328,11 +1447,11 @@
     <col min="7" max="7" width="255.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="129.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1354,11 +1473,14 @@
       <c r="J6" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="K6" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="L6" s="13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="4:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D7" s="4" t="s">
         <v>2</v>
       </c>
@@ -1374,11 +1496,14 @@
       <c r="J7" t="s">
         <v>202</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K7" t="s">
+        <v>258</v>
+      </c>
+      <c r="L7" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="4:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="4" t="s">
         <v>2</v>
       </c>
@@ -1392,11 +1517,14 @@
       <c r="J8" t="s">
         <v>203</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="K8" t="s">
+        <v>259</v>
+      </c>
+      <c r="L8" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="4:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D9" s="4" t="s">
         <v>2</v>
       </c>
@@ -1416,11 +1544,14 @@
       <c r="J9" t="s">
         <v>204</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="K9" t="s">
+        <v>260</v>
+      </c>
+      <c r="L9" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="4:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D10" s="4" t="s">
         <v>2</v>
       </c>
@@ -1437,11 +1568,14 @@
       <c r="J10" t="s">
         <v>205</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="K10" t="s">
+        <v>261</v>
+      </c>
+      <c r="L10" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="4:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D11" s="4" t="s">
         <v>7</v>
       </c>
@@ -1461,11 +1595,14 @@
       <c r="J11" t="s">
         <v>206</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="K11" t="s">
+        <v>262</v>
+      </c>
+      <c r="L11" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="4:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D12" s="4" t="s">
         <v>7</v>
       </c>
@@ -1481,11 +1618,14 @@
       <c r="J12" t="s">
         <v>207</v>
       </c>
-      <c r="K12" s="5" t="s">
+      <c r="K12" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="L12" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="4:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D13" s="4" t="s">
         <v>7</v>
       </c>
@@ -1499,11 +1639,11 @@
       <c r="J13" t="s">
         <v>208</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="L13" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="4:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D14" s="4" t="s">
         <v>11</v>
       </c>
@@ -1520,11 +1660,14 @@
       <c r="J14" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="K14" s="5" t="s">
+      <c r="K14" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="L14" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="4:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D15" s="4" t="s">
         <v>11</v>
       </c>
@@ -1537,11 +1680,11 @@
       <c r="J15" t="s">
         <v>210</v>
       </c>
-      <c r="K15" s="5" t="s">
+      <c r="L15" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="4:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D16" s="4" t="s">
         <v>14</v>
       </c>
@@ -1551,11 +1694,11 @@
       <c r="I16" t="s">
         <v>169</v>
       </c>
-      <c r="K16" s="5" t="s">
+      <c r="L16" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="4:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D17" s="4" t="s">
         <v>14</v>
       </c>
@@ -1565,11 +1708,12 @@
       <c r="J17" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="K17" s="9"/>
+      <c r="L17" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="4:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D18" s="4" t="s">
         <v>14</v>
       </c>
@@ -1583,11 +1727,11 @@
       <c r="J18" t="s">
         <v>212</v>
       </c>
-      <c r="K18" s="5" t="s">
+      <c r="L18" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="4:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D19" s="4" t="s">
         <v>7</v>
       </c>
@@ -1597,11 +1741,11 @@
       <c r="J19" t="s">
         <v>213</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="L19" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="4:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D20" s="4" t="s">
         <v>7</v>
       </c>
@@ -1615,22 +1759,25 @@
       <c r="J20" t="s">
         <v>214</v>
       </c>
-      <c r="K20" s="5" t="s">
+      <c r="L20" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="4:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D21" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K21" s="5" t="s">
+      <c r="K21" t="s">
+        <v>265</v>
+      </c>
+      <c r="L21" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="4:11" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D22" s="4" t="s">
         <v>21</v>
       </c>
@@ -1644,16 +1791,19 @@
       <c r="J22" t="s">
         <v>215</v>
       </c>
-      <c r="K22" s="5" t="s">
+      <c r="K22" t="s">
+        <v>266</v>
+      </c>
+      <c r="L22" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D23" s="2"/>
       <c r="E23" s="3"/>
-      <c r="K23" s="3"/>
-    </row>
-    <row r="24" spans="4:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L23" s="3"/>
+    </row>
+    <row r="24" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D24" s="4" t="s">
         <v>23</v>
       </c>
@@ -1668,11 +1818,11 @@
       <c r="J24" t="s">
         <v>216</v>
       </c>
-      <c r="K24" s="5" t="s">
+      <c r="L24" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="4:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D25" s="4" t="s">
         <v>23</v>
       </c>
@@ -1682,11 +1832,11 @@
       <c r="J25" t="s">
         <v>217</v>
       </c>
-      <c r="K25" s="5" t="s">
+      <c r="L25" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="4:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D26" s="4" t="s">
         <v>23</v>
       </c>
@@ -1700,55 +1850,55 @@
       <c r="J26" t="s">
         <v>218</v>
       </c>
-      <c r="K26" s="5" t="s">
+      <c r="L26" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="4:11" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D27" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K27" s="5" t="s">
+      <c r="L27" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="4:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D28" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="K28" s="5" t="s">
+      <c r="L28" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="4:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D29" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="K29" s="5" t="s">
+      <c r="L29" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="4:11" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D30" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="K30" s="5" t="s">
+      <c r="L30" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="4:11" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D31" s="4" t="s">
         <v>31</v>
       </c>
@@ -1759,22 +1909,22 @@
         <v>124</v>
       </c>
       <c r="G31" s="9"/>
-      <c r="K31" s="5" t="s">
+      <c r="L31" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="4:11" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D32" s="7" t="s">
         <v>34</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="K32" s="8" t="s">
+      <c r="L32" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="4:11" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:12" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D33" s="4" t="s">
         <v>34</v>
       </c>
@@ -1785,33 +1935,39 @@
         <v>125</v>
       </c>
       <c r="G33" s="9"/>
-      <c r="K33" s="5" t="s">
+      <c r="K33" t="s">
+        <v>267</v>
+      </c>
+      <c r="L33" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="4:11" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:12" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D34" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="K34" s="5" t="s">
+      <c r="L34" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="4:11" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D35" s="4" t="s">
         <v>38</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="K35" s="5" t="s">
+      <c r="K35" t="s">
+        <v>268</v>
+      </c>
+      <c r="L35" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="4:11" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D36" s="4" t="s">
         <v>34</v>
       </c>
@@ -1821,16 +1977,16 @@
       <c r="I36" t="s">
         <v>171</v>
       </c>
-      <c r="K36" s="5" t="s">
+      <c r="L36" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D37" s="2"/>
       <c r="E37" s="3"/>
-      <c r="K37" s="3"/>
-    </row>
-    <row r="38" spans="4:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L37" s="3"/>
+    </row>
+    <row r="38" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D38" s="4" t="s">
         <v>41</v>
       </c>
@@ -1844,11 +2000,14 @@
       <c r="J38" t="s">
         <v>219</v>
       </c>
-      <c r="K38" s="5" t="s">
+      <c r="K38" t="s">
+        <v>269</v>
+      </c>
+      <c r="L38" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="4:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D39" s="4" t="s">
         <v>41</v>
       </c>
@@ -1862,11 +2021,14 @@
       <c r="J39" t="s">
         <v>220</v>
       </c>
-      <c r="K39" s="5" t="s">
+      <c r="K39" t="s">
+        <v>270</v>
+      </c>
+      <c r="L39" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="4:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D40" s="4" t="s">
         <v>41</v>
       </c>
@@ -1882,11 +2044,11 @@
       <c r="J40" t="s">
         <v>223</v>
       </c>
-      <c r="K40" s="5" t="s">
+      <c r="L40" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="4:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D41" s="4" t="s">
         <v>41</v>
       </c>
@@ -1896,11 +2058,14 @@
       <c r="J41" t="s">
         <v>224</v>
       </c>
-      <c r="K41" s="5" t="s">
+      <c r="K41" t="s">
+        <v>271</v>
+      </c>
+      <c r="L41" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="4:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D42" s="4" t="s">
         <v>41</v>
       </c>
@@ -1910,11 +2075,12 @@
       <c r="J42" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="K42" s="5" t="s">
+      <c r="K42" s="9"/>
+      <c r="L42" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="43" spans="4:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D43" s="4" t="s">
         <v>41</v>
       </c>
@@ -1928,27 +2094,30 @@
       <c r="J43" t="s">
         <v>222</v>
       </c>
-      <c r="K43" s="5" t="s">
+      <c r="L43" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D44" s="2"/>
       <c r="E44" s="3"/>
-      <c r="K44" s="3"/>
-    </row>
-    <row r="45" spans="4:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L44" s="3"/>
+    </row>
+    <row r="45" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D45" s="4" t="s">
         <v>48</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="K45" s="5" t="s">
+      <c r="K45" t="s">
+        <v>273</v>
+      </c>
+      <c r="L45" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="4:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D46" s="4" t="s">
         <v>48</v>
       </c>
@@ -1962,11 +2131,14 @@
       <c r="J46" t="s">
         <v>225</v>
       </c>
-      <c r="K46" s="5" t="s">
+      <c r="K46" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="L46" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="4:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D47" s="4" t="s">
         <v>48</v>
       </c>
@@ -1974,11 +2146,11 @@
         <v>51</v>
       </c>
       <c r="H47" s="9"/>
-      <c r="K47" s="5" t="s">
+      <c r="L47" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="48" spans="4:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D48" s="4" t="s">
         <v>52</v>
       </c>
@@ -1998,11 +2170,14 @@
       <c r="J48" t="s">
         <v>226</v>
       </c>
-      <c r="K48" s="5" t="s">
+      <c r="K48" t="s">
+        <v>274</v>
+      </c>
+      <c r="L48" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="4:11" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D49" s="4" t="s">
         <v>52</v>
       </c>
@@ -2016,11 +2191,14 @@
       <c r="J49" t="s">
         <v>227</v>
       </c>
-      <c r="K49" s="5" t="s">
+      <c r="K49" t="s">
+        <v>275</v>
+      </c>
+      <c r="L49" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="4:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D50" s="4" t="s">
         <v>52</v>
       </c>
@@ -2033,11 +2211,12 @@
       <c r="J50" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="K50" s="5" t="s">
+      <c r="K50" s="9"/>
+      <c r="L50" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="4:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D51" s="4" t="s">
         <v>52</v>
       </c>
@@ -2047,49 +2226,52 @@
       <c r="J51" t="s">
         <v>229</v>
       </c>
-      <c r="K51" s="5" t="s">
+      <c r="L51" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="52" spans="4:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D52" s="4" t="s">
         <v>57</v>
       </c>
       <c r="E52" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="K52" s="5" t="s">
+      <c r="K52" t="s">
+        <v>276</v>
+      </c>
+      <c r="L52" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="53" spans="4:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D53" s="4" t="s">
         <v>57</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="K53" s="5" t="s">
+      <c r="L53" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="54" spans="4:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D54" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="K54" s="5" t="s">
+      <c r="L54" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="55" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D55" s="2"/>
       <c r="E55" s="3"/>
-      <c r="K55" s="3"/>
-    </row>
-    <row r="56" spans="4:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L55" s="3"/>
+    </row>
+    <row r="56" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D56" s="4" t="s">
         <v>62</v>
       </c>
@@ -2106,11 +2288,14 @@
       <c r="J56" t="s">
         <v>230</v>
       </c>
-      <c r="K56" s="5" t="s">
+      <c r="K56" t="s">
+        <v>277</v>
+      </c>
+      <c r="L56" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="57" spans="4:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="4" t="s">
         <v>62</v>
       </c>
@@ -2120,11 +2305,11 @@
       <c r="J57" t="s">
         <v>231</v>
       </c>
-      <c r="K57" s="5" t="s">
+      <c r="L57" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="58" spans="4:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="4" t="s">
         <v>62</v>
       </c>
@@ -2140,19 +2325,22 @@
       <c r="J58" t="s">
         <v>232</v>
       </c>
-      <c r="K58" s="5" t="s">
+      <c r="K58" t="s">
+        <v>278</v>
+      </c>
+      <c r="L58" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="59" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D59" s="2"/>
       <c r="E59" s="3"/>
       <c r="I59" t="s">
         <v>175</v>
       </c>
-      <c r="K59" s="3"/>
-    </row>
-    <row r="60" spans="4:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L59" s="3"/>
+    </row>
+    <row r="60" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D60" s="4" t="s">
         <v>66</v>
       </c>
@@ -2166,14 +2354,17 @@
       <c r="I60" t="s">
         <v>176</v>
       </c>
-      <c r="J60" t="s">
+      <c r="J60" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="K60" s="5" t="s">
+      <c r="K60" t="s">
+        <v>279</v>
+      </c>
+      <c r="L60" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="61" spans="4:11" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="4:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D61" s="4" t="s">
         <v>66</v>
       </c>
@@ -2183,11 +2374,11 @@
       <c r="J61" t="s">
         <v>234</v>
       </c>
-      <c r="K61" s="5" t="s">
+      <c r="L61" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="62" spans="4:11" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D62" s="4" t="s">
         <v>66</v>
       </c>
@@ -2200,11 +2391,11 @@
       <c r="J62" t="s">
         <v>235</v>
       </c>
-      <c r="K62" s="5" t="s">
+      <c r="L62" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="63" spans="4:11" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D63" s="4" t="s">
         <v>66</v>
       </c>
@@ -2217,11 +2408,14 @@
       <c r="J63" t="s">
         <v>236</v>
       </c>
-      <c r="K63" s="5" t="s">
+      <c r="K63" t="s">
+        <v>280</v>
+      </c>
+      <c r="L63" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="64" spans="4:11" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="4:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D64" s="4" t="s">
         <v>66</v>
       </c>
@@ -2237,11 +2431,14 @@
       <c r="J64" t="s">
         <v>237</v>
       </c>
-      <c r="K64" s="5" t="s">
+      <c r="K64" t="s">
+        <v>281</v>
+      </c>
+      <c r="L64" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="65" spans="4:11" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="4:12" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D65" s="4" t="s">
         <v>66</v>
       </c>
@@ -2257,11 +2454,11 @@
       <c r="J65" t="s">
         <v>238</v>
       </c>
-      <c r="K65" s="5" t="s">
+      <c r="L65" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="4:11" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="4:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D66" s="4" t="s">
         <v>66</v>
       </c>
@@ -2274,19 +2471,19 @@
       <c r="I66" t="s">
         <v>181</v>
       </c>
-      <c r="K66" s="5" t="s">
+      <c r="L66" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D67" s="2"/>
       <c r="E67" s="3"/>
       <c r="I67" t="s">
         <v>182</v>
       </c>
-      <c r="K67" s="3"/>
-    </row>
-    <row r="68" spans="4:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L67" s="3"/>
+    </row>
+    <row r="68" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D68" s="4" t="s">
         <v>74</v>
       </c>
@@ -2299,11 +2496,14 @@
       <c r="J68" t="s">
         <v>239</v>
       </c>
-      <c r="K68" s="5" t="s">
+      <c r="K68" t="s">
+        <v>282</v>
+      </c>
+      <c r="L68" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="69" spans="4:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D69" s="4" t="s">
         <v>74</v>
       </c>
@@ -2319,11 +2519,14 @@
       <c r="J69" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="K69" s="5" t="s">
+      <c r="K69" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="L69" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="70" spans="4:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D70" s="4" t="s">
         <v>74</v>
       </c>
@@ -2333,11 +2536,11 @@
       <c r="I70" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="K70" s="5" t="s">
+      <c r="L70" s="5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="71" spans="4:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D71" s="4" t="s">
         <v>74</v>
       </c>
@@ -2356,11 +2559,11 @@
       <c r="J71" t="s">
         <v>241</v>
       </c>
-      <c r="K71" s="5" t="s">
+      <c r="L71" s="5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="72" spans="4:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D72" s="4" t="s">
         <v>74</v>
       </c>
@@ -2373,11 +2576,14 @@
       <c r="I72" t="s">
         <v>185</v>
       </c>
-      <c r="K72" s="5" t="s">
+      <c r="K72" t="s">
+        <v>284</v>
+      </c>
+      <c r="L72" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="73" spans="4:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D73" s="4" t="s">
         <v>74</v>
       </c>
@@ -2390,11 +2596,12 @@
       <c r="J73" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="K73" s="5" t="s">
+      <c r="K73" s="9"/>
+      <c r="L73" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="74" spans="4:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D74" s="4" t="s">
         <v>74</v>
       </c>
@@ -2407,19 +2614,19 @@
       <c r="J74" t="s">
         <v>243</v>
       </c>
-      <c r="K74" s="5" t="s">
+      <c r="L74" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="75" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D75" s="2"/>
       <c r="E75" s="3"/>
       <c r="I75" t="s">
         <v>187</v>
       </c>
-      <c r="K75" s="3"/>
-    </row>
-    <row r="76" spans="4:11" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L75" s="3"/>
+    </row>
+    <row r="76" spans="4:12" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D76" s="4" t="s">
         <v>82</v>
       </c>
@@ -2435,11 +2642,11 @@
       <c r="J76" t="s">
         <v>244</v>
       </c>
-      <c r="K76" s="5" t="s">
+      <c r="L76" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="77" spans="4:11" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="4:12" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D77" s="4" t="s">
         <v>82</v>
       </c>
@@ -2453,11 +2660,11 @@
       <c r="J77" t="s">
         <v>245</v>
       </c>
-      <c r="K77" s="5" t="s">
+      <c r="L77" s="5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="78" spans="4:11" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="4:12" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D78" s="4" t="s">
         <v>85</v>
       </c>
@@ -2474,11 +2681,11 @@
       <c r="I78" t="s">
         <v>188</v>
       </c>
-      <c r="K78" s="5" t="s">
+      <c r="L78" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="79" spans="4:11" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="4:12" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D79" s="4" t="s">
         <v>85</v>
       </c>
@@ -2495,11 +2702,11 @@
       <c r="J79" t="s">
         <v>246</v>
       </c>
-      <c r="K79" s="5" t="s">
+      <c r="L79" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="80" spans="4:11" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="4:12" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D80" s="4" t="s">
         <v>85</v>
       </c>
@@ -2515,11 +2722,14 @@
       <c r="J80" t="s">
         <v>247</v>
       </c>
-      <c r="K80" s="5" t="s">
+      <c r="K80" t="s">
+        <v>285</v>
+      </c>
+      <c r="L80" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="81" spans="4:11" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="4:12" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D81" s="4" t="s">
         <v>85</v>
       </c>
@@ -2535,11 +2745,11 @@
       <c r="J81" t="s">
         <v>248</v>
       </c>
-      <c r="K81" s="5" t="s">
+      <c r="L81" s="5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="82" spans="4:11" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="4:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D82" s="4" t="s">
         <v>85</v>
       </c>
@@ -2556,19 +2766,19 @@
       <c r="J82" t="s">
         <v>249</v>
       </c>
-      <c r="K82" s="5" t="s">
+      <c r="L82" s="5" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="83" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D83" s="2"/>
       <c r="E83" s="3"/>
       <c r="I83" t="s">
         <v>192</v>
       </c>
-      <c r="K83" s="3"/>
-    </row>
-    <row r="84" spans="4:11" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L83" s="3"/>
+    </row>
+    <row r="84" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D84" s="4" t="s">
         <v>91</v>
       </c>
@@ -2587,22 +2797,22 @@
       <c r="J84" t="s">
         <v>250</v>
       </c>
-      <c r="K84" s="5" t="s">
+      <c r="L84" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="85" spans="4:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D85" s="4" t="s">
         <v>91</v>
       </c>
       <c r="E85" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="K85" s="5" t="s">
+      <c r="L85" s="5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="86" spans="4:11" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="4:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D86" s="4" t="s">
         <v>91</v>
       </c>
@@ -2615,11 +2825,14 @@
       <c r="J86" t="s">
         <v>251</v>
       </c>
-      <c r="K86" s="5" t="s">
+      <c r="K86" t="s">
+        <v>286</v>
+      </c>
+      <c r="L86" s="5" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="87" spans="4:11" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="4:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D87" s="4" t="s">
         <v>91</v>
       </c>
@@ -2632,22 +2845,25 @@
       <c r="J87" t="s">
         <v>252</v>
       </c>
-      <c r="K87" s="5" t="s">
+      <c r="K87" t="s">
+        <v>287</v>
+      </c>
+      <c r="L87" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="88" spans="4:11" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="4:12" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D88" s="4" t="s">
         <v>96</v>
       </c>
       <c r="E88" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="K88" s="5" t="s">
+      <c r="L88" s="5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="89" spans="4:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D89" s="4" t="s">
         <v>98</v>
       </c>
@@ -2660,19 +2876,19 @@
       <c r="J89" t="s">
         <v>253</v>
       </c>
-      <c r="K89" s="5" t="s">
+      <c r="L89" s="5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="90" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D90" s="2"/>
       <c r="E90" s="3"/>
       <c r="I90" t="s">
         <v>197</v>
       </c>
-      <c r="K90" s="3"/>
-    </row>
-    <row r="91" spans="4:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L90" s="3"/>
+    </row>
+    <row r="91" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D91" s="4" t="s">
         <v>100</v>
       </c>
@@ -2682,11 +2898,11 @@
       <c r="I91" t="s">
         <v>198</v>
       </c>
-      <c r="K91" s="5" t="s">
+      <c r="L91" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="92" spans="4:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D92" s="4" t="s">
         <v>100</v>
       </c>
@@ -2696,11 +2912,14 @@
       <c r="J92" t="s">
         <v>254</v>
       </c>
-      <c r="K92" s="5" t="s">
+      <c r="K92" t="s">
+        <v>288</v>
+      </c>
+      <c r="L92" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="93" spans="4:11" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="4:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D93" s="4" t="s">
         <v>100</v>
       </c>
@@ -2714,11 +2933,14 @@
       <c r="J93" t="s">
         <v>255</v>
       </c>
-      <c r="K93" s="5" t="s">
+      <c r="K93" t="s">
+        <v>289</v>
+      </c>
+      <c r="L93" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="94" spans="4:11" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="4:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D94" s="4" t="s">
         <v>100</v>
       </c>
@@ -2731,11 +2953,14 @@
       <c r="J94" t="s">
         <v>256</v>
       </c>
-      <c r="K94" s="5" t="s">
+      <c r="K94" t="s">
+        <v>290</v>
+      </c>
+      <c r="L94" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="95" spans="4:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="4:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D95" s="4" t="s">
         <v>100</v>
       </c>
@@ -2748,7 +2973,10 @@
       <c r="I95" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="K95" s="5" t="s">
+      <c r="K95" t="s">
+        <v>291</v>
+      </c>
+      <c r="L95" s="5" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2797,8 +3025,11 @@
     <hyperlink ref="J50" r:id="rId40" xr:uid="{C121E486-6DC5-4AB8-BDD6-D4F32794A3A4}"/>
     <hyperlink ref="J69" r:id="rId41" xr:uid="{7F316388-2C20-4908-B372-14903C2E8EAA}"/>
     <hyperlink ref="J73" r:id="rId42" xr:uid="{851CBC7D-F6E3-4C94-816D-5E4B54BC54F2}"/>
+    <hyperlink ref="K12" r:id="rId43" xr:uid="{06AD9E37-3909-452B-AF07-1A08C94977D7}"/>
+    <hyperlink ref="K46" r:id="rId44" xr:uid="{96CAC567-3F0E-49CA-8DEC-F36C45823856}"/>
+    <hyperlink ref="J60" r:id="rId45" xr:uid="{159BA102-A07E-4CCA-B39C-0649E37DABAB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId43"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId46"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added dixy to db
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mihail\PycharmProjects\parce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95EA9A6-25FF-4B3A-AB8E-1F6D89EE10F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B9C73AD-58D9-445E-8CC9-E0F771BBAB86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{FFE27364-2778-47AC-8397-2059D7069E9C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="324">
   <si>
     <t>Бренд</t>
   </si>
@@ -600,9 +600,6 @@
     <t>https://www.ozon.ru/product/makfa-hlopya-gerkules-traditsionnyy-400-g-140800403/?asb=URtDxEY6%252F2LNjpCkmI%252BXJ7A4PptVvMtu5HPTuqoc%252FeI%253D&amp;asb2=XDSsXHVGRizDkslwdk2E36nMsCAAUMNDi05FORKwjipYfbtESstPtR2QSYKRRmPx&amp;keywords=%D0%B3%D0%B5%D1%80%D0%BA%D1%83%D0%BB%D0%B5%D1%81+%D1%82%D1%80%D0%B0%D0%B4%D0%B8%D1%86%D0%B8%D0%BE%D0%BD%D0%BD%D1%8B%D0%B9+15+%D0%BC%D0%B8%D0%BD%D0%B8&amp;sh=K5xV8WkwHQ</t>
   </si>
   <si>
-    <t>https://www.ozon.ru/product/zubnaya-pasta-splat-professional-white-plus-otbelivanie-plyus-100-ml-14125568/?asb=kL4zHBvOKJrLT2qhqS5kKkYYwpMXfpQOBhO%252FlkuXQNk%253D&amp;asb2=9H8mx7qiOJZCpYxTDSNrzQdTSLzRdhx3sb5vztz7Dsn5yRv39kaNJexj_Lvqzn4M&amp;keywords=splat&amp;sh=K5xV8XtVQQ</t>
-  </si>
-  <si>
     <t>https://www.ozon.ru/product/biomio-ekologichnyy-gel-dlya-stirki-delikatnyh-tkaney-bio-sensitive-bez-zapaha-1-5-l-275671748/?asb=ncPCrnTbHUuIWCvcIbLsJqD3F%252FDLTXGEj4vTj13m4To%253D&amp;asb2=VicgGbfDAYfrr5REKKrgyZmjqSl1byRDxamz4gH_4fx7B_kAuYIqAUB10czaImwR&amp;keywords=%D0%AD%D0%BA%D0%BE%D0%BB%D0%BE%D0%B3%D0%B8%D1%87%D0%BD%D1%8B%D0%B9+%D0%B3%D0%B5%D0%BB%D1%8C+++%D0%B4%D0%BB%D1%8F+%D0%B4%D0%B5%D0%BB%D0%B8%D0%BA%D0%B0%D1%82%D0%BD%D1%8B%D1%85+%D1%82%D0%BA%D0%B0%D0%BD%D0%B5%D0%B9+BioMio%C2%AE+BIO-SENSITIVE+1%2C5+%D0%BB.&amp;sh=K5xV8XHVNg</t>
   </si>
   <si>
@@ -612,9 +609,6 @@
     <t>https://www.ozon.ru/product/biomio-ekologichnoe-sredstvo-dlya-mytya-posudy-ovoshchey-i-fruktov-bio-care-bez-zapaha-450-ml-26431422/?asb=ERqDx3N%252B3XaJqlYdrUOv50bqRXMpcn%252FDm%252F9Ea0s0eH0%253D&amp;asb2=QrllhsWNJ6re4htULZqdeyEFLjROBZYSwpLePPXS0Pyigc34wr3pMyqjZWyxV4dk&amp;keywords=%D1%81%D1%80%D0%B5%D0%B4%D1%81%D1%82%D0%B2%D0%BE+%D0%B4%D0%BB%D1%8F+%D0%BC%D1%8B%D1%82%D1%8C%D1%8F+%D0%BF%D0%BE%D1%81%D1%83%D0%B4%D1%8B%2C+%D0%BE%D0%B2%D0%BE%D1%89%D0%B5%D0%B9+%D0%B8+%D1%84%D1%80%D1%83%D0%BA%D1%82%D0%BE%D0%B2+BioMio%C2%AE+BIO-CARE%2C+450+%D0%BC%D0%BB&amp;sh=K5xV8ZE-Gg</t>
   </si>
   <si>
-    <t>https://www.ozon.ru/product/tabletki-dlya-posudomoechnoy-mashiny-biomio-bio-total-7-v-1-evkalipt-60-sht-291986540/?asb=TShp3jb%252Faj%252BgMFGnG5dlD8qIuDH%252FqAaoMxFhJQKCmcs%253D&amp;asb2=LUfFZNCnFH_tG4U8HhxkPJFN8YjoQ8dl34MIZpwWPokHRk7hrq3Xf6_3URqJ7Sxn&amp;keywords=%D1%82%D0%B0%D0%B1%D0%BB%D0%B5%D1%82%D0%BA%D0%B8+%D0%B4%D0%BB%D1%8F+%D0%BF%D0%BE%D1%81%D1%83%D0%B4%D0%BE%D0%BC%D0%BE%D0%B5%D1%87%D0%BD%D0%BE%D0%B9+%D0%BC%D0%B0%D1%88%D0%B8%D0%BD%D1%8B+BioMio%C2%AE+BIO-TOTAL+%C2%AB7+%D0%B2+1%C2%BB%2C+%D0%B1%D0%B5%D0%B7+%D1%84%D0%BE%D1%81%D1%84%D0%B0%D1%82%D0%BE%D0%B2%2C+30+%D1%88%D1%82&amp;sh=K5xV8cb7FA</t>
-  </si>
-  <si>
     <t>https://www.ozon.ru/product/biomio-ekologichnoe-chistyashchee-sredstvo-dlya-stekol-zerkal-plastika-bio-glass-cleaner-bez-zapaha-147577585/?asb=z4TqFNrAWCwUTbgpOZEhsTe4WDv5bl0LaZ5Bm88en0A%253D&amp;asb2=O5TFSRttjbZd-AXtQMEIis57QE_fuXJzNMDWrTMnF_nwyNxaMGpwNOby174cWL0b&amp;keywords=%D1%87%D0%B8%D1%81%D1%82%D1%8F%D1%89%D0%B8%D0%B9+%D1%81%D0%BF%D1%80%D0%B5%D0%B9+%D0%B4%D0%BB%D1%8F+%D1%81%D1%82%D0%B5%D0%BA%D0%BE%D0%BB+BioMio%C2%AE+BIO-CLEANER%2C+%D0%B1%D0%B5%D0%B7+%D0%B7%D0%B0%D0%BF%D0%B0%D1%85%D0%B0%2C+500+%D0%BC%D0%BB.&amp;sh=K5xV8bgtMQ</t>
   </si>
   <si>
@@ -910,6 +904,108 @@
   </si>
   <si>
     <t>https://www.auchan.ru/product/syr-polutverdyy-brest-litovsk-rossiyskiy-50-narezka-150-g/</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/423/p/napitok-bezalkogolnyj-cernogolovka-limonad-originalnyj-silnogazirovannyj-1-25l-4098221</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/390/p/lapsa-sen-soy-premium-soba-grecnevaa-300g-2151515</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/390/p/lapsa-sen-soy-udon-psenicnaa-300g-3052127</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/390/p/vermisel-sen-soy-premium-funcoza-200g-3227619</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/465/p/sup-sen-soy-premium-pho-bo-s-risovoj-lapsoj-pod-sousom-125g-4028316</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/371/p/syr-brest-litovsk-klassiceskij-narezka-45-150g-3388814</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/376/p/maslo-sladkoslivocnoe-brest-litovsk-nesolenoe-vyssego-sorta-82-5-180g-3413519</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/zubnaya-pasta-splat-professional-biocalcium-biokaltsiy-100-ml-14125564/?asb=DQh2d2CXCPJhOsLCUsKD7IeWYbVtyE1bN1bmh1qFJlQ%253D&amp;asb2=iKz35uWcXwnGVyZZt_GtV2MjRDj33vLNg5IhYFtxx5UrJwueCIfZPJ--SPmerBuL&amp;keywords=splat+%D0%B7%D1%83%D0%B1%D0%BD%D0%B0%D1%8F+%D0%BF%D0%B0%D1%81%D1%82%D0%B0&amp;sh=K5xV8fHweA</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ru/product/krem-mylo-ushastyy-nyan-s-olivkovym-maslom-i-aloe-vera-300-ml/</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/biomio-ekologichnye-tabletki-dlya-posudomoechnoy-mashiny-7-v-1-bio-total-s-efirnym-maslom-evkalipta-26431435/?asb=DouF%252BVPCQamL9FhU692H1xqffhfk67OyVWjBHhMBhXhh%252FRzlSVLDnfPd0lA%252F9DIx&amp;asb2=77vgEV7r0eqKtmB55MlP472Q4qSngYJQ2Lcd7rlQzehyQNscwQ51rabPiyNdxmg6LV_n0HO6xdRHUCWCX1ynGfERYVh1WRVhIJP8lvQtjvxecsEfKNejMBmVqr26bBKn&amp;keywords=%D0%A2%D0%B0%D0%B1%D0%BB%D0%B5%D1%82%D0%BA%D0%B8+%D0%B4%D0%BB%D1%8F+%D0%BF%D0%BE%D1%81%D1%83%D0%B4%D0%BE%D0%BC%D0%BE%D0%B5%D1%87%D0%BD%D0%BE%D0%B9+%D0%BC%D0%B0%D1%88%D0%B8%D0%BD%D1%8B+BioMio+BIO-TOTAL+7-%D0%B2-1+%D1%8D%D0%B2%D0%BA%D0%B0%D0%BB%D0%B8%D0%BF%D1%82%2C+30+%D1%88%D1%82&amp;sh=K5xV8fdMzQ</t>
+  </si>
+  <si>
+    <t>Дикси</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/zamorozhennye_produkty/pelmeni_vareniki_khinkali_manty/135554/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/zamorozhennye_produkty/polufabrikaty/304674/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/zamorozhennye_produkty/pelmeni_vareniki_khinkali_manty/299073/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/zamorozhennye_produkty/pelmeni_vareniki_khinkali_manty/225786/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/zamorozhennye_produkty/gotovaya_eda_1/132809/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/syry_2/tvyerdye_polutvyerdye_syry/296998/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/sousy_spetsii/mayonez/132750/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/sousy_spetsii/mayonez/134858/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/sousy_spetsii/sousy_ketchupy_tomatnye_pasty/132764/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/molochnye_produkty_yaytsa/slivochnoe_maslo_margarin_spred/133171/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/detskoe_pitanie/voda_detskaya/302000/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/bakaleya_2/makarony_pasta/134608/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/bakaleya_2/makarony_pasta/132747/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/bakaleya_2/makarony_pasta/134645/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/bakaleya_2/muka_vse_dlya_vypechki/134630/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/bakaleya_2/makarony_pasta/134611/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/gigiena_i_kosmetika/ukhod_za_polostyu_rta/133318/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/gigiena_i_kosmetika/ukhod_za_polostyu_rta/132837/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/bytovaya_khimiya/stirka_i_ukhod_za_belem/226821/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/bytovaya_khimiya/stirka_i_ukhod_za_belem/132902/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/syry_2/syrnaya_narezka/132909/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/syry_2/syrnaya_narezka/203511/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/molochnye_produkty_yaytsa/slivochnoe_maslo_margarin_spred/132835/</t>
   </si>
 </sst>
 </file>
@@ -971,7 +1067,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1078,12 +1174,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1118,6 +1227,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -1433,10 +1543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF1A69E3-A9E5-424F-8F16-B76B324D2ACC}">
-  <dimension ref="D5:L95"/>
+  <dimension ref="D5:M95"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J88" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M95" sqref="M95"/>
+      <selection activeCell="O92" sqref="O92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1447,11 +1557,11 @@
     <col min="7" max="7" width="255.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="129.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1471,16 +1581,19 @@
         <v>108</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>201</v>
-      </c>
-      <c r="K6" s="12" t="s">
-        <v>257</v>
-      </c>
-      <c r="L6" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="M6" s="13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D7" s="4" t="s">
         <v>2</v>
       </c>
@@ -1494,16 +1607,17 @@
         <v>149</v>
       </c>
       <c r="J7" t="s">
-        <v>202</v>
-      </c>
-      <c r="K7" t="s">
-        <v>258</v>
-      </c>
-      <c r="L7" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="L7" s="9"/>
+      <c r="M7" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="4" t="s">
         <v>2</v>
       </c>
@@ -1515,16 +1629,16 @@
       </c>
       <c r="G8" s="9"/>
       <c r="J8" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="K8" t="s">
-        <v>259</v>
-      </c>
-      <c r="L8" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="M8" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D9" s="4" t="s">
         <v>2</v>
       </c>
@@ -1542,16 +1656,19 @@
         <v>110</v>
       </c>
       <c r="J9" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="K9" t="s">
-        <v>260</v>
-      </c>
-      <c r="L9" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="L9" t="s">
+        <v>301</v>
+      </c>
+      <c r="M9" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D10" s="4" t="s">
         <v>2</v>
       </c>
@@ -1566,16 +1683,17 @@
         <v>114</v>
       </c>
       <c r="J10" t="s">
-        <v>205</v>
-      </c>
-      <c r="K10" t="s">
-        <v>261</v>
-      </c>
-      <c r="L10" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="L10" s="9"/>
+      <c r="M10" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D11" s="4" t="s">
         <v>7</v>
       </c>
@@ -1593,16 +1711,16 @@
         <v>166</v>
       </c>
       <c r="J11" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K11" t="s">
-        <v>262</v>
-      </c>
-      <c r="L11" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="M11" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D12" s="4" t="s">
         <v>7</v>
       </c>
@@ -1616,16 +1734,17 @@
         <v>150</v>
       </c>
       <c r="J12" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>263</v>
-      </c>
-      <c r="L12" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="L12" s="9"/>
+      <c r="M12" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D13" s="4" t="s">
         <v>7</v>
       </c>
@@ -1637,13 +1756,13 @@
       </c>
       <c r="G13" s="9"/>
       <c r="J13" t="s">
-        <v>208</v>
-      </c>
-      <c r="L13" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="M13" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D14" s="4" t="s">
         <v>11</v>
       </c>
@@ -1658,16 +1777,17 @@
         <v>167</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="L14" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="L14" s="9"/>
+      <c r="M14" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D15" s="4" t="s">
         <v>11</v>
       </c>
@@ -1678,13 +1798,13 @@
         <v>168</v>
       </c>
       <c r="J15" t="s">
-        <v>210</v>
-      </c>
-      <c r="L15" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="M15" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D16" s="4" t="s">
         <v>14</v>
       </c>
@@ -1694,11 +1814,11 @@
       <c r="I16" t="s">
         <v>169</v>
       </c>
-      <c r="L16" s="5" t="s">
+      <c r="M16" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D17" s="4" t="s">
         <v>14</v>
       </c>
@@ -1706,14 +1826,15 @@
         <v>16</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K17" s="9"/>
-      <c r="L17" s="5" t="s">
+      <c r="L17" s="9"/>
+      <c r="M17" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D18" s="4" t="s">
         <v>14</v>
       </c>
@@ -1725,13 +1846,16 @@
       </c>
       <c r="G18" s="9"/>
       <c r="J18" t="s">
-        <v>212</v>
-      </c>
-      <c r="L18" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="L18" t="s">
+        <v>302</v>
+      </c>
+      <c r="M18" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D19" s="4" t="s">
         <v>7</v>
       </c>
@@ -1739,13 +1863,13 @@
         <v>18</v>
       </c>
       <c r="J19" t="s">
-        <v>213</v>
-      </c>
-      <c r="L19" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="M19" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D20" s="4" t="s">
         <v>7</v>
       </c>
@@ -1757,13 +1881,13 @@
       </c>
       <c r="G20" s="9"/>
       <c r="J20" t="s">
-        <v>214</v>
-      </c>
-      <c r="L20" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="M20" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D21" s="4" t="s">
         <v>7</v>
       </c>
@@ -1771,13 +1895,13 @@
         <v>20</v>
       </c>
       <c r="K21" t="s">
-        <v>265</v>
-      </c>
-      <c r="L21" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="M21" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D22" s="4" t="s">
         <v>21</v>
       </c>
@@ -1789,21 +1913,21 @@
       </c>
       <c r="G22" s="9"/>
       <c r="J22" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K22" t="s">
-        <v>266</v>
-      </c>
-      <c r="L22" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="M22" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D23" s="2"/>
       <c r="E23" s="3"/>
-      <c r="L23" s="3"/>
-    </row>
-    <row r="24" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M23" s="3"/>
+    </row>
+    <row r="24" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D24" s="4" t="s">
         <v>23</v>
       </c>
@@ -1816,13 +1940,13 @@
         <v>170</v>
       </c>
       <c r="J24" t="s">
-        <v>216</v>
-      </c>
-      <c r="L24" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="M24" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D25" s="4" t="s">
         <v>23</v>
       </c>
@@ -1830,13 +1954,16 @@
         <v>25</v>
       </c>
       <c r="J25" t="s">
-        <v>217</v>
-      </c>
-      <c r="L25" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="L25" t="s">
+        <v>303</v>
+      </c>
+      <c r="M25" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D26" s="4" t="s">
         <v>23</v>
       </c>
@@ -1848,57 +1975,57 @@
       </c>
       <c r="G26" s="9"/>
       <c r="J26" t="s">
-        <v>218</v>
-      </c>
-      <c r="L26" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="M26" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D27" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="L27" s="5" t="s">
+      <c r="M27" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D28" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="L28" s="5" t="s">
+      <c r="M28" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D29" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="L29" s="5" t="s">
+      <c r="M29" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D30" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="L30" s="5" t="s">
+      <c r="M30" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D31" s="4" t="s">
         <v>31</v>
       </c>
@@ -1909,22 +2036,25 @@
         <v>124</v>
       </c>
       <c r="G31" s="9"/>
-      <c r="L31" s="5" t="s">
+      <c r="L31" t="s">
+        <v>304</v>
+      </c>
+      <c r="M31" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="4:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D32" s="7" t="s">
         <v>34</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="L32" s="8" t="s">
+      <c r="M32" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="4:12" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D33" s="4" t="s">
         <v>34</v>
       </c>
@@ -1936,24 +2066,27 @@
       </c>
       <c r="G33" s="9"/>
       <c r="K33" t="s">
-        <v>267</v>
-      </c>
-      <c r="L33" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="L33" t="s">
+        <v>305</v>
+      </c>
+      <c r="M33" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="4:12" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D34" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="L34" s="5" t="s">
+      <c r="M34" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="4:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D35" s="4" t="s">
         <v>38</v>
       </c>
@@ -1961,13 +2094,13 @@
         <v>39</v>
       </c>
       <c r="K35" t="s">
-        <v>268</v>
-      </c>
-      <c r="L35" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="M35" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="4:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D36" s="4" t="s">
         <v>34</v>
       </c>
@@ -1977,16 +2110,16 @@
       <c r="I36" t="s">
         <v>171</v>
       </c>
-      <c r="L36" s="5" t="s">
+      <c r="M36" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D37" s="2"/>
       <c r="E37" s="3"/>
-      <c r="L37" s="3"/>
-    </row>
-    <row r="38" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M37" s="3"/>
+    </row>
+    <row r="38" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D38" s="4" t="s">
         <v>41</v>
       </c>
@@ -1998,16 +2131,16 @@
       </c>
       <c r="G38" s="9"/>
       <c r="J38" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="K38" t="s">
-        <v>269</v>
-      </c>
-      <c r="L38" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="M38" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D39" s="4" t="s">
         <v>41</v>
       </c>
@@ -2019,16 +2152,16 @@
       </c>
       <c r="G39" s="9"/>
       <c r="J39" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="K39" t="s">
-        <v>270</v>
-      </c>
-      <c r="L39" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="M39" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D40" s="4" t="s">
         <v>41</v>
       </c>
@@ -2042,13 +2175,16 @@
         <v>151</v>
       </c>
       <c r="J40" t="s">
-        <v>223</v>
-      </c>
-      <c r="L40" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="L40" t="s">
+        <v>306</v>
+      </c>
+      <c r="M40" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D41" s="4" t="s">
         <v>41</v>
       </c>
@@ -2056,16 +2192,16 @@
         <v>45</v>
       </c>
       <c r="J41" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="K41" t="s">
-        <v>271</v>
-      </c>
-      <c r="L41" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="M41" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D42" s="4" t="s">
         <v>41</v>
       </c>
@@ -2073,14 +2209,15 @@
         <v>46</v>
       </c>
       <c r="J42" s="9" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="K42" s="9"/>
-      <c r="L42" s="5" t="s">
+      <c r="L42" s="9"/>
+      <c r="M42" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="43" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D43" s="4" t="s">
         <v>41</v>
       </c>
@@ -2092,18 +2229,18 @@
       </c>
       <c r="G43" s="9"/>
       <c r="J43" t="s">
-        <v>222</v>
-      </c>
-      <c r="L43" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="M43" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D44" s="2"/>
       <c r="E44" s="3"/>
-      <c r="L44" s="3"/>
-    </row>
-    <row r="45" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M44" s="3"/>
+    </row>
+    <row r="45" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D45" s="4" t="s">
         <v>48</v>
       </c>
@@ -2111,13 +2248,16 @@
         <v>49</v>
       </c>
       <c r="K45" t="s">
-        <v>273</v>
-      </c>
-      <c r="L45" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="L45" t="s">
+        <v>307</v>
+      </c>
+      <c r="M45" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D46" s="4" t="s">
         <v>48</v>
       </c>
@@ -2129,16 +2269,19 @@
       </c>
       <c r="G46" s="9"/>
       <c r="J46" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="K46" s="9" t="s">
-        <v>272</v>
-      </c>
-      <c r="L46" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="L46" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="M46" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D47" s="4" t="s">
         <v>48</v>
       </c>
@@ -2146,11 +2289,11 @@
         <v>51</v>
       </c>
       <c r="H47" s="9"/>
-      <c r="L47" s="5" t="s">
+      <c r="M47" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="48" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D48" s="4" t="s">
         <v>52</v>
       </c>
@@ -2161,23 +2304,26 @@
         <v>132</v>
       </c>
       <c r="G48" s="9"/>
-      <c r="H48" t="s">
+      <c r="H48" s="9" t="s">
         <v>130</v>
       </c>
       <c r="I48" t="s">
         <v>172</v>
       </c>
       <c r="J48" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K48" t="s">
-        <v>274</v>
-      </c>
-      <c r="L48" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="L48" t="s">
+        <v>309</v>
+      </c>
+      <c r="M48" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D49" s="4" t="s">
         <v>52</v>
       </c>
@@ -2189,16 +2335,16 @@
       </c>
       <c r="G49" s="9"/>
       <c r="J49" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="K49" t="s">
-        <v>275</v>
-      </c>
-      <c r="L49" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="M49" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D50" s="4" t="s">
         <v>52</v>
       </c>
@@ -2209,14 +2355,15 @@
         <v>172</v>
       </c>
       <c r="J50" s="9" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="K50" s="9"/>
-      <c r="L50" s="5" t="s">
+      <c r="L50" s="9"/>
+      <c r="M50" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D51" s="4" t="s">
         <v>52</v>
       </c>
@@ -2224,13 +2371,13 @@
         <v>56</v>
       </c>
       <c r="J51" t="s">
-        <v>229</v>
-      </c>
-      <c r="L51" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="M51" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="52" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D52" s="4" t="s">
         <v>57</v>
       </c>
@@ -2238,40 +2385,43 @@
         <v>58</v>
       </c>
       <c r="K52" t="s">
-        <v>276</v>
-      </c>
-      <c r="L52" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="M52" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="53" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D53" s="4" t="s">
         <v>57</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="L53" s="5" t="s">
+      <c r="L53" t="s">
+        <v>310</v>
+      </c>
+      <c r="M53" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="54" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D54" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="L54" s="5" t="s">
+      <c r="M54" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="55" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D55" s="2"/>
       <c r="E55" s="3"/>
-      <c r="L55" s="3"/>
-    </row>
-    <row r="56" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M55" s="3"/>
+    </row>
+    <row r="56" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D56" s="4" t="s">
         <v>62</v>
       </c>
@@ -2286,16 +2436,19 @@
         <v>174</v>
       </c>
       <c r="J56" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="K56" t="s">
-        <v>277</v>
-      </c>
-      <c r="L56" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="L56" t="s">
+        <v>311</v>
+      </c>
+      <c r="M56" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="57" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="4" t="s">
         <v>62</v>
       </c>
@@ -2303,19 +2456,22 @@
         <v>64</v>
       </c>
       <c r="J57" t="s">
-        <v>231</v>
-      </c>
-      <c r="L57" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="M57" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="58" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="4" t="s">
         <v>62</v>
       </c>
       <c r="E58" s="5" t="s">
         <v>65</v>
       </c>
+      <c r="F58" t="s">
+        <v>290</v>
+      </c>
       <c r="H58" t="s">
         <v>161</v>
       </c>
@@ -2323,24 +2479,25 @@
         <v>173</v>
       </c>
       <c r="J58" t="s">
-        <v>232</v>
-      </c>
-      <c r="K58" t="s">
-        <v>278</v>
-      </c>
-      <c r="L58" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="K58" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="L58" s="9"/>
+      <c r="M58" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="59" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D59" s="2"/>
       <c r="E59" s="3"/>
       <c r="I59" t="s">
         <v>175</v>
       </c>
-      <c r="L59" s="3"/>
-    </row>
-    <row r="60" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M59" s="3"/>
+    </row>
+    <row r="60" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D60" s="4" t="s">
         <v>66</v>
       </c>
@@ -2355,16 +2512,16 @@
         <v>176</v>
       </c>
       <c r="J60" s="9" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K60" t="s">
-        <v>279</v>
-      </c>
-      <c r="L60" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="M60" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="61" spans="4:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D61" s="4" t="s">
         <v>66</v>
       </c>
@@ -2372,56 +2529,68 @@
         <v>68</v>
       </c>
       <c r="J61" t="s">
-        <v>234</v>
-      </c>
-      <c r="L61" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="M61" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="62" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D62" s="4" t="s">
         <v>66</v>
       </c>
       <c r="E62" s="5" t="s">
         <v>69</v>
       </c>
+      <c r="F62" t="s">
+        <v>292</v>
+      </c>
       <c r="I62" t="s">
         <v>177</v>
       </c>
       <c r="J62" t="s">
-        <v>235</v>
-      </c>
-      <c r="L62" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="M62" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="63" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D63" s="4" t="s">
         <v>66</v>
       </c>
       <c r="E63" s="5" t="s">
         <v>70</v>
       </c>
+      <c r="F63" s="9" t="s">
+        <v>291</v>
+      </c>
       <c r="I63" t="s">
         <v>178</v>
       </c>
       <c r="J63" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="K63" t="s">
-        <v>280</v>
-      </c>
-      <c r="L63" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="L63" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="M63" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="64" spans="4:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D64" s="4" t="s">
         <v>66</v>
       </c>
       <c r="E64" s="5" t="s">
         <v>71</v>
       </c>
+      <c r="F64" t="s">
+        <v>293</v>
+      </c>
       <c r="G64" t="s">
         <v>152</v>
       </c>
@@ -2429,16 +2598,19 @@
         <v>179</v>
       </c>
       <c r="J64" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K64" t="s">
-        <v>281</v>
-      </c>
-      <c r="L64" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="L64" t="s">
+        <v>313</v>
+      </c>
+      <c r="M64" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="65" spans="4:12" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="4:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D65" s="4" t="s">
         <v>66</v>
       </c>
@@ -2452,38 +2624,41 @@
         <v>180</v>
       </c>
       <c r="J65" t="s">
-        <v>238</v>
-      </c>
-      <c r="L65" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="M65" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="4:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D66" s="4" t="s">
         <v>66</v>
       </c>
       <c r="E66" s="5" t="s">
         <v>73</v>
       </c>
+      <c r="F66" t="s">
+        <v>294</v>
+      </c>
       <c r="G66" t="s">
         <v>154</v>
       </c>
       <c r="I66" t="s">
         <v>181</v>
       </c>
-      <c r="L66" s="5" t="s">
+      <c r="M66" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D67" s="2"/>
       <c r="E67" s="3"/>
       <c r="I67" t="s">
         <v>182</v>
       </c>
-      <c r="L67" s="3"/>
-    </row>
-    <row r="68" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M67" s="3"/>
+    </row>
+    <row r="68" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D68" s="4" t="s">
         <v>74</v>
       </c>
@@ -2494,16 +2669,19 @@
         <v>155</v>
       </c>
       <c r="J68" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="K68" t="s">
-        <v>282</v>
-      </c>
-      <c r="L68" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="L68" t="s">
+        <v>314</v>
+      </c>
+      <c r="M68" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="69" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D69" s="4" t="s">
         <v>74</v>
       </c>
@@ -2517,16 +2695,19 @@
         <v>156</v>
       </c>
       <c r="J69" s="9" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="K69" s="9" t="s">
-        <v>283</v>
-      </c>
-      <c r="L69" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="L69" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="M69" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="70" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D70" s="4" t="s">
         <v>74</v>
       </c>
@@ -2536,11 +2717,11 @@
       <c r="I70" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="L70" s="5" t="s">
+      <c r="M70" s="5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="71" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D71" s="4" t="s">
         <v>74</v>
       </c>
@@ -2557,13 +2738,13 @@
         <v>184</v>
       </c>
       <c r="J71" t="s">
-        <v>241</v>
-      </c>
-      <c r="L71" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="M71" s="5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="72" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D72" s="4" t="s">
         <v>74</v>
       </c>
@@ -2576,14 +2757,17 @@
       <c r="I72" t="s">
         <v>185</v>
       </c>
-      <c r="K72" t="s">
-        <v>284</v>
-      </c>
-      <c r="L72" s="5" t="s">
+      <c r="K72" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="L72" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="M72" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="73" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D73" s="4" t="s">
         <v>74</v>
       </c>
@@ -2594,14 +2778,15 @@
         <v>186</v>
       </c>
       <c r="J73" s="9" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="K73" s="9"/>
-      <c r="L73" s="5" t="s">
+      <c r="L73" s="9"/>
+      <c r="M73" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="74" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D74" s="4" t="s">
         <v>74</v>
       </c>
@@ -2612,21 +2797,21 @@
         <v>163</v>
       </c>
       <c r="J74" t="s">
-        <v>243</v>
-      </c>
-      <c r="L74" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="M74" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="75" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D75" s="2"/>
       <c r="E75" s="3"/>
       <c r="I75" t="s">
         <v>187</v>
       </c>
-      <c r="L75" s="3"/>
-    </row>
-    <row r="76" spans="4:12" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M75" s="3"/>
+    </row>
+    <row r="76" spans="4:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D76" s="4" t="s">
         <v>82</v>
       </c>
@@ -2640,13 +2825,16 @@
         <v>157</v>
       </c>
       <c r="J76" t="s">
-        <v>244</v>
-      </c>
-      <c r="L76" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="L76" t="s">
+        <v>317</v>
+      </c>
+      <c r="M76" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="77" spans="4:12" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="4:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D77" s="4" t="s">
         <v>82</v>
       </c>
@@ -2658,13 +2846,16 @@
       </c>
       <c r="G77" s="9"/>
       <c r="J77" t="s">
-        <v>245</v>
-      </c>
-      <c r="L77" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="L77" t="s">
+        <v>318</v>
+      </c>
+      <c r="M77" s="5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="78" spans="4:12" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="4:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D78" s="4" t="s">
         <v>85</v>
       </c>
@@ -2678,14 +2869,14 @@
       <c r="H78" t="s">
         <v>164</v>
       </c>
-      <c r="I78" t="s">
-        <v>188</v>
-      </c>
-      <c r="L78" s="5" t="s">
+      <c r="I78" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="M78" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="79" spans="4:12" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="4:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D79" s="4" t="s">
         <v>85</v>
       </c>
@@ -2700,13 +2891,16 @@
         <v>165</v>
       </c>
       <c r="J79" t="s">
-        <v>246</v>
-      </c>
-      <c r="L79" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="L79" t="s">
+        <v>319</v>
+      </c>
+      <c r="M79" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="80" spans="4:12" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="4:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D80" s="4" t="s">
         <v>85</v>
       </c>
@@ -2717,19 +2911,19 @@
         <v>143</v>
       </c>
       <c r="I80" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J80" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="K80" t="s">
-        <v>285</v>
-      </c>
-      <c r="L80" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="M80" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="81" spans="4:12" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="4:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D81" s="4" t="s">
         <v>85</v>
       </c>
@@ -2740,16 +2934,16 @@
         <v>144</v>
       </c>
       <c r="I81" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J81" t="s">
-        <v>248</v>
-      </c>
-      <c r="L81" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="M81" s="5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="82" spans="4:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D82" s="4" t="s">
         <v>85</v>
       </c>
@@ -2761,24 +2955,24 @@
       </c>
       <c r="G82" s="9"/>
       <c r="I82" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J82" t="s">
-        <v>249</v>
-      </c>
-      <c r="L82" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="M82" s="5" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="83" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D83" s="2"/>
       <c r="E83" s="3"/>
       <c r="I83" t="s">
-        <v>192</v>
-      </c>
-      <c r="L83" s="3"/>
-    </row>
-    <row r="84" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>299</v>
+      </c>
+      <c r="M83" s="3"/>
+    </row>
+    <row r="84" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D84" s="4" t="s">
         <v>91</v>
       </c>
@@ -2792,27 +2986,30 @@
         <v>158</v>
       </c>
       <c r="I84" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="J84" t="s">
-        <v>250</v>
-      </c>
-      <c r="L84" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="K84" t="s">
+        <v>298</v>
+      </c>
+      <c r="M84" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="85" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D85" s="4" t="s">
         <v>91</v>
       </c>
       <c r="E85" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="L85" s="5" t="s">
+      <c r="M85" s="5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="86" spans="4:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D86" s="4" t="s">
         <v>91</v>
       </c>
@@ -2820,19 +3017,19 @@
         <v>94</v>
       </c>
       <c r="I86" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J86" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="K86" t="s">
-        <v>286</v>
-      </c>
-      <c r="L86" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="M86" s="5" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="87" spans="4:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D87" s="4" t="s">
         <v>91</v>
       </c>
@@ -2840,30 +3037,33 @@
         <v>95</v>
       </c>
       <c r="I87" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J87" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="K87" t="s">
-        <v>287</v>
-      </c>
-      <c r="L87" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="L87" t="s">
+        <v>320</v>
+      </c>
+      <c r="M87" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="88" spans="4:12" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="4:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D88" s="4" t="s">
         <v>96</v>
       </c>
       <c r="E88" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="L88" s="5" t="s">
+      <c r="M88" s="5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="89" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D89" s="4" t="s">
         <v>98</v>
       </c>
@@ -2871,24 +3071,24 @@
         <v>99</v>
       </c>
       <c r="I89" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J89" t="s">
-        <v>253</v>
-      </c>
-      <c r="L89" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="M89" s="5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="90" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D90" s="2"/>
       <c r="E90" s="3"/>
       <c r="I90" t="s">
-        <v>197</v>
-      </c>
-      <c r="L90" s="3"/>
-    </row>
-    <row r="91" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+      <c r="M90" s="3"/>
+    </row>
+    <row r="91" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D91" s="4" t="s">
         <v>100</v>
       </c>
@@ -2896,51 +3096,62 @@
         <v>101</v>
       </c>
       <c r="I91" t="s">
-        <v>198</v>
-      </c>
-      <c r="L91" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="M91" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="92" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D92" s="4" t="s">
         <v>100</v>
       </c>
       <c r="E92" s="5" t="s">
         <v>102</v>
       </c>
+      <c r="F92" t="s">
+        <v>296</v>
+      </c>
       <c r="J92" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="K92" t="s">
-        <v>288</v>
-      </c>
-      <c r="L92" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="L92" t="s">
+        <v>323</v>
+      </c>
+      <c r="M92" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="93" spans="4:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D93" s="4" t="s">
         <v>100</v>
       </c>
       <c r="E93" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="F93" s="9"/>
+      <c r="F93" s="9" t="s">
+        <v>295</v>
+      </c>
       <c r="G93" s="9" t="s">
         <v>159</v>
       </c>
       <c r="J93" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="K93" t="s">
-        <v>289</v>
-      </c>
-      <c r="L93" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="L93" t="s">
+        <v>321</v>
+      </c>
+      <c r="M93" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="94" spans="4:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D94" s="4" t="s">
         <v>100</v>
       </c>
@@ -2948,19 +3159,19 @@
         <v>104</v>
       </c>
       <c r="I94" s="9" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J94" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="K94" t="s">
-        <v>290</v>
-      </c>
-      <c r="L94" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="M94" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="95" spans="4:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D95" s="4" t="s">
         <v>100</v>
       </c>
@@ -2971,12 +3182,15 @@
         <v>147</v>
       </c>
       <c r="I95" s="9" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="K95" t="s">
-        <v>291</v>
-      </c>
-      <c r="L95" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="L95" t="s">
+        <v>322</v>
+      </c>
+      <c r="M95" s="5" t="s">
         <v>105</v>
       </c>
     </row>
@@ -3028,8 +3242,15 @@
     <hyperlink ref="K12" r:id="rId43" xr:uid="{06AD9E37-3909-452B-AF07-1A08C94977D7}"/>
     <hyperlink ref="K46" r:id="rId44" xr:uid="{96CAC567-3F0E-49CA-8DEC-F36C45823856}"/>
     <hyperlink ref="J60" r:id="rId45" xr:uid="{159BA102-A07E-4CCA-B39C-0649E37DABAB}"/>
+    <hyperlink ref="F63" r:id="rId46" xr:uid="{02308EB3-0D4F-43E5-B4E2-B6F6C09AEFBB}"/>
+    <hyperlink ref="K7" r:id="rId47" xr:uid="{12963AA2-BE9C-48F6-ADD3-656C6E23B39C}"/>
+    <hyperlink ref="H48" r:id="rId48" xr:uid="{8E5E12B2-C9E3-4CE9-A709-1339EBF59243}"/>
+    <hyperlink ref="K10" r:id="rId49" xr:uid="{A00C7BE9-6CBD-4A4B-AB12-2C62A70BE084}"/>
+    <hyperlink ref="K58" r:id="rId50" xr:uid="{7593D602-EECA-4B89-A6ED-6CF677EB1C0D}"/>
+    <hyperlink ref="K72" r:id="rId51" xr:uid="{46977EFB-3B7E-4A69-822A-E021388A83CE}"/>
+    <hyperlink ref="L63" r:id="rId52" xr:uid="{A6E2704C-7779-416A-BF8F-0168747F4B17}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId46"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId53"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added some changes to db
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mihail\PycharmProjects\parce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6939690A-8C74-41E9-BC73-50CE8E5C77A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE55A1A0-A46C-416E-917F-98FB8729518D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{FFE27364-2778-47AC-8397-2059D7069E9C}"/>
+    <workbookView xWindow="3375" yWindow="1605" windowWidth="21600" windowHeight="11505" xr2:uid="{FFE27364-2778-47AC-8397-2059D7069E9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="324">
   <si>
     <t>Бренд</t>
   </si>
@@ -600,9 +600,6 @@
     <t>https://www.ozon.ru/product/makfa-hlopya-gerkules-traditsionnyy-400-g-140800403/?asb=URtDxEY6%252F2LNjpCkmI%252BXJ7A4PptVvMtu5HPTuqoc%252FeI%253D&amp;asb2=XDSsXHVGRizDkslwdk2E36nMsCAAUMNDi05FORKwjipYfbtESstPtR2QSYKRRmPx&amp;keywords=%D0%B3%D0%B5%D1%80%D0%BA%D1%83%D0%BB%D0%B5%D1%81+%D1%82%D1%80%D0%B0%D0%B4%D0%B8%D1%86%D0%B8%D0%BE%D0%BD%D0%BD%D1%8B%D0%B9+15+%D0%BC%D0%B8%D0%BD%D0%B8&amp;sh=K5xV8WkwHQ</t>
   </si>
   <si>
-    <t>https://www.ozon.ru/product/zubnaya-pasta-splat-professional-white-plus-otbelivanie-plyus-100-ml-14125568/?asb=kL4zHBvOKJrLT2qhqS5kKkYYwpMXfpQOBhO%252FlkuXQNk%253D&amp;asb2=9H8mx7qiOJZCpYxTDSNrzQdTSLzRdhx3sb5vztz7Dsn5yRv39kaNJexj_Lvqzn4M&amp;keywords=splat&amp;sh=K5xV8XtVQQ</t>
-  </si>
-  <si>
     <t>https://www.ozon.ru/product/biomio-ekologichnyy-gel-dlya-stirki-delikatnyh-tkaney-bio-sensitive-bez-zapaha-1-5-l-275671748/?asb=ncPCrnTbHUuIWCvcIbLsJqD3F%252FDLTXGEj4vTj13m4To%253D&amp;asb2=VicgGbfDAYfrr5REKKrgyZmjqSl1byRDxamz4gH_4fx7B_kAuYIqAUB10czaImwR&amp;keywords=%D0%AD%D0%BA%D0%BE%D0%BB%D0%BE%D0%B3%D0%B8%D1%87%D0%BD%D1%8B%D0%B9+%D0%B3%D0%B5%D0%BB%D1%8C+++%D0%B4%D0%BB%D1%8F+%D0%B4%D0%B5%D0%BB%D0%B8%D0%BA%D0%B0%D1%82%D0%BD%D1%8B%D1%85+%D1%82%D0%BA%D0%B0%D0%BD%D0%B5%D0%B9+BioMio%C2%AE+BIO-SENSITIVE+1%2C5+%D0%BB.&amp;sh=K5xV8XHVNg</t>
   </si>
   <si>
@@ -612,9 +609,6 @@
     <t>https://www.ozon.ru/product/biomio-ekologichnoe-sredstvo-dlya-mytya-posudy-ovoshchey-i-fruktov-bio-care-bez-zapaha-450-ml-26431422/?asb=ERqDx3N%252B3XaJqlYdrUOv50bqRXMpcn%252FDm%252F9Ea0s0eH0%253D&amp;asb2=QrllhsWNJ6re4htULZqdeyEFLjROBZYSwpLePPXS0Pyigc34wr3pMyqjZWyxV4dk&amp;keywords=%D1%81%D1%80%D0%B5%D0%B4%D1%81%D1%82%D0%B2%D0%BE+%D0%B4%D0%BB%D1%8F+%D0%BC%D1%8B%D1%82%D1%8C%D1%8F+%D0%BF%D0%BE%D1%81%D1%83%D0%B4%D1%8B%2C+%D0%BE%D0%B2%D0%BE%D1%89%D0%B5%D0%B9+%D0%B8+%D1%84%D1%80%D1%83%D0%BA%D1%82%D0%BE%D0%B2+BioMio%C2%AE+BIO-CARE%2C+450+%D0%BC%D0%BB&amp;sh=K5xV8ZE-Gg</t>
   </si>
   <si>
-    <t>https://www.ozon.ru/product/tabletki-dlya-posudomoechnoy-mashiny-biomio-bio-total-7-v-1-evkalipt-60-sht-291986540/?asb=TShp3jb%252Faj%252BgMFGnG5dlD8qIuDH%252FqAaoMxFhJQKCmcs%253D&amp;asb2=LUfFZNCnFH_tG4U8HhxkPJFN8YjoQ8dl34MIZpwWPokHRk7hrq3Xf6_3URqJ7Sxn&amp;keywords=%D1%82%D0%B0%D0%B1%D0%BB%D0%B5%D1%82%D0%BA%D0%B8+%D0%B4%D0%BB%D1%8F+%D0%BF%D0%BE%D1%81%D1%83%D0%B4%D0%BE%D0%BC%D0%BE%D0%B5%D1%87%D0%BD%D0%BE%D0%B9+%D0%BC%D0%B0%D1%88%D0%B8%D0%BD%D1%8B+BioMio%C2%AE+BIO-TOTAL+%C2%AB7+%D0%B2+1%C2%BB%2C+%D0%B1%D0%B5%D0%B7+%D1%84%D0%BE%D1%81%D1%84%D0%B0%D1%82%D0%BE%D0%B2%2C+30+%D1%88%D1%82&amp;sh=K5xV8cb7FA</t>
-  </si>
-  <si>
     <t>https://www.ozon.ru/product/biomio-ekologichnoe-chistyashchee-sredstvo-dlya-stekol-zerkal-plastika-bio-glass-cleaner-bez-zapaha-147577585/?asb=z4TqFNrAWCwUTbgpOZEhsTe4WDv5bl0LaZ5Bm88en0A%253D&amp;asb2=O5TFSRttjbZd-AXtQMEIis57QE_fuXJzNMDWrTMnF_nwyNxaMGpwNOby174cWL0b&amp;keywords=%D1%87%D0%B8%D1%81%D1%82%D1%8F%D1%89%D0%B8%D0%B9+%D1%81%D0%BF%D1%80%D0%B5%D0%B9+%D0%B4%D0%BB%D1%8F+%D1%81%D1%82%D0%B5%D0%BA%D0%BE%D0%BB+BioMio%C2%AE+BIO-CLEANER%2C+%D0%B1%D0%B5%D0%B7+%D0%B7%D0%B0%D0%BF%D0%B0%D1%85%D0%B0%2C+500+%D0%BC%D0%BB.&amp;sh=K5xV8bgtMQ</t>
   </si>
   <si>
@@ -910,6 +904,108 @@
   </si>
   <si>
     <t>https://www.auchan.ru/product/syr-polutverdyy-brest-litovsk-rossiyskiy-50-narezka-150-g/</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/423/p/napitok-bezalkogolnyj-cernogolovka-limonad-originalnyj-silnogazirovannyj-1-25l-4098221</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/390/p/lapsa-sen-soy-premium-soba-grecnevaa-300g-2151515</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/390/p/lapsa-sen-soy-udon-psenicnaa-300g-3052127</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/390/p/vermisel-sen-soy-premium-funcoza-200g-3227619</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/465/p/sup-sen-soy-premium-pho-bo-s-risovoj-lapsoj-pod-sousom-125g-4028316</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/371/p/syr-brest-litovsk-klassiceskij-narezka-45-150g-3388814</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/376/p/maslo-sladkoslivocnoe-brest-litovsk-nesolenoe-vyssego-sorta-82-5-180g-3413519</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/zubnaya-pasta-splat-professional-biocalcium-biokaltsiy-100-ml-14125564/?asb=DQh2d2CXCPJhOsLCUsKD7IeWYbVtyE1bN1bmh1qFJlQ%253D&amp;asb2=iKz35uWcXwnGVyZZt_GtV2MjRDj33vLNg5IhYFtxx5UrJwueCIfZPJ--SPmerBuL&amp;keywords=splat+%D0%B7%D1%83%D0%B1%D0%BD%D0%B0%D1%8F+%D0%BF%D0%B0%D1%81%D1%82%D0%B0&amp;sh=K5xV8fHweA</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ru/product/krem-mylo-ushastyy-nyan-s-olivkovym-maslom-i-aloe-vera-300-ml/</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/biomio-ekologichnye-tabletki-dlya-posudomoechnoy-mashiny-7-v-1-bio-total-s-efirnym-maslom-evkalipta-26431435/?asb=DouF%252BVPCQamL9FhU692H1xqffhfk67OyVWjBHhMBhXhh%252FRzlSVLDnfPd0lA%252F9DIx&amp;asb2=77vgEV7r0eqKtmB55MlP472Q4qSngYJQ2Lcd7rlQzehyQNscwQ51rabPiyNdxmg6LV_n0HO6xdRHUCWCX1ynGfERYVh1WRVhIJP8lvQtjvxecsEfKNejMBmVqr26bBKn&amp;keywords=%D0%A2%D0%B0%D0%B1%D0%BB%D0%B5%D1%82%D0%BA%D0%B8+%D0%B4%D0%BB%D1%8F+%D0%BF%D0%BE%D1%81%D1%83%D0%B4%D0%BE%D0%BC%D0%BE%D0%B5%D1%87%D0%BD%D0%BE%D0%B9+%D0%BC%D0%B0%D1%88%D0%B8%D0%BD%D1%8B+BioMio+BIO-TOTAL+7-%D0%B2-1+%D1%8D%D0%B2%D0%BA%D0%B0%D0%BB%D0%B8%D0%BF%D1%82%2C+30+%D1%88%D1%82&amp;sh=K5xV8fdMzQ</t>
+  </si>
+  <si>
+    <t>Дикси</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/zamorozhennye_produkty/pelmeni_vareniki_khinkali_manty/135554/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/zamorozhennye_produkty/polufabrikaty/304674/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/zamorozhennye_produkty/pelmeni_vareniki_khinkali_manty/299073/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/zamorozhennye_produkty/pelmeni_vareniki_khinkali_manty/225786/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/zamorozhennye_produkty/gotovaya_eda_1/132809/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/syry_2/tvyerdye_polutvyerdye_syry/296998/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/sousy_spetsii/mayonez/132750/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/sousy_spetsii/mayonez/134858/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/sousy_spetsii/sousy_ketchupy_tomatnye_pasty/132764/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/molochnye_produkty_yaytsa/slivochnoe_maslo_margarin_spred/133171/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/detskoe_pitanie/voda_detskaya/302000/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/bakaleya_2/makarony_pasta/134608/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/bakaleya_2/makarony_pasta/132747/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/bakaleya_2/makarony_pasta/134645/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/bakaleya_2/muka_vse_dlya_vypechki/134630/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/bakaleya_2/makarony_pasta/134611/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/gigiena_i_kosmetika/ukhod_za_polostyu_rta/133318/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/gigiena_i_kosmetika/ukhod_za_polostyu_rta/132837/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/bytovaya_khimiya/stirka_i_ukhod_za_belem/226821/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/bytovaya_khimiya/stirka_i_ukhod_za_belem/132902/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/syry_2/syrnaya_narezka/132909/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/syry_2/syrnaya_narezka/203511/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/molochnye_produkty_yaytsa/slivochnoe_maslo_margarin_spred/132835/</t>
   </si>
 </sst>
 </file>
@@ -971,7 +1067,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1078,12 +1174,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1118,6 +1227,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -1433,10 +1543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF1A69E3-A9E5-424F-8F16-B76B324D2ACC}">
-  <dimension ref="D5:L95"/>
+  <dimension ref="D5:M95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="J22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1447,11 +1557,11 @@
     <col min="7" max="7" width="255.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="129.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1471,16 +1581,19 @@
         <v>108</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>201</v>
-      </c>
-      <c r="K6" s="12" t="s">
-        <v>257</v>
-      </c>
-      <c r="L6" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="M6" s="13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D7" s="4" t="s">
         <v>2</v>
       </c>
@@ -1494,16 +1607,17 @@
         <v>149</v>
       </c>
       <c r="J7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>258</v>
-      </c>
-      <c r="L7" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="L7" s="9"/>
+      <c r="M7" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="4" t="s">
         <v>2</v>
       </c>
@@ -1515,16 +1629,16 @@
       </c>
       <c r="G8" s="9"/>
       <c r="J8" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="K8" t="s">
-        <v>259</v>
-      </c>
-      <c r="L8" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="M8" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D9" s="4" t="s">
         <v>2</v>
       </c>
@@ -1542,16 +1656,19 @@
         <v>110</v>
       </c>
       <c r="J9" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="K9" t="s">
-        <v>260</v>
-      </c>
-      <c r="L9" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="M9" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D10" s="4" t="s">
         <v>2</v>
       </c>
@@ -1566,16 +1683,17 @@
         <v>114</v>
       </c>
       <c r="J10" t="s">
-        <v>205</v>
-      </c>
-      <c r="K10" t="s">
-        <v>261</v>
-      </c>
-      <c r="L10" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="L10" s="9"/>
+      <c r="M10" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D11" s="4" t="s">
         <v>7</v>
       </c>
@@ -1593,16 +1711,16 @@
         <v>166</v>
       </c>
       <c r="J11" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K11" t="s">
-        <v>262</v>
-      </c>
-      <c r="L11" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="M11" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D12" s="4" t="s">
         <v>7</v>
       </c>
@@ -1616,16 +1734,17 @@
         <v>150</v>
       </c>
       <c r="J12" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>263</v>
-      </c>
-      <c r="L12" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="L12" s="9"/>
+      <c r="M12" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D13" s="4" t="s">
         <v>7</v>
       </c>
@@ -1637,13 +1756,13 @@
       </c>
       <c r="G13" s="9"/>
       <c r="J13" t="s">
-        <v>208</v>
-      </c>
-      <c r="L13" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="M13" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D14" s="4" t="s">
         <v>11</v>
       </c>
@@ -1658,16 +1777,17 @@
         <v>167</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="L14" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="L14" s="9"/>
+      <c r="M14" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D15" s="4" t="s">
         <v>11</v>
       </c>
@@ -1678,13 +1798,13 @@
         <v>168</v>
       </c>
       <c r="J15" t="s">
-        <v>210</v>
-      </c>
-      <c r="L15" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="M15" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D16" s="4" t="s">
         <v>14</v>
       </c>
@@ -1694,11 +1814,11 @@
       <c r="I16" t="s">
         <v>169</v>
       </c>
-      <c r="L16" s="5" t="s">
+      <c r="M16" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D17" s="4" t="s">
         <v>14</v>
       </c>
@@ -1706,14 +1826,15 @@
         <v>16</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K17" s="9"/>
-      <c r="L17" s="5" t="s">
+      <c r="L17" s="9"/>
+      <c r="M17" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D18" s="4" t="s">
         <v>14</v>
       </c>
@@ -1725,13 +1846,16 @@
       </c>
       <c r="G18" s="9"/>
       <c r="J18" t="s">
-        <v>212</v>
-      </c>
-      <c r="L18" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="L18" t="s">
+        <v>302</v>
+      </c>
+      <c r="M18" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D19" s="4" t="s">
         <v>7</v>
       </c>
@@ -1739,13 +1863,13 @@
         <v>18</v>
       </c>
       <c r="J19" t="s">
-        <v>213</v>
-      </c>
-      <c r="L19" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="M19" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D20" s="4" t="s">
         <v>7</v>
       </c>
@@ -1757,13 +1881,13 @@
       </c>
       <c r="G20" s="9"/>
       <c r="J20" t="s">
-        <v>214</v>
-      </c>
-      <c r="L20" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="M20" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D21" s="4" t="s">
         <v>7</v>
       </c>
@@ -1771,13 +1895,13 @@
         <v>20</v>
       </c>
       <c r="K21" t="s">
-        <v>265</v>
-      </c>
-      <c r="L21" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="M21" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D22" s="4" t="s">
         <v>21</v>
       </c>
@@ -1789,21 +1913,21 @@
       </c>
       <c r="G22" s="9"/>
       <c r="J22" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K22" t="s">
-        <v>266</v>
-      </c>
-      <c r="L22" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="M22" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D23" s="2"/>
       <c r="E23" s="3"/>
-      <c r="L23" s="3"/>
-    </row>
-    <row r="24" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M23" s="3"/>
+    </row>
+    <row r="24" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D24" s="4" t="s">
         <v>23</v>
       </c>
@@ -1816,13 +1940,13 @@
         <v>170</v>
       </c>
       <c r="J24" t="s">
-        <v>216</v>
-      </c>
-      <c r="L24" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="M24" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D25" s="4" t="s">
         <v>23</v>
       </c>
@@ -1830,13 +1954,16 @@
         <v>25</v>
       </c>
       <c r="J25" t="s">
-        <v>217</v>
-      </c>
-      <c r="L25" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="L25" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="M25" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D26" s="4" t="s">
         <v>23</v>
       </c>
@@ -1848,57 +1975,57 @@
       </c>
       <c r="G26" s="9"/>
       <c r="J26" t="s">
-        <v>218</v>
-      </c>
-      <c r="L26" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="M26" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D27" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="L27" s="5" t="s">
+      <c r="M27" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D28" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="L28" s="5" t="s">
+      <c r="M28" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D29" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="L29" s="5" t="s">
+      <c r="M29" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D30" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="L30" s="5" t="s">
+      <c r="M30" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D31" s="4" t="s">
         <v>31</v>
       </c>
@@ -1909,22 +2036,25 @@
         <v>124</v>
       </c>
       <c r="G31" s="9"/>
-      <c r="L31" s="5" t="s">
+      <c r="L31" t="s">
+        <v>304</v>
+      </c>
+      <c r="M31" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="4:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D32" s="7" t="s">
         <v>34</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="L32" s="8" t="s">
+      <c r="M32" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="4:12" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D33" s="4" t="s">
         <v>34</v>
       </c>
@@ -1936,24 +2066,27 @@
       </c>
       <c r="G33" s="9"/>
       <c r="K33" t="s">
-        <v>267</v>
-      </c>
-      <c r="L33" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="L33" t="s">
+        <v>305</v>
+      </c>
+      <c r="M33" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="4:12" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D34" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="L34" s="5" t="s">
+      <c r="M34" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="4:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D35" s="4" t="s">
         <v>38</v>
       </c>
@@ -1961,13 +2094,13 @@
         <v>39</v>
       </c>
       <c r="K35" t="s">
-        <v>268</v>
-      </c>
-      <c r="L35" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="M35" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="4:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D36" s="4" t="s">
         <v>34</v>
       </c>
@@ -1977,16 +2110,16 @@
       <c r="I36" t="s">
         <v>171</v>
       </c>
-      <c r="L36" s="5" t="s">
+      <c r="M36" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D37" s="2"/>
       <c r="E37" s="3"/>
-      <c r="L37" s="3"/>
-    </row>
-    <row r="38" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M37" s="3"/>
+    </row>
+    <row r="38" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D38" s="4" t="s">
         <v>41</v>
       </c>
@@ -1998,16 +2131,16 @@
       </c>
       <c r="G38" s="9"/>
       <c r="J38" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="K38" t="s">
-        <v>269</v>
-      </c>
-      <c r="L38" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="M38" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D39" s="4" t="s">
         <v>41</v>
       </c>
@@ -2019,16 +2152,16 @@
       </c>
       <c r="G39" s="9"/>
       <c r="J39" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="K39" t="s">
-        <v>270</v>
-      </c>
-      <c r="L39" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="M39" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D40" s="4" t="s">
         <v>41</v>
       </c>
@@ -2042,13 +2175,16 @@
         <v>151</v>
       </c>
       <c r="J40" t="s">
-        <v>223</v>
-      </c>
-      <c r="L40" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="L40" t="s">
+        <v>306</v>
+      </c>
+      <c r="M40" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D41" s="4" t="s">
         <v>41</v>
       </c>
@@ -2056,16 +2192,16 @@
         <v>45</v>
       </c>
       <c r="J41" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="K41" t="s">
-        <v>271</v>
-      </c>
-      <c r="L41" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="M41" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D42" s="4" t="s">
         <v>41</v>
       </c>
@@ -2073,14 +2209,15 @@
         <v>46</v>
       </c>
       <c r="J42" s="9" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="K42" s="9"/>
-      <c r="L42" s="5" t="s">
+      <c r="L42" s="9"/>
+      <c r="M42" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="43" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D43" s="4" t="s">
         <v>41</v>
       </c>
@@ -2092,18 +2229,18 @@
       </c>
       <c r="G43" s="9"/>
       <c r="J43" t="s">
-        <v>222</v>
-      </c>
-      <c r="L43" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="M43" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D44" s="2"/>
       <c r="E44" s="3"/>
-      <c r="L44" s="3"/>
-    </row>
-    <row r="45" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M44" s="3"/>
+    </row>
+    <row r="45" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D45" s="4" t="s">
         <v>48</v>
       </c>
@@ -2111,13 +2248,16 @@
         <v>49</v>
       </c>
       <c r="K45" t="s">
-        <v>273</v>
-      </c>
-      <c r="L45" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="L45" t="s">
+        <v>307</v>
+      </c>
+      <c r="M45" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D46" s="4" t="s">
         <v>48</v>
       </c>
@@ -2129,16 +2269,19 @@
       </c>
       <c r="G46" s="9"/>
       <c r="J46" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="K46" s="9" t="s">
-        <v>272</v>
-      </c>
-      <c r="L46" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="L46" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="M46" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D47" s="4" t="s">
         <v>48</v>
       </c>
@@ -2146,11 +2289,11 @@
         <v>51</v>
       </c>
       <c r="H47" s="9"/>
-      <c r="L47" s="5" t="s">
+      <c r="M47" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="48" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D48" s="4" t="s">
         <v>52</v>
       </c>
@@ -2161,23 +2304,26 @@
         <v>132</v>
       </c>
       <c r="G48" s="9"/>
-      <c r="H48" t="s">
+      <c r="H48" s="9" t="s">
         <v>130</v>
       </c>
       <c r="I48" t="s">
         <v>172</v>
       </c>
       <c r="J48" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K48" t="s">
-        <v>274</v>
-      </c>
-      <c r="L48" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="L48" t="s">
+        <v>309</v>
+      </c>
+      <c r="M48" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D49" s="4" t="s">
         <v>52</v>
       </c>
@@ -2189,16 +2335,16 @@
       </c>
       <c r="G49" s="9"/>
       <c r="J49" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="K49" t="s">
-        <v>275</v>
-      </c>
-      <c r="L49" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="M49" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D50" s="4" t="s">
         <v>52</v>
       </c>
@@ -2209,14 +2355,15 @@
         <v>172</v>
       </c>
       <c r="J50" s="9" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="K50" s="9"/>
-      <c r="L50" s="5" t="s">
+      <c r="L50" s="9"/>
+      <c r="M50" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D51" s="4" t="s">
         <v>52</v>
       </c>
@@ -2224,13 +2371,13 @@
         <v>56</v>
       </c>
       <c r="J51" t="s">
-        <v>229</v>
-      </c>
-      <c r="L51" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="M51" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="52" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D52" s="4" t="s">
         <v>57</v>
       </c>
@@ -2238,40 +2385,43 @@
         <v>58</v>
       </c>
       <c r="K52" t="s">
-        <v>276</v>
-      </c>
-      <c r="L52" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="M52" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="53" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D53" s="4" t="s">
         <v>57</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="L53" s="5" t="s">
+      <c r="L53" t="s">
+        <v>310</v>
+      </c>
+      <c r="M53" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="54" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D54" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="L54" s="5" t="s">
+      <c r="M54" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="55" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D55" s="2"/>
       <c r="E55" s="3"/>
-      <c r="L55" s="3"/>
-    </row>
-    <row r="56" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M55" s="3"/>
+    </row>
+    <row r="56" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D56" s="4" t="s">
         <v>62</v>
       </c>
@@ -2286,16 +2436,19 @@
         <v>174</v>
       </c>
       <c r="J56" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="K56" t="s">
-        <v>277</v>
-      </c>
-      <c r="L56" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="L56" t="s">
+        <v>311</v>
+      </c>
+      <c r="M56" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="57" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="4" t="s">
         <v>62</v>
       </c>
@@ -2303,19 +2456,22 @@
         <v>64</v>
       </c>
       <c r="J57" t="s">
-        <v>231</v>
-      </c>
-      <c r="L57" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="M57" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="58" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="4" t="s">
         <v>62</v>
       </c>
       <c r="E58" s="5" t="s">
         <v>65</v>
       </c>
+      <c r="F58" t="s">
+        <v>290</v>
+      </c>
       <c r="H58" t="s">
         <v>161</v>
       </c>
@@ -2323,24 +2479,25 @@
         <v>173</v>
       </c>
       <c r="J58" t="s">
-        <v>232</v>
-      </c>
-      <c r="K58" t="s">
-        <v>278</v>
-      </c>
-      <c r="L58" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="K58" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="L58" s="9"/>
+      <c r="M58" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="59" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D59" s="2"/>
       <c r="E59" s="3"/>
       <c r="I59" t="s">
         <v>175</v>
       </c>
-      <c r="L59" s="3"/>
-    </row>
-    <row r="60" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M59" s="3"/>
+    </row>
+    <row r="60" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D60" s="4" t="s">
         <v>66</v>
       </c>
@@ -2355,16 +2512,16 @@
         <v>176</v>
       </c>
       <c r="J60" s="9" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K60" t="s">
-        <v>279</v>
-      </c>
-      <c r="L60" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="M60" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="61" spans="4:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D61" s="4" t="s">
         <v>66</v>
       </c>
@@ -2372,56 +2529,68 @@
         <v>68</v>
       </c>
       <c r="J61" t="s">
-        <v>234</v>
-      </c>
-      <c r="L61" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="M61" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="62" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D62" s="4" t="s">
         <v>66</v>
       </c>
       <c r="E62" s="5" t="s">
         <v>69</v>
       </c>
+      <c r="F62" t="s">
+        <v>292</v>
+      </c>
       <c r="I62" t="s">
         <v>177</v>
       </c>
       <c r="J62" t="s">
-        <v>235</v>
-      </c>
-      <c r="L62" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="M62" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="63" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D63" s="4" t="s">
         <v>66</v>
       </c>
       <c r="E63" s="5" t="s">
         <v>70</v>
       </c>
+      <c r="F63" s="9" t="s">
+        <v>291</v>
+      </c>
       <c r="I63" t="s">
         <v>178</v>
       </c>
       <c r="J63" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="K63" t="s">
-        <v>280</v>
-      </c>
-      <c r="L63" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="L63" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="M63" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="64" spans="4:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D64" s="4" t="s">
         <v>66</v>
       </c>
       <c r="E64" s="5" t="s">
         <v>71</v>
       </c>
+      <c r="F64" t="s">
+        <v>293</v>
+      </c>
       <c r="G64" t="s">
         <v>152</v>
       </c>
@@ -2429,16 +2598,19 @@
         <v>179</v>
       </c>
       <c r="J64" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K64" t="s">
-        <v>281</v>
-      </c>
-      <c r="L64" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="L64" t="s">
+        <v>313</v>
+      </c>
+      <c r="M64" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="65" spans="4:12" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="4:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D65" s="4" t="s">
         <v>66</v>
       </c>
@@ -2452,38 +2624,41 @@
         <v>180</v>
       </c>
       <c r="J65" t="s">
-        <v>238</v>
-      </c>
-      <c r="L65" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="M65" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="4:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D66" s="4" t="s">
         <v>66</v>
       </c>
       <c r="E66" s="5" t="s">
         <v>73</v>
       </c>
+      <c r="F66" t="s">
+        <v>294</v>
+      </c>
       <c r="G66" t="s">
         <v>154</v>
       </c>
       <c r="I66" t="s">
         <v>181</v>
       </c>
-      <c r="L66" s="5" t="s">
+      <c r="M66" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D67" s="2"/>
       <c r="E67" s="3"/>
       <c r="I67" t="s">
         <v>182</v>
       </c>
-      <c r="L67" s="3"/>
-    </row>
-    <row r="68" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M67" s="3"/>
+    </row>
+    <row r="68" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D68" s="4" t="s">
         <v>74</v>
       </c>
@@ -2494,16 +2669,19 @@
         <v>155</v>
       </c>
       <c r="J68" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="K68" t="s">
-        <v>282</v>
-      </c>
-      <c r="L68" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="L68" t="s">
+        <v>314</v>
+      </c>
+      <c r="M68" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="69" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D69" s="4" t="s">
         <v>74</v>
       </c>
@@ -2517,16 +2695,19 @@
         <v>156</v>
       </c>
       <c r="J69" s="9" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="K69" s="9" t="s">
-        <v>283</v>
-      </c>
-      <c r="L69" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="L69" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="M69" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="70" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D70" s="4" t="s">
         <v>74</v>
       </c>
@@ -2536,11 +2717,11 @@
       <c r="I70" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="L70" s="5" t="s">
+      <c r="M70" s="5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="71" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D71" s="4" t="s">
         <v>74</v>
       </c>
@@ -2557,13 +2738,13 @@
         <v>184</v>
       </c>
       <c r="J71" t="s">
-        <v>241</v>
-      </c>
-      <c r="L71" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="M71" s="5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="72" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D72" s="4" t="s">
         <v>74</v>
       </c>
@@ -2576,14 +2757,17 @@
       <c r="I72" t="s">
         <v>185</v>
       </c>
-      <c r="K72" t="s">
-        <v>284</v>
-      </c>
-      <c r="L72" s="5" t="s">
+      <c r="K72" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="L72" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="M72" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="73" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D73" s="4" t="s">
         <v>74</v>
       </c>
@@ -2594,14 +2778,15 @@
         <v>186</v>
       </c>
       <c r="J73" s="9" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="K73" s="9"/>
-      <c r="L73" s="5" t="s">
+      <c r="L73" s="9"/>
+      <c r="M73" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="74" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D74" s="4" t="s">
         <v>74</v>
       </c>
@@ -2612,21 +2797,21 @@
         <v>163</v>
       </c>
       <c r="J74" t="s">
-        <v>243</v>
-      </c>
-      <c r="L74" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="M74" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="75" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D75" s="2"/>
       <c r="E75" s="3"/>
       <c r="I75" t="s">
         <v>187</v>
       </c>
-      <c r="L75" s="3"/>
-    </row>
-    <row r="76" spans="4:12" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M75" s="3"/>
+    </row>
+    <row r="76" spans="4:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D76" s="4" t="s">
         <v>82</v>
       </c>
@@ -2640,13 +2825,16 @@
         <v>157</v>
       </c>
       <c r="J76" t="s">
-        <v>244</v>
-      </c>
-      <c r="L76" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="L76" t="s">
+        <v>317</v>
+      </c>
+      <c r="M76" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="77" spans="4:12" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="4:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D77" s="4" t="s">
         <v>82</v>
       </c>
@@ -2658,13 +2846,16 @@
       </c>
       <c r="G77" s="9"/>
       <c r="J77" t="s">
-        <v>245</v>
-      </c>
-      <c r="L77" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="L77" t="s">
+        <v>318</v>
+      </c>
+      <c r="M77" s="5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="78" spans="4:12" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="4:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D78" s="4" t="s">
         <v>85</v>
       </c>
@@ -2678,14 +2869,14 @@
       <c r="H78" t="s">
         <v>164</v>
       </c>
-      <c r="I78" t="s">
-        <v>188</v>
-      </c>
-      <c r="L78" s="5" t="s">
+      <c r="I78" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="M78" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="79" spans="4:12" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="4:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D79" s="4" t="s">
         <v>85</v>
       </c>
@@ -2700,13 +2891,16 @@
         <v>165</v>
       </c>
       <c r="J79" t="s">
-        <v>246</v>
-      </c>
-      <c r="L79" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="L79" t="s">
+        <v>319</v>
+      </c>
+      <c r="M79" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="80" spans="4:12" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="4:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D80" s="4" t="s">
         <v>85</v>
       </c>
@@ -2717,19 +2911,19 @@
         <v>143</v>
       </c>
       <c r="I80" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J80" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="K80" t="s">
-        <v>285</v>
-      </c>
-      <c r="L80" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="M80" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="81" spans="4:12" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="4:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D81" s="4" t="s">
         <v>85</v>
       </c>
@@ -2740,16 +2934,16 @@
         <v>144</v>
       </c>
       <c r="I81" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J81" t="s">
-        <v>248</v>
-      </c>
-      <c r="L81" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="M81" s="5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="82" spans="4:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D82" s="4" t="s">
         <v>85</v>
       </c>
@@ -2761,24 +2955,24 @@
       </c>
       <c r="G82" s="9"/>
       <c r="I82" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J82" t="s">
-        <v>249</v>
-      </c>
-      <c r="L82" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="M82" s="5" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="83" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D83" s="2"/>
       <c r="E83" s="3"/>
       <c r="I83" t="s">
-        <v>192</v>
-      </c>
-      <c r="L83" s="3"/>
-    </row>
-    <row r="84" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>299</v>
+      </c>
+      <c r="M83" s="3"/>
+    </row>
+    <row r="84" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D84" s="4" t="s">
         <v>91</v>
       </c>
@@ -2792,27 +2986,30 @@
         <v>158</v>
       </c>
       <c r="I84" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="J84" t="s">
-        <v>250</v>
-      </c>
-      <c r="L84" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="K84" t="s">
+        <v>298</v>
+      </c>
+      <c r="M84" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="85" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D85" s="4" t="s">
         <v>91</v>
       </c>
       <c r="E85" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="L85" s="5" t="s">
+      <c r="M85" s="5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="86" spans="4:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D86" s="4" t="s">
         <v>91</v>
       </c>
@@ -2820,19 +3017,19 @@
         <v>94</v>
       </c>
       <c r="I86" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J86" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="K86" t="s">
-        <v>286</v>
-      </c>
-      <c r="L86" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="M86" s="5" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="87" spans="4:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D87" s="4" t="s">
         <v>91</v>
       </c>
@@ -2840,30 +3037,33 @@
         <v>95</v>
       </c>
       <c r="I87" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J87" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="K87" t="s">
-        <v>287</v>
-      </c>
-      <c r="L87" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="L87" t="s">
+        <v>320</v>
+      </c>
+      <c r="M87" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="88" spans="4:12" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="4:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D88" s="4" t="s">
         <v>96</v>
       </c>
       <c r="E88" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="L88" s="5" t="s">
+      <c r="M88" s="5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="89" spans="4:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D89" s="4" t="s">
         <v>98</v>
       </c>
@@ -2871,24 +3071,24 @@
         <v>99</v>
       </c>
       <c r="I89" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J89" t="s">
-        <v>253</v>
-      </c>
-      <c r="L89" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="M89" s="5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="90" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D90" s="2"/>
       <c r="E90" s="3"/>
       <c r="I90" t="s">
-        <v>197</v>
-      </c>
-      <c r="L90" s="3"/>
-    </row>
-    <row r="91" spans="4:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+      <c r="M90" s="3"/>
+    </row>
+    <row r="91" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D91" s="4" t="s">
         <v>100</v>
       </c>
@@ -2896,51 +3096,62 @@
         <v>101</v>
       </c>
       <c r="I91" t="s">
-        <v>198</v>
-      </c>
-      <c r="L91" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="M91" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="92" spans="4:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D92" s="4" t="s">
         <v>100</v>
       </c>
       <c r="E92" s="5" t="s">
         <v>102</v>
       </c>
+      <c r="F92" t="s">
+        <v>296</v>
+      </c>
       <c r="J92" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="K92" t="s">
-        <v>288</v>
-      </c>
-      <c r="L92" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="L92" t="s">
+        <v>323</v>
+      </c>
+      <c r="M92" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="93" spans="4:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D93" s="4" t="s">
         <v>100</v>
       </c>
       <c r="E93" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="F93" s="9"/>
+      <c r="F93" s="9" t="s">
+        <v>295</v>
+      </c>
       <c r="G93" s="9" t="s">
         <v>159</v>
       </c>
       <c r="J93" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="K93" t="s">
-        <v>289</v>
-      </c>
-      <c r="L93" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="L93" t="s">
+        <v>321</v>
+      </c>
+      <c r="M93" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="94" spans="4:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D94" s="4" t="s">
         <v>100</v>
       </c>
@@ -2948,19 +3159,19 @@
         <v>104</v>
       </c>
       <c r="I94" s="9" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J94" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="K94" t="s">
-        <v>290</v>
-      </c>
-      <c r="L94" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="M94" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="95" spans="4:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D95" s="4" t="s">
         <v>100</v>
       </c>
@@ -2971,12 +3182,15 @@
         <v>147</v>
       </c>
       <c r="I95" s="9" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="K95" t="s">
-        <v>291</v>
-      </c>
-      <c r="L95" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="L95" t="s">
+        <v>322</v>
+      </c>
+      <c r="M95" s="5" t="s">
         <v>105</v>
       </c>
     </row>
@@ -3028,9 +3242,17 @@
     <hyperlink ref="K12" r:id="rId43" xr:uid="{06AD9E37-3909-452B-AF07-1A08C94977D7}"/>
     <hyperlink ref="K46" r:id="rId44" xr:uid="{96CAC567-3F0E-49CA-8DEC-F36C45823856}"/>
     <hyperlink ref="J60" r:id="rId45" xr:uid="{159BA102-A07E-4CCA-B39C-0649E37DABAB}"/>
-    <hyperlink ref="K7" r:id="rId46" xr:uid="{7035E742-78D6-48F9-9CFF-F9BF634E5A01}"/>
+    <hyperlink ref="F63" r:id="rId46" xr:uid="{02308EB3-0D4F-43E5-B4E2-B6F6C09AEFBB}"/>
+    <hyperlink ref="K7" r:id="rId47" xr:uid="{12963AA2-BE9C-48F6-ADD3-656C6E23B39C}"/>
+    <hyperlink ref="H48" r:id="rId48" xr:uid="{8E5E12B2-C9E3-4CE9-A709-1339EBF59243}"/>
+    <hyperlink ref="K10" r:id="rId49" xr:uid="{A00C7BE9-6CBD-4A4B-AB12-2C62A70BE084}"/>
+    <hyperlink ref="K58" r:id="rId50" xr:uid="{7593D602-EECA-4B89-A6ED-6CF677EB1C0D}"/>
+    <hyperlink ref="K72" r:id="rId51" xr:uid="{46977EFB-3B7E-4A69-822A-E021388A83CE}"/>
+    <hyperlink ref="L63" r:id="rId52" xr:uid="{A6E2704C-7779-416A-BF8F-0168747F4B17}"/>
+    <hyperlink ref="L9" r:id="rId53" xr:uid="{46BB625B-5DD0-40C1-B43C-C15BBCE72883}"/>
+    <hyperlink ref="L25" r:id="rId54" xr:uid="{F005BE67-DBF7-4D9F-BEDA-F1C1FD409FD3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId47"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId55"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added new data to db
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mihail\PycharmProjects\parce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B9C73AD-58D9-445E-8CC9-E0F771BBAB86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA835E5-A3CB-4412-BA29-38058CE40D66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{FFE27364-2778-47AC-8397-2059D7069E9C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="335">
   <si>
     <t>Бренд</t>
   </si>
@@ -366,9 +366,6 @@
     <t>https://www.perekrestok.ru/cat/417/p/kotlety-morozko-green-ovosnye-150g-3507842</t>
   </si>
   <si>
-    <t>https://www.ozon.ru/product/pelmeni-tsezar-gosudar-imperator-800-g-162288228/?sh=K5xV8Qbdkw</t>
-  </si>
-  <si>
     <t>https://online.metro-cc.ru/category/gotovye-bljuda-polufabrikaty/pelmeni-vareniki/cezar-gosudar-imperator-800g</t>
   </si>
   <si>
@@ -621,12 +618,6 @@
     <t>https://www.ozon.ru/product/stiralnyy-poroshok-detskiy-ushastyy-nyan-gipoallergennyy-0-2-4-kg-172622421/?asb=m6mKjPTymXCcI2Or18lU0oJvTQ0QJiKq6q53A71Opaw%253D&amp;asb2=eM-rr3bGfQ9lNcdnbdf6ngawAaZtgkCxzc7-E228u9mF2QUyNYNzNqIBRQQF1f3b&amp;keywords=%D0%A1%D1%82%D0%B8%D1%80%D0%B0%D0%BB%D1%8C%D0%BD%D1%8B%D0%B9+%D0%BF%D0%BE%D1%80%D0%BE%D1%88%D0%BE%D0%BA+%D0%B4%D0%BB%D1%8F+%D0%B4%D0%B5%D1%82%D1%81%D0%BA%D0%BE%D0%B3%D0%BE+%D0%B1%D0%B5%D0%BB%D1%8C%D1%8F+%C2%AB%D0%A3%D1%88%D0%B0%D1%81%D1%82%D1%8B%D0%B9+%D0%BD%D1%8F%D0%BD%D1%8C%C2%BB%2C+2%2C4+%D0%BA%D0%B3.&amp;sh=K5xV8Tp3GQ</t>
   </si>
   <si>
-    <t>https://www.ozon.ru/product/vorsinka-sredstvo-d-stirki-d-shersti-i-delikatnyh-tkaney-1-2-l-318960508/?asb=FjaFHD2F6r8QXNM1AaacatHGS882f5RksVS26tlVamE%253D&amp;asb2=eo_vImhJnV6ONQsfICRKPaf-_6pAcuxPXaQ6i9SQ-gDpjYS4ym4IZqzf-L3zcw7o&amp;keywords=%D1%81%D1%80%D0%B5%D0%B4%D1%81%D1%82%D0%B2%D0%BE+%D0%B4%D0%BB%D1%8F+%D1%81%D1%82%D0%B8%D1%80%D0%BA%D0%B8+%D1%88%D0%B5%D1%80%D1%81%D1%82%D1%8F%D0%BD%D1%8B%D1%85+%D0%B8+%D0%B4%D0%B5%D0%BB%D0%B8%D0%BA%D0%B0%D1%82%D0%BD%D1%8B%D1%85+%D1%82%D0%BA%D0%B0%D0%BD%D0%B5%D0%B9+%C2%AB%D0%92%D0%BE%D1%80%D1%81%D0%B8%D0%BD%D0%BA%D0%B0%C2%BB%2C+1%2C2+%D0%BB.&amp;sh=K5xV8S8H-Q</t>
-  </si>
-  <si>
-    <t>https://www.ozon.ru/product/zubnaya-pasta-novyy-zhemchug-sem-trav-100-ml-4-sht-147240451/?asb=92fMnqLmECeYUhW3cKCl6da73rYwfKCYUVna5kcMry8%253D&amp;asb2=91kjH_mPPDx23IDJ063DVAYT0i9iwKQCetHw6zOm2NBSpmPkSv48UvaGbyK_PNR_&amp;ectx=1&amp;keywords=%D0%97%D1%83%D0%B1%D0%BD%D0%B0%D1%8F+%D0%BF%D0%B0%D1%81%D1%82%D0%B0+%C2%AB%D0%9D%D0%BE%D0%B2%D1%8B%D0%B9+%D0%96%D0%B5%D0%BC%D1%87%D1%83%D0%B3+%D0%A1%D0%B5%D0%BC%D1%8C+%D1%82%D1%80%D0%B0%D0%B2%C2%BB%2C+100+%D0%BC%D0%BB.&amp;miniapp=supermarket&amp;sh=K5xV8eXYOg</t>
-  </si>
-  <si>
     <t>https://www.ozon.ru/product/brest-litovsk-maslo-sladko-slivochnoe-nesolenoe-82-5-180-g-145923184/?asb=jIkcWaZ8F2DraHiq9EkWSqHPHpJGeby2dptq6D3zZMw%253D&amp;asb2=jU54E3oIkNKIgSViutQjlT_4Mgd1c3ms7hb00oP7TOiu8wiJapREib7WfJBxMz2F&amp;ectx=1&amp;keywords=%D0%91%D1%80%D0%B5%D1%81%D1%82+%D0%9B%D0%B8%D1%82%D0%BE%D0%B2%D1%81%D0%BA&amp;miniapp=supermarket&amp;sh=K5xV8Xe3Fg</t>
   </si>
   <si>
@@ -1006,6 +997,48 @@
   </si>
   <si>
     <t>https://dostavka.dixy.ru/catalog/molochnye_produkty_yaytsa/slivochnoe_maslo_margarin_spred/132835/</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/371/p/syr-kiprino-svejcarskij-50-125g-4096580</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/394/p/majonez-raba-provansal-67-400ml-3277399</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/376/p/margarin-slivocnyj-hozauska-nizegorodskij-60-200g-58471</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/471/p/porosok-stiralnyj-usastyj-nan-dla-detskogo-bela-2-4kg-3010586</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3059759/shnicel-sytoedov-s-kartofelnym-pjure-pod-krasnym-sousom-zamorozhennyj-350-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3062492/grudka-kurinaja-sytoedov-v-teste-s-sousom-sjuprem-i-kartofelnym-pjure-zamorozhennoe-350-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3076743/chebureki-chebureche-govjadina-i-svinina-zamorozhennye-280-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3187671/sup-sytoedov-gorokhovyj-s-govjadinoj-zamorozhennyj-300-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3223483/muka-makfa-pshenichnaja-vysshij-sort-2-kg</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3360771/sredstvo-dlja-stirki-biomio-bio-sensitive-dlja-delikatnykh-tkanej-gel-1-5-l</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3410194/tvorog-savushkin-rassypchatyj-5-350-g</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/pelmeni-imperator-tsezar-zamorozhennye-800-g-360092984/?asb=qjxJOzyaP5eiIp3dFFhocI2vC%252B0BwHzNexEcZ6ME9vI%253D&amp;asb2=kIq6DZcBFl2HVot5SyrOtbinVyUMRC8Yhi57ws0_MSIKiAv1lBgKMWLbe0sKN4G1&amp;ectx=1&amp;keywords=%D1%86%D0%B5%D0%B7%D0%B0%D1%80%D1%8C&amp;miniapp=supermarket&amp;sh=K5xV8Uep1Q</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/gel-dlya-stirki-vorsinka-dlya-chernyh-i-temnyh-veshchey-bez-fosfatov-1-2-l-547683262/?asb=lTppReURzvBkEidramqdCzOt4GVtAdPku3nQt1M8DL4%253D&amp;asb2=kOdgFDWVvuoLQyH6CJ5i0c9hB5Y_j8xiNIALt1GfCpUwUFTVS1vpQntZ_Spd3snC&amp;keywords=%D0%B2%D0%BE%D1%80%D1%81%D0%B8%D0%BD%D0%BA%D0%B0&amp;sh=K5xV8Zl-aA</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/zamorozhennye_produkty/gotovaya_eda_1/133090/</t>
   </si>
 </sst>
 </file>
@@ -1543,10 +1576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF1A69E3-A9E5-424F-8F16-B76B324D2ACC}">
-  <dimension ref="D5:M95"/>
+  <dimension ref="D5:M98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J88" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O92" sqref="O92"/>
+    <sheetView tabSelected="1" topLeftCell="J34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1572,7 +1605,7 @@
         <v>106</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H6" s="11" t="s">
         <v>107</v>
@@ -1581,13 +1614,13 @@
         <v>108</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="M6" s="13" t="s">
         <v>1</v>
@@ -1601,16 +1634,16 @@
         <v>3</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J7" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="L7" s="9"/>
       <c r="M7" s="5" t="s">
@@ -1625,14 +1658,14 @@
         <v>4</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G8" s="9"/>
       <c r="J8" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="K8" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="M8" s="6" t="s">
         <v>4</v>
@@ -1646,23 +1679,23 @@
         <v>5</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>110</v>
+        <v>332</v>
       </c>
       <c r="J9" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="K9" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="L9" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="M9" s="5" t="s">
         <v>5</v>
@@ -1676,17 +1709,17 @@
         <v>6</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G10" s="9"/>
       <c r="I10" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J10" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="L10" s="9"/>
       <c r="M10" s="5" t="s">
@@ -1701,20 +1734,20 @@
         <v>8</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G11" s="9"/>
       <c r="H11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J11" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="K11" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="M11" s="5" t="s">
         <v>8</v>
@@ -1728,16 +1761,16 @@
         <v>9</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J12" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="L12" s="9"/>
       <c r="M12" s="5" t="s">
@@ -1752,11 +1785,11 @@
         <v>10</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G13" s="9"/>
       <c r="J13" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="M13" s="5" t="s">
         <v>10</v>
@@ -1770,17 +1803,17 @@
         <v>12</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G14" s="9"/>
       <c r="I14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="L14" s="9"/>
       <c r="M14" s="5" t="s">
@@ -1795,10 +1828,10 @@
         <v>13</v>
       </c>
       <c r="I15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J15" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="M15" s="5" t="s">
         <v>13</v>
@@ -1812,7 +1845,7 @@
         <v>15</v>
       </c>
       <c r="I16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M16" s="5" t="s">
         <v>15</v>
@@ -1826,7 +1859,7 @@
         <v>16</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="K17" s="9"/>
       <c r="L17" s="9"/>
@@ -1846,10 +1879,10 @@
       </c>
       <c r="G18" s="9"/>
       <c r="J18" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="L18" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="M18" s="5" t="s">
         <v>17</v>
@@ -1863,7 +1896,7 @@
         <v>18</v>
       </c>
       <c r="J19" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="M19" s="5" t="s">
         <v>18</v>
@@ -1877,11 +1910,11 @@
         <v>19</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G20" s="9"/>
       <c r="J20" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M20" s="5" t="s">
         <v>19</v>
@@ -1895,7 +1928,7 @@
         <v>20</v>
       </c>
       <c r="K21" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="M21" s="5" t="s">
         <v>20</v>
@@ -1909,14 +1942,14 @@
         <v>22</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G22" s="9"/>
       <c r="J22" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="K22" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="M22" s="5" t="s">
         <v>22</v>
@@ -1937,10 +1970,10 @@
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
       <c r="I24" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J24" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="M24" s="5" t="s">
         <v>24</v>
@@ -1954,10 +1987,10 @@
         <v>25</v>
       </c>
       <c r="J25" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="L25" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="M25" s="5" t="s">
         <v>25</v>
@@ -1971,11 +2004,11 @@
         <v>26</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G26" s="9"/>
       <c r="J26" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="M26" s="5" t="s">
         <v>26</v>
@@ -2033,11 +2066,11 @@
         <v>33</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G31" s="9"/>
       <c r="L31" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="M31" s="5" t="s">
         <v>33</v>
@@ -2062,14 +2095,17 @@
         <v>36</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G33" s="9"/>
+      <c r="J33" t="s">
+        <v>325</v>
+      </c>
       <c r="K33" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="L33" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="M33" s="5" t="s">
         <v>36</v>
@@ -2082,6 +2118,12 @@
       <c r="E34" s="5" t="s">
         <v>37</v>
       </c>
+      <c r="J34" t="s">
+        <v>326</v>
+      </c>
+      <c r="L34" t="s">
+        <v>334</v>
+      </c>
       <c r="M34" s="5" t="s">
         <v>37</v>
       </c>
@@ -2093,8 +2135,11 @@
       <c r="E35" s="5" t="s">
         <v>39</v>
       </c>
+      <c r="J35" t="s">
+        <v>327</v>
+      </c>
       <c r="K35" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="M35" s="5" t="s">
         <v>39</v>
@@ -2108,7 +2153,10 @@
         <v>40</v>
       </c>
       <c r="I36" t="s">
-        <v>171</v>
+        <v>170</v>
+      </c>
+      <c r="J36" t="s">
+        <v>328</v>
       </c>
       <c r="M36" s="5" t="s">
         <v>40</v>
@@ -2127,14 +2175,14 @@
         <v>42</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G38" s="9"/>
       <c r="J38" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="K38" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="M38" s="5" t="s">
         <v>42</v>
@@ -2148,14 +2196,14 @@
         <v>43</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G39" s="9"/>
       <c r="J39" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="K39" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="M39" s="5" t="s">
         <v>43</v>
@@ -2169,16 +2217,16 @@
         <v>44</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J40" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="L40" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="M40" s="5" t="s">
         <v>44</v>
@@ -2191,11 +2239,14 @@
       <c r="E41" s="5" t="s">
         <v>45</v>
       </c>
+      <c r="F41" t="s">
+        <v>321</v>
+      </c>
       <c r="J41" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="K41" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="M41" s="5" t="s">
         <v>45</v>
@@ -2209,7 +2260,7 @@
         <v>46</v>
       </c>
       <c r="J42" s="9" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="K42" s="9"/>
       <c r="L42" s="9"/>
@@ -2225,11 +2276,11 @@
         <v>47</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G43" s="9"/>
       <c r="J43" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="M43" s="5" t="s">
         <v>47</v>
@@ -2247,11 +2298,14 @@
       <c r="E45" s="5" t="s">
         <v>49</v>
       </c>
+      <c r="F45" t="s">
+        <v>322</v>
+      </c>
       <c r="K45" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="L45" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="M45" s="5" t="s">
         <v>49</v>
@@ -2265,17 +2319,17 @@
         <v>50</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G46" s="9"/>
       <c r="J46" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="K46" s="9" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="L46" s="9" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="M46" s="5" t="s">
         <v>50</v>
@@ -2301,23 +2355,23 @@
         <v>53</v>
       </c>
       <c r="F48" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G48" s="9"/>
       <c r="H48" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I48" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J48" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="K48" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="L48" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="M48" s="5" t="s">
         <v>53</v>
@@ -2331,14 +2385,14 @@
         <v>54</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G49" s="9"/>
       <c r="J49" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="K49" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="M49" s="5" t="s">
         <v>54</v>
@@ -2352,10 +2406,10 @@
         <v>55</v>
       </c>
       <c r="I50" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J50" s="9" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="K50" s="9"/>
       <c r="L50" s="9"/>
@@ -2371,7 +2425,7 @@
         <v>56</v>
       </c>
       <c r="J51" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="M51" s="5" t="s">
         <v>56</v>
@@ -2385,7 +2439,7 @@
         <v>58</v>
       </c>
       <c r="K52" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="M52" s="5" t="s">
         <v>58</v>
@@ -2398,8 +2452,11 @@
       <c r="E53" s="5" t="s">
         <v>59</v>
       </c>
+      <c r="F53" t="s">
+        <v>323</v>
+      </c>
       <c r="L53" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="M53" s="5" t="s">
         <v>59</v>
@@ -2429,20 +2486,20 @@
         <v>63</v>
       </c>
       <c r="F56" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G56" s="9"/>
       <c r="I56" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J56" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="K56" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="L56" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="M56" s="5" t="s">
         <v>63</v>
@@ -2456,7 +2513,7 @@
         <v>64</v>
       </c>
       <c r="J57" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="M57" s="5" t="s">
         <v>64</v>
@@ -2470,19 +2527,19 @@
         <v>65</v>
       </c>
       <c r="F58" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="H58" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I58" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J58" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="K58" s="9" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="L58" s="9"/>
       <c r="M58" s="5" t="s">
@@ -2493,7 +2550,7 @@
       <c r="D59" s="2"/>
       <c r="E59" s="3"/>
       <c r="I59" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M59" s="3"/>
     </row>
@@ -2505,17 +2562,17 @@
         <v>67</v>
       </c>
       <c r="F60" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G60" s="9"/>
       <c r="I60" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J60" s="9" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="K60" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="M60" s="5" t="s">
         <v>67</v>
@@ -2529,7 +2586,7 @@
         <v>68</v>
       </c>
       <c r="J61" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="M61" s="5" t="s">
         <v>68</v>
@@ -2543,13 +2600,13 @@
         <v>69</v>
       </c>
       <c r="F62" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I62" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J62" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="M62" s="5" t="s">
         <v>69</v>
@@ -2563,19 +2620,19 @@
         <v>70</v>
       </c>
       <c r="F63" s="9" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="I63" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J63" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="K63" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="L63" s="9" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="M63" s="5" t="s">
         <v>70</v>
@@ -2589,22 +2646,22 @@
         <v>71</v>
       </c>
       <c r="F64" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="G64" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I64" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J64" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="K64" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="L64" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="M64" s="5" t="s">
         <v>71</v>
@@ -2618,13 +2675,13 @@
         <v>72</v>
       </c>
       <c r="G65" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I65" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J65" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="M65" s="5" t="s">
         <v>72</v>
@@ -2638,13 +2695,13 @@
         <v>73</v>
       </c>
       <c r="F66" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="G66" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I66" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M66" s="5" t="s">
         <v>73</v>
@@ -2654,7 +2711,7 @@
       <c r="D67" s="2"/>
       <c r="E67" s="3"/>
       <c r="I67" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M67" s="3"/>
     </row>
@@ -2666,16 +2723,16 @@
         <v>75</v>
       </c>
       <c r="G68" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J68" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="K68" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="L68" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="M68" s="5" t="s">
         <v>75</v>
@@ -2689,19 +2746,19 @@
         <v>76</v>
       </c>
       <c r="F69" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G69" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J69" s="9" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="K69" s="9" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="L69" s="9" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="M69" s="5" t="s">
         <v>76</v>
@@ -2715,7 +2772,7 @@
         <v>77</v>
       </c>
       <c r="I70" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M70" s="5" t="s">
         <v>77</v>
@@ -2729,16 +2786,16 @@
         <v>78</v>
       </c>
       <c r="F71" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H71" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I71" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J71" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="M71" s="5" t="s">
         <v>78</v>
@@ -2752,16 +2809,19 @@
         <v>79</v>
       </c>
       <c r="F72" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I72" t="s">
-        <v>185</v>
+        <v>184</v>
+      </c>
+      <c r="J72" t="s">
+        <v>329</v>
       </c>
       <c r="K72" s="9" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="L72" s="9" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="M72" s="5" t="s">
         <v>79</v>
@@ -2775,10 +2835,10 @@
         <v>80</v>
       </c>
       <c r="I73" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J73" s="9" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="K73" s="9"/>
       <c r="L73" s="9"/>
@@ -2794,10 +2854,10 @@
         <v>81</v>
       </c>
       <c r="H74" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J74" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="M74" s="5" t="s">
         <v>81</v>
@@ -2807,7 +2867,7 @@
       <c r="D75" s="2"/>
       <c r="E75" s="3"/>
       <c r="I75" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M75" s="3"/>
     </row>
@@ -2819,16 +2879,16 @@
         <v>83</v>
       </c>
       <c r="F76" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G76" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J76" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="L76" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="M76" s="5" t="s">
         <v>83</v>
@@ -2842,14 +2902,14 @@
         <v>84</v>
       </c>
       <c r="F77" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G77" s="9"/>
       <c r="J77" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="L77" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="M77" s="5" t="s">
         <v>84</v>
@@ -2863,14 +2923,17 @@
         <v>86</v>
       </c>
       <c r="F78" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G78" s="9"/>
       <c r="H78" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I78" s="9" t="s">
-        <v>297</v>
+        <v>294</v>
+      </c>
+      <c r="J78" t="s">
+        <v>330</v>
       </c>
       <c r="M78" s="5" t="s">
         <v>86</v>
@@ -2884,17 +2947,17 @@
         <v>87</v>
       </c>
       <c r="F79" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G79" s="9"/>
       <c r="H79" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J79" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="L79" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="M79" s="5" t="s">
         <v>87</v>
@@ -2908,16 +2971,16 @@
         <v>88</v>
       </c>
       <c r="F80" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I80" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J80" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="K80" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="M80" s="5" t="s">
         <v>88</v>
@@ -2931,13 +2994,13 @@
         <v>89</v>
       </c>
       <c r="F81" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I81" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J81" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="M81" s="5" t="s">
         <v>89</v>
@@ -2951,14 +3014,14 @@
         <v>90</v>
       </c>
       <c r="F82" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G82" s="9"/>
       <c r="I82" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J82" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="M82" s="5" t="s">
         <v>90</v>
@@ -2968,7 +3031,7 @@
       <c r="D83" s="2"/>
       <c r="E83" s="3"/>
       <c r="I83" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="M83" s="3"/>
     </row>
@@ -2980,19 +3043,19 @@
         <v>92</v>
       </c>
       <c r="F84" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G84" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I84" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J84" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="K84" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="M84" s="5" t="s">
         <v>92</v>
@@ -3017,13 +3080,13 @@
         <v>94</v>
       </c>
       <c r="I86" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J86" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="K86" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="M86" s="5" t="s">
         <v>94</v>
@@ -3036,17 +3099,20 @@
       <c r="E87" s="5" t="s">
         <v>95</v>
       </c>
+      <c r="F87" t="s">
+        <v>324</v>
+      </c>
       <c r="I87" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J87" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="K87" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="L87" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="M87" s="5" t="s">
         <v>95</v>
@@ -3071,10 +3137,10 @@
         <v>99</v>
       </c>
       <c r="I89" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J89" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="M89" s="5" t="s">
         <v>99</v>
@@ -3084,7 +3150,7 @@
       <c r="D90" s="2"/>
       <c r="E90" s="3"/>
       <c r="I90" t="s">
-        <v>195</v>
+        <v>333</v>
       </c>
       <c r="M90" s="3"/>
     </row>
@@ -3095,9 +3161,6 @@
       <c r="E91" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="I91" t="s">
-        <v>196</v>
-      </c>
       <c r="M91" s="5" t="s">
         <v>101</v>
       </c>
@@ -3110,16 +3173,16 @@
         <v>102</v>
       </c>
       <c r="F92" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="J92" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="K92" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="L92" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="M92" s="5" t="s">
         <v>102</v>
@@ -3133,19 +3196,19 @@
         <v>103</v>
       </c>
       <c r="F93" s="9" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="G93" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J93" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="K93" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="L93" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="M93" s="5" t="s">
         <v>103</v>
@@ -3159,13 +3222,13 @@
         <v>104</v>
       </c>
       <c r="I94" s="9" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J94" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="K94" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="M94" s="5" t="s">
         <v>104</v>
@@ -3179,19 +3242,24 @@
         <v>105</v>
       </c>
       <c r="F95" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I95" s="9" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="K95" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="L95" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="M95" s="5" t="s">
         <v>105</v>
+      </c>
+    </row>
+    <row r="98" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J98" t="s">
+        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -3226,7 +3294,7 @@
     <hyperlink ref="F78" r:id="rId27" xr:uid="{AE505ADC-5D84-4887-8B45-D1B047108302}"/>
     <hyperlink ref="F77" r:id="rId28" xr:uid="{4B851A94-480D-4562-A61A-EB57C6B36F7F}"/>
     <hyperlink ref="I70" r:id="rId29" display="https://www.ozon.ru/product/makfa-lyubitelskaya-vermishel-dlinnaya-spagetti-500-g-140800360/?asb=PiXAxdUD%252Fb8Q6qcfNBYgYZSa74CfvsYST7VXIKCqsI4%253D&amp;asb2=oFSDihkMWoB8nWmHdebLJHz0vIatpYbUNfq2HRXzEndDi0EfZLepBYnsQxQRgmua&amp;ectx=1&amp;keywords=%D0%BC%D0%B0%D0%BA%D1%84%D0%B0&amp;miniapp=supermarket&amp;sh=K5xV8WIg-g" xr:uid="{E76EC934-5688-487D-8CEB-7EECD8297302}"/>
-    <hyperlink ref="I9" r:id="rId30" xr:uid="{2ECD4382-FE90-4913-80D1-5C2CD19FDA74}"/>
+    <hyperlink ref="I9" r:id="rId30" display="https://www.ozon.ru/product/pelmeni-imperator-tsezar-zamorozhennye-800-g-360092984/?asb=qjxJOzyaP5eiIp3dFFhocI2vC%252B0BwHzNexEcZ6ME9vI%253D&amp;asb2=kIq6DZcBFl2HVot5SyrOtbinVyUMRC8Yhi57ws0_MSIKiAv1lBgKMWLbe0sKN4G1&amp;ectx=1&amp;keywords=%D1%86%D0%B5%D0%B7%D0%B0%D1%80%D1%8C&amp;miniapp=supermarket&amp;sh=K5xV8Uep1Q" xr:uid="{2ECD4382-FE90-4913-80D1-5C2CD19FDA74}"/>
     <hyperlink ref="I10" r:id="rId31" xr:uid="{715D8978-E09F-4537-A640-856992E7F8CB}"/>
     <hyperlink ref="I95" r:id="rId32" display="https://www.ozon.ru/product/syr-brest-litovsk-klassicheskiy-45-150-g-152141663/?asb=Tdv9tczfDa0PTKhltcp1Q6PBJg4kEMxiQyThzh5iKbU%253D&amp;asb2=gf9xWzcVUAeRvGgIa54q929unGEPpy48EadGcnul4r-wPb6gcWYx1GFdDzqUI3ln&amp;ectx=1&amp;keywords=%D0%91%D1%80%D0%B5%D1%81%D1%82+%D0%9B%D0%B8%D1%82%D0%BE%D0%B2%D1%81%D0%BA&amp;miniapp=supermarket&amp;sh=K5xV8Y4_HQ" xr:uid="{EA030594-B44A-4F70-BE65-1EAA753D15CB}"/>
     <hyperlink ref="I94" r:id="rId33" display="https://www.ozon.ru/product/brest-litovsk-maslo-sladko-slivochnoe-nesolenoe-82-5-180-g-145923184/?asb=jIkcWaZ8F2DraHiq9EkWSqHPHpJGeby2dptq6D3zZMw%253D&amp;asb2=jU54E3oIkNKIgSViutQjlT_4Mgd1c3ms7hb00oP7TOiu8wiJapREib7WfJBxMz2F&amp;ectx=1&amp;keywords=%D0%91%D1%80%D0%B5%D1%81%D1%82+%D0%9B%D0%B8%D1%82%D0%BE%D0%B2%D1%81%D0%BA&amp;miniapp=supermarket&amp;sh=K5xV8Xe3Fg" xr:uid="{B8E2B196-F6B7-4B8D-B1DC-360FE9199845}"/>

</xml_diff>

<commit_message>
new changes in db
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mihail\PycharmProjects\parce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E2C50C-9E92-44AF-969E-E262B4E027D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{361BB478-CF76-40EF-9AF7-CE4C220101EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2565" yWindow="1725" windowWidth="21600" windowHeight="11505" xr2:uid="{FFE27364-2778-47AC-8397-2059D7069E9C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{FFE27364-2778-47AC-8397-2059D7069E9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="398">
   <si>
     <t>Бренд</t>
   </si>
@@ -372,9 +372,6 @@
     <t>https://www.perekrestok.ru/cat/417/p/pelmeni-cezar-imperator-800g-3669807</t>
   </si>
   <si>
-    <t>https://www.perekrestok.ru/cat/417/p/pelmeni-cezar-carskoe-zastole-kategoria-v-750g-3658116</t>
-  </si>
-  <si>
     <t>https://www.ozon.ru/product/pelmeni-zamorozhennye-tsezar-tsarskoe-zastole-750-g-167975764/?sh=K5xV8cKooA</t>
   </si>
   <si>
@@ -498,9 +495,6 @@
     <t>https://lavka.yandex.ru/213/good/66e0df9fd4a14ce194bf001b88ee231d000200010000?searchQuery=%D0%A1%D1%83%D0%BF%20%C2%ABPho%20Bo%C2%BB%20(%D0%A4%D0%BE%20%D0%91%D0%BE)%20%D1%81%20%D1%80%D0%B8%D1%81%D0%BE%D0%B2%D0%BE%D0%B9%20%D0%BB%D0%B0%D0%BF%D1%88%D0%BE%D0%B9%20%D0%9A%D0%B0%D1%80%D1%82%D0%BE%D0%BD%D0%BD%D1%8B%D0%B9%20%D0%BA%D0%BE%D1%80%D0%BE%D0%B1%20125%20%D0%B3%D1%80&amp;searchPosition=-1</t>
   </si>
   <si>
-    <t>https://lavka.yandex.ru/213/good/dc3ca56ea30a439c91afbe14cbaa0ca9000100010001?searchQuery=%D0%A1%D0%BF%D0%B0%D0%B3%D0%B5%D1%82%D1%82%D0%B8,%20500%20%D0%B3%D1%80.&amp;searchPosition=-1</t>
-  </si>
-  <si>
     <t>https://lavka.yandex.ru/213/good/8486f37fb9ac4e42b9f2229588556fa3000100010001?searchQuery=%D0%92%D0%B5%D1%80%D0%BC%D0%B5%D1%88%D0%B5%D0%BB%D1%8C%20%D0%BF%D0%B0%D1%83%D1%82%D0%B8%D0%BD%D0%BA%D0%B0%20450%20%D0%B3%D1%80.&amp;searchPosition=-1</t>
   </si>
   <si>
@@ -630,9 +624,6 @@
     <t>https://www.utkonos.ru/item/3358100/pelmeni-cezar-gosudar-imperator-800-g</t>
   </si>
   <si>
-    <t>https://www.utkonos.ru/item/3396163/pelmeni-cezar-carskoe-zastole-750-g</t>
-  </si>
-  <si>
     <t>https://www.utkonos.ru/item/3358133/pelmeni-cezar-gordost-sibiri-800-g</t>
   </si>
   <si>
@@ -645,27 +636,12 @@
     <t>https://www.utkonos.ru/item/3057261/bliny-morozko-s-mjasom-zamorozhennye-420-g</t>
   </si>
   <si>
-    <t>https://www.utkonos.ru/item/3063161/bliny-morozko-s-tvorogom-zamorozhennye-420-g</t>
-  </si>
-  <si>
-    <t>https://www.utkonos.ru/item/3366065/picca-la-trattoria-vetchina-i-griby-zamorozhennaja-335-g</t>
-  </si>
-  <si>
-    <t>https://www.utkonos.ru/item/3366068/picca-la-trattoria-pepperoni-zamorozhennaja-335-g</t>
-  </si>
-  <si>
-    <t>https://www.utkonos.ru/item/3325035/griby-shampinony-morozko-green-rezanye-zamorozhennye-400-g</t>
-  </si>
-  <si>
     <t>https://www.utkonos.ru/item/3325041/kotlety-morozko-green-ovoshhnye-zamorozhennye</t>
   </si>
   <si>
     <t>https://www.utkonos.ru/item/3396152/kotlety-morozko-iz-govjadiny-zamorozhennye-330-g</t>
   </si>
   <si>
-    <t>https://www.utkonos.ru/item/3396150/bifshteks-morozko-mjasnoj-zamorozhennyj-330-g</t>
-  </si>
-  <si>
     <t>https://www.utkonos.ru/item/3404645/kruassan-la-reine-bez-nachinki-zamorozhennye-6-shtuk-po-70-g</t>
   </si>
   <si>
@@ -738,15 +714,9 @@
     <t>https://www.utkonos.ru/item/3381705/vermishel-sen-soy-funchoza-premium-pod-japonskim-sousom-terijaki-125-g</t>
   </si>
   <si>
-    <t>https://www.utkonos.ru/item/3371208/makaronnye-izdelija-makfa-spagetti-500-g</t>
-  </si>
-  <si>
     <t>https://www.utkonos.ru/item/3351690/makaronnye-izdelija-makfa-vermishel-pautinka-400-g</t>
   </si>
   <si>
-    <t>https://www.utkonos.ru/item/3357377/makaronnye-izdelija-makfa-spagetti-bez-gljutena-300-g</t>
-  </si>
-  <si>
     <t>https://www.utkonos.ru/item/3286457/gerkules-makfa-tradicionnyj-400-g</t>
   </si>
   <si>
@@ -933,9 +903,6 @@
     <t>https://dostavka.dixy.ru/catalog/zamorozhennye_produkty/pelmeni_vareniki_khinkali_manty/135554/</t>
   </si>
   <si>
-    <t>https://dostavka.dixy.ru/catalog/zamorozhennye_produkty/polufabrikaty/304674/</t>
-  </si>
-  <si>
     <t>https://dostavka.dixy.ru/catalog/zamorozhennye_produkty/pelmeni_vareniki_khinkali_manty/299073/</t>
   </si>
   <si>
@@ -969,9 +936,6 @@
     <t>https://dostavka.dixy.ru/catalog/bakaleya_2/makarony_pasta/132747/</t>
   </si>
   <si>
-    <t>https://dostavka.dixy.ru/catalog/bakaleya_2/makarony_pasta/134645/</t>
-  </si>
-  <si>
     <t>https://dostavka.dixy.ru/catalog/bakaleya_2/muka_vse_dlya_vypechki/134630/</t>
   </si>
   <si>
@@ -1051,6 +1015,219 @@
   </si>
   <si>
     <t>https://www.auchan.ru/product/aura-vatnye-palochki-st-100sht/</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/417/p/pelmeni-cezar-klassika-800g-3666703</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/417/p/picca-caesar-la-trattoria-s-mocarelloj-335g-3450997</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/444/p/diski-vatnye-a-samaa-hlopok-i-len-100st-4003974</t>
+  </si>
+  <si>
+    <t>https://lavka.yandex.ru/213/good/60817c2c481e48839f5e7020e04c68f7000300010000?searchQuery=%D1%86%D0%B5%D0%B7%D0%B0%D1%80%D1%8C&amp;searchPosition=-1</t>
+  </si>
+  <si>
+    <t>https://lavka.yandex.ru/213/good/d4fc8209388e4fd8a2857c2de639e89e000200010000?searchQuery=%D1%86%D0%B5%D0%B7%D0%B0%D1%80%D1%8C&amp;searchPosition=-1</t>
+  </si>
+  <si>
+    <t>https://lavka.yandex.ru/213/good/73b6f26bad35425c987f349dd2a9bd6a000300010000?searchQuery=%D0%BC%D0%BE%D1%80%D0%BE%D0%B7%D0%BA%D0%BE&amp;searchPosition=-1</t>
+  </si>
+  <si>
+    <t>https://lavka.yandex.ru/213/good/4da18a9bb696407ba92907c48e616d1e000200010001?searchQuery=%D0%BC%D0%BE%D1%80%D0%BE%D0%B7%D0%BA%D0%BE&amp;searchPosition=-1</t>
+  </si>
+  <si>
+    <t>https://lavka.yandex.ru/213/good/329d76cf004e4a2985a5b240f98c6d4d000300010000?searchQuery=sen%20soy&amp;searchPosition=-1</t>
+  </si>
+  <si>
+    <t>https://lavka.yandex.ru/213/good/813a309311324c6dbd5144bb676fd936000200010001?searchQuery=%D0%BC%D0%B0%D0%BA%D1%84%D0%B0&amp;searchPosition=-1</t>
+  </si>
+  <si>
+    <t>https://lavka.yandex.ru/213/good/ae8cc776b4e3408c836dd1e90deef59f000100010001?searchQuery=bio%20mio&amp;searchPosition=-1</t>
+  </si>
+  <si>
+    <t>https://lavka.yandex.ru/213/good/8f2d2d545cf24c94aa1655b878f0fbe8000200010001?searchQuery=bio%20mio&amp;searchPosition=-1</t>
+  </si>
+  <si>
+    <t>https://lavka.yandex.ru/213/good/cebd8ee8a29e49ba8e180ebeee64da4c000200010001?searchQuery=bio%20mio&amp;searchPosition=-1</t>
+  </si>
+  <si>
+    <t>https://lavka.yandex.ru/213/good/9cdd633b40744e848ff4bb7e25fc6a4e000200010000?searchQuery=%D0%B1%D1%80%D0%B5%D1%81%D1%82%20%D0%BB%D0%B8%D1%82%D0%BE%D0%B2%D1%81%D0%BA&amp;searchPosition=-1</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3358131/pelmeni-cezar-klassika-800-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3396165/picca-cezar-kvartet-zamorozhennaja-420-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3366066/picca-la-trattoria-mocarella-zamorozhennaja-335-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3372728/picca-morozko-la-trattoria-assorti-zamorozhennaja-335-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3396155/naggetsy-morozko-kurinye-zamorozhennye-300-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3267982/testo-morozko-sloenoe-drozhzhevoe-zamorozhennoe-500-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3396167/testo-morozko-sloenoe-drozhzhevoe-zamorozhennoe-400-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3396166/testo-morozko-sloenoe-bezdrozhzhevoe-zamorozhennoe-400-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3366055/bliny-cezar-s-derevenskim-tvorogom-zamorozhennye-450-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3351688/makaronnye-izdelija-makfa-spirali-400-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3371209/makaronnye-izdelija-makfa-perja-400-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3368035/krupa-grechnevaja-makfa-jadrica-800-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3351691/makaronnye-izdelija-makfa-vitki-400-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3439299/makaronnye-izdelija-livingood-lg-energy-pasta-fusilli-400-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3439304/makaronnye-izdelija-livingood-spaghetti-s-vodorosljami-400-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3439302/makaronnye-izdelija-livingood-fusilli-s-vodorosljami-400-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3439303/makaronnye-izdelija-livingood-penne-s-vodorosljami-400-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3286634/khlopja-makfa-5-zlakov-400-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3286633/khlopja-makfa-4-zlaka-400-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3284516/vlazhnye-salfetki-aura-family-wet-wipes-ochishhajushhie-s-antibakterialnym-effektom-120-shtuk</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3268513/vatnye-palochki-ja-samaja-zip-paket-300-shtuk</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3264399/vatnye-diski-aura-120-shtuk</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3284520/vatnye-diski-ja-samaja-100-shtuk</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3329126/tualetnaja-bumaga-vlazhnaja-aura-comfort-80-listov</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3264388/mylo-zhidkoe-dlja-ruk-aura-uvlazhnjajushhee-s-antibakterialnym-effektom-s-aloe-vera-300-ml</t>
+  </si>
+  <si>
+    <t>https://online.metro-cc.ru/category/gotovye-bljuda-polufabrikaty/zamorozhennye-gotovye-blyuda/klassika-cezar-800-g</t>
+  </si>
+  <si>
+    <t>https://online.metro-cc.ru/category/gotovye-bljuda-polufabrikaty/zamorozhennye-gotovye-blyuda/picca-la-trattoria-mocarella-335g</t>
+  </si>
+  <si>
+    <t>https://online.metro-cc.ru/category/gotovye-bljuda-polufabrikaty/zamorozhennye-gotovye-blyuda/picca-la-trattoria-assorti-335g</t>
+  </si>
+  <si>
+    <t>https://online.metro-cc.ru/category/molochnye-prodkuty-syry-i-yayca/syry/shvejcarskij-kiprino-50-125-g-narezka-bzmzh</t>
+  </si>
+  <si>
+    <t>https://online.metro-cc.ru/category/molochnye-prodkuty-syry-i-yayca/syry/altajskij-kiprino-50-125-g-narezka-bzmzh</t>
+  </si>
+  <si>
+    <t>https://online.metro-cc.ru/category/bakaleya/sousy-pripravy-specii/majonez-ryaba-provansal-67-400-g</t>
+  </si>
+  <si>
+    <t>https://online.metro-cc.ru/category/bakaleya/sousy-pripravy-specii/astoriya-syrnyj-42-233g</t>
+  </si>
+  <si>
+    <t>https://online.metro-cc.ru/category/bakaleya/sousy-pripravy-specii/astoriya-slivochno-chesnochnyj-233g</t>
+  </si>
+  <si>
+    <t>https://online.metro-cc.ru/category/molochnye-prodkuty-syry-i-yayca/slivochnoe-maslo-i-margarin/margarin-slivochnyj-nizhegorodskij-hozyayushka-200g</t>
+  </si>
+  <si>
+    <t>https://online.metro-cc.ru/category/bakaleya/aziatskaya-kuhnya/art_352562</t>
+  </si>
+  <si>
+    <t>https://online.metro-cc.ru/category/bakaleya/aziatskaya-kuhnya/vermishel-funchoza-sen-soy-200g</t>
+  </si>
+  <si>
+    <t>https://online.metro-cc.ru/category/bakaleya/makaronnye-izdeliya/spiralki-ekspress-makfa-400-g</t>
+  </si>
+  <si>
+    <t>https://online.metro-cc.ru/category/bakaleya/makaronnye-izdeliya/makfa-perya-lyubitelskie-450g</t>
+  </si>
+  <si>
+    <t>https://online.metro-cc.ru/category/bytovaya-himiya/sredstva-dlya-stirki/stiralnye-poroshki/15l-poroshok-belogo-bel</t>
+  </si>
+  <si>
+    <t>https://online.metro-cc.ru/category/bytovaya-himiya/sredstva-dlya-mytya-posudy/dlya-ruchnogo-mytya/biomio-bio-care-mandarin-ekologichnoe-ovoschej-fruktov-450ml</t>
+  </si>
+  <si>
+    <t>https://online.metro-cc.ru/category/bytovaya-himiya/sredstva-dlya-mytya-posudy/dlya-posudomoechnyh-mashin/biomio-bio-total-tabletki-s-maslom-evkalipta-100-sht</t>
+  </si>
+  <si>
+    <t>https://online.metro-cc.ru/category/detskie-tovary/detskaya-kosmetika/sredstva-dlya-kupaniya/ushastyj-nyan-krem-mylo-zhidkoe-dlya-detej-300ml</t>
+  </si>
+  <si>
+    <t>https://online.metro-cc.ru/category/molochnye-prodkuty-syry-i-yayca/slivochnoe-maslo-i-margarin/brest-litovskoe-825-180g-bzmzh</t>
+  </si>
+  <si>
+    <t>https://online.metro-cc.ru/category/molochnye-prodkuty-syry-i-yayca/syry/brest-litovskoe-klassicheskij-45-narezka-150g-bzmzh</t>
+  </si>
+  <si>
+    <t>https://online.metro-cc.ru/category/kosmetika/gigienicheskie-prinadlezhnosti/bumazhnye-vatnye-izdeliya/salfetki-aura-ultra-comfort-detskie-s-aloe-vitaminom-e-100sht</t>
+  </si>
+  <si>
+    <t>https://online.metro-cc.ru/category/tovary-dlya-doma-dachi-sada/hozyajstvennye-tovary/sredstva-dlya-uborki/vlazhnye-salfetki-aura-proexpert-antibakterialnye-120sht</t>
+  </si>
+  <si>
+    <t>https://online.metro-cc.ru/category/kosmetika/uhod-za-telom-i-licom/mylo/art_595704</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets/d/1IN-M_-KAUiS_tJWIjTLl1T1TDyb54L4E/edit#gid=827366537</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/zamorozhennye_produkty/pelmeni_vareniki_khinkali_manty/133776/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/zamorozhennye_produkty/pelmeni_vareniki_khinkali_manty/150708/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/zamorozhennye_produkty/khleb_vypechka_testo_torty_pirozhnye/133224/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/zamorozhennye_produkty/khleb_vypechka_testo_torty_pirozhnye/133223/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/zamorozhennye_produkty/gotovaya_eda_1/289321/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/bakaleya_2/krupy_bobovye/135205/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/bakaleya_2/krupy_bobovye/299186/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/bakaleya_2/kashi_khlopya_sukhie_zavtraki/307363/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/bakaleya_2/kashi_khlopya_sukhie_zavtraki/307373/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/gigiena_i_kosmetika/salfetki_i_nosovye_platki/308089/</t>
   </si>
 </sst>
 </file>
@@ -1588,10 +1765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF1A69E3-A9E5-424F-8F16-B76B324D2ACC}">
-  <dimension ref="D5:M100"/>
+  <dimension ref="D5:M115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J97" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K97" sqref="K97"/>
+    <sheetView tabSelected="1" topLeftCell="J104" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L106" sqref="L106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1617,7 +1794,7 @@
         <v>106</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H6" s="11" t="s">
         <v>107</v>
@@ -1626,13 +1803,13 @@
         <v>108</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="M6" s="13" t="s">
         <v>1</v>
@@ -1649,15 +1826,17 @@
         <v>111</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="L7" s="9"/>
+        <v>243</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>388</v>
+      </c>
       <c r="M7" s="5" t="s">
         <v>3</v>
       </c>
@@ -1670,14 +1849,19 @@
         <v>4</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="G8" s="9"/>
+        <v>327</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>330</v>
+      </c>
+      <c r="H8" t="s">
+        <v>365</v>
+      </c>
       <c r="J8" t="s">
-        <v>198</v>
+        <v>340</v>
       </c>
       <c r="K8" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="M8" s="6" t="s">
         <v>4</v>
@@ -1691,23 +1875,23 @@
         <v>5</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="9" t="s">
         <v>110</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>332</v>
-      </c>
-      <c r="J9" t="s">
-        <v>199</v>
+        <v>320</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>196</v>
       </c>
       <c r="K9" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="L9" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="M9" s="5" t="s">
         <v>5</v>
@@ -1721,19 +1905,21 @@
         <v>6</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G10" s="9"/>
       <c r="I10" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J10" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>256</v>
-      </c>
-      <c r="L10" s="9"/>
+        <v>246</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>389</v>
+      </c>
       <c r="M10" s="5" t="s">
         <v>6</v>
       </c>
@@ -1746,20 +1932,23 @@
         <v>8</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G11" s="9"/>
       <c r="H11" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J11" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="K11" t="s">
-        <v>257</v>
+        <v>247</v>
+      </c>
+      <c r="L11" t="s">
+        <v>390</v>
       </c>
       <c r="M11" s="5" t="s">
         <v>8</v>
@@ -1773,18 +1962,20 @@
         <v>9</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J12" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>258</v>
-      </c>
-      <c r="L12" s="9"/>
+        <v>248</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>391</v>
+      </c>
       <c r="M12" s="5" t="s">
         <v>9</v>
       </c>
@@ -1797,11 +1988,11 @@
         <v>10</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G13" s="9"/>
       <c r="J13" t="s">
-        <v>203</v>
+        <v>345</v>
       </c>
       <c r="M13" s="5" t="s">
         <v>10</v>
@@ -1815,17 +2006,22 @@
         <v>12</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="G14" s="9"/>
+        <v>118</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="H14" t="s">
+        <v>366</v>
+      </c>
       <c r="I14" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>204</v>
+        <v>342</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="L14" s="9"/>
       <c r="M14" s="5" t="s">
@@ -1839,11 +2035,20 @@
       <c r="E15" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="F15" t="s">
+        <v>328</v>
+      </c>
+      <c r="G15" t="s">
+        <v>332</v>
+      </c>
+      <c r="H15" t="s">
+        <v>367</v>
+      </c>
       <c r="I15" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J15" t="s">
-        <v>205</v>
+        <v>343</v>
       </c>
       <c r="M15" s="5" t="s">
         <v>13</v>
@@ -1856,8 +2061,17 @@
       <c r="E16" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="G16" t="s">
+        <v>333</v>
+      </c>
       <c r="I16" t="s">
-        <v>168</v>
+        <v>166</v>
+      </c>
+      <c r="J16" t="s">
+        <v>341</v>
+      </c>
+      <c r="L16" t="s">
+        <v>392</v>
       </c>
       <c r="M16" s="5" t="s">
         <v>15</v>
@@ -1870,8 +2084,11 @@
       <c r="E17" s="5" t="s">
         <v>16</v>
       </c>
+      <c r="H17" t="s">
+        <v>368</v>
+      </c>
       <c r="J17" s="9" t="s">
-        <v>206</v>
+        <v>346</v>
       </c>
       <c r="K17" s="9"/>
       <c r="L17" s="9"/>
@@ -1890,12 +2107,13 @@
         <v>109</v>
       </c>
       <c r="G18" s="9"/>
+      <c r="H18" t="s">
+        <v>369</v>
+      </c>
       <c r="J18" t="s">
-        <v>207</v>
-      </c>
-      <c r="L18" t="s">
-        <v>299</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="L18" s="9"/>
       <c r="M18" s="5" t="s">
         <v>17</v>
       </c>
@@ -1908,7 +2126,7 @@
         <v>18</v>
       </c>
       <c r="J19" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="M19" s="5" t="s">
         <v>18</v>
@@ -1922,11 +2140,11 @@
         <v>19</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G20" s="9"/>
       <c r="J20" t="s">
-        <v>209</v>
+        <v>347</v>
       </c>
       <c r="M20" s="5" t="s">
         <v>19</v>
@@ -1939,8 +2157,11 @@
       <c r="E21" s="5" t="s">
         <v>20</v>
       </c>
+      <c r="J21" t="s">
+        <v>344</v>
+      </c>
       <c r="K21" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="M21" s="5" t="s">
         <v>20</v>
@@ -1954,64 +2175,57 @@
         <v>22</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G22" s="9"/>
       <c r="J22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="K22" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="M22" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D23" s="2"/>
-      <c r="E23" s="3"/>
-      <c r="M23" s="3"/>
-    </row>
-    <row r="24" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D24" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="I24" t="s">
-        <v>169</v>
-      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="J23" t="s">
+        <v>387</v>
+      </c>
+      <c r="M23" s="5"/>
+    </row>
+    <row r="24" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D24" s="2"/>
+      <c r="E24" s="3"/>
       <c r="J24" t="s">
-        <v>211</v>
-      </c>
-      <c r="K24" t="s">
-        <v>335</v>
-      </c>
-      <c r="M24" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>348</v>
+      </c>
+      <c r="M24" s="3"/>
+    </row>
+    <row r="25" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D25" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="I25" t="s">
+        <v>167</v>
       </c>
       <c r="J25" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="K25" t="s">
-        <v>336</v>
-      </c>
-      <c r="L25" t="s">
-        <v>300</v>
+        <v>323</v>
       </c>
       <c r="M25" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2019,114 +2233,110 @@
         <v>23</v>
       </c>
       <c r="E26" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J26" t="s">
+        <v>204</v>
+      </c>
+      <c r="K26" t="s">
+        <v>324</v>
+      </c>
+      <c r="L26" t="s">
+        <v>289</v>
+      </c>
+      <c r="M26" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D27" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F26" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="G26" s="9"/>
-      <c r="J26" t="s">
-        <v>213</v>
-      </c>
-      <c r="M26" s="5" t="s">
+      <c r="F27" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="G27" s="9"/>
+      <c r="J27" t="s">
+        <v>205</v>
+      </c>
+      <c r="M27" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D27" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="M27" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D28" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M28" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D29" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E29" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M29" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D30" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="M29" s="5" t="s">
+      <c r="M30" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D30" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="M30" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D31" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E31" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M31" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D32" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E32" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F31" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="G31" s="9"/>
-      <c r="L31" t="s">
-        <v>301</v>
-      </c>
-      <c r="M31" s="5" t="s">
+      <c r="F32" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="G32" s="9"/>
+      <c r="L32" t="s">
+        <v>290</v>
+      </c>
+      <c r="M32" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="7" t="s">
+    <row r="33" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D33" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="E33" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="M32" s="8" t="s">
+      <c r="M33" s="8" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="33" spans="4:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D33" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F33" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="G33" s="9"/>
-      <c r="J33" t="s">
-        <v>325</v>
-      </c>
-      <c r="K33" t="s">
-        <v>262</v>
-      </c>
-      <c r="L33" t="s">
-        <v>302</v>
-      </c>
-      <c r="M33" s="5" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="34" spans="4:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2134,305 +2344,313 @@
         <v>34</v>
       </c>
       <c r="E34" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="G34" s="9"/>
+      <c r="J34" t="s">
+        <v>313</v>
+      </c>
+      <c r="K34" t="s">
+        <v>252</v>
+      </c>
+      <c r="L34" t="s">
+        <v>291</v>
+      </c>
+      <c r="M34" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="4:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D35" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E35" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="J34" t="s">
-        <v>326</v>
-      </c>
-      <c r="L34" t="s">
-        <v>334</v>
-      </c>
-      <c r="M34" s="5" t="s">
+      <c r="J35" t="s">
+        <v>314</v>
+      </c>
+      <c r="L35" t="s">
+        <v>322</v>
+      </c>
+      <c r="M35" s="5" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="35" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D35" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="J35" t="s">
-        <v>327</v>
-      </c>
-      <c r="K35" t="s">
-        <v>263</v>
-      </c>
-      <c r="M35" s="5" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="36" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D36" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J36" t="s">
+        <v>315</v>
+      </c>
+      <c r="K36" t="s">
+        <v>253</v>
+      </c>
+      <c r="M36" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D37" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E36" s="5" t="s">
+      <c r="E37" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="I36" t="s">
-        <v>170</v>
-      </c>
-      <c r="J36" t="s">
-        <v>328</v>
-      </c>
-      <c r="M36" s="5" t="s">
+      <c r="I37" t="s">
+        <v>168</v>
+      </c>
+      <c r="J37" t="s">
+        <v>316</v>
+      </c>
+      <c r="M37" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D37" s="2"/>
-      <c r="E37" s="3"/>
-      <c r="M37" s="3"/>
-    </row>
-    <row r="38" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D38" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F38" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="G38" s="9"/>
-      <c r="J38" t="s">
-        <v>214</v>
-      </c>
-      <c r="K38" t="s">
-        <v>264</v>
-      </c>
-      <c r="M38" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="39" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="2"/>
+      <c r="E38" s="3"/>
+      <c r="M38" s="3"/>
+    </row>
+    <row r="39" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D39" s="4" t="s">
         <v>41</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F39" s="9" t="s">
         <v>125</v>
       </c>
       <c r="G39" s="9"/>
       <c r="J39" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="K39" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="M39" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="40" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D40" s="4" t="s">
         <v>41</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="G40" s="9" t="s">
-        <v>150</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="G40" s="9"/>
       <c r="J40" t="s">
-        <v>218</v>
-      </c>
-      <c r="L40" t="s">
-        <v>303</v>
+        <v>207</v>
+      </c>
+      <c r="K40" t="s">
+        <v>255</v>
       </c>
       <c r="M40" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="41" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D41" s="4" t="s">
         <v>41</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F41" t="s">
-        <v>321</v>
+        <v>44</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>149</v>
       </c>
       <c r="J41" t="s">
-        <v>219</v>
-      </c>
-      <c r="K41" t="s">
-        <v>266</v>
+        <v>210</v>
+      </c>
+      <c r="L41" t="s">
+        <v>292</v>
       </c>
       <c r="M41" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="42" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D42" s="4" t="s">
         <v>41</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="J42" s="9" t="s">
-        <v>216</v>
-      </c>
-      <c r="K42" s="9"/>
-      <c r="L42" s="9"/>
+        <v>45</v>
+      </c>
+      <c r="F42" t="s">
+        <v>309</v>
+      </c>
+      <c r="J42" t="s">
+        <v>211</v>
+      </c>
+      <c r="K42" t="s">
+        <v>256</v>
+      </c>
       <c r="M42" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="43" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D43" s="4" t="s">
         <v>41</v>
       </c>
       <c r="E43" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J43" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="K43" s="9"/>
+      <c r="L43" s="9"/>
+      <c r="M43" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D44" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E44" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F43" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="G43" s="9"/>
-      <c r="J43" t="s">
-        <v>217</v>
-      </c>
-      <c r="M43" s="5" t="s">
+      <c r="F44" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="G44" s="9"/>
+      <c r="J44" t="s">
+        <v>209</v>
+      </c>
+      <c r="M44" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D44" s="2"/>
-      <c r="E44" s="3"/>
-      <c r="M44" s="3"/>
-    </row>
-    <row r="45" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D45" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F45" t="s">
-        <v>322</v>
-      </c>
-      <c r="K45" t="s">
-        <v>268</v>
-      </c>
-      <c r="L45" t="s">
-        <v>304</v>
-      </c>
-      <c r="M45" s="5" t="s">
-        <v>49</v>
-      </c>
+    <row r="45" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D45" s="2"/>
+      <c r="E45" s="3"/>
+      <c r="M45" s="3"/>
     </row>
     <row r="46" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D46" s="4" t="s">
         <v>48</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F46" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="G46" s="9"/>
-      <c r="J46" t="s">
-        <v>220</v>
-      </c>
-      <c r="K46" s="9" t="s">
-        <v>267</v>
-      </c>
-      <c r="L46" s="9" t="s">
-        <v>305</v>
+        <v>49</v>
+      </c>
+      <c r="F46" t="s">
+        <v>310</v>
+      </c>
+      <c r="K46" t="s">
+        <v>258</v>
+      </c>
+      <c r="L46" t="s">
+        <v>293</v>
       </c>
       <c r="M46" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="47" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D47" s="4" t="s">
         <v>48</v>
       </c>
       <c r="E47" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="G47" s="9"/>
+      <c r="J47" t="s">
+        <v>212</v>
+      </c>
+      <c r="K47" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="L47" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="M47" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D48" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E48" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="H47" s="9"/>
-      <c r="M47" s="5" t="s">
+      <c r="H48" s="9"/>
+      <c r="M48" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="48" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D48" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F48" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="G48" s="9"/>
-      <c r="H48" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="I48" t="s">
-        <v>171</v>
-      </c>
-      <c r="J48" t="s">
-        <v>221</v>
-      </c>
-      <c r="K48" t="s">
-        <v>269</v>
-      </c>
-      <c r="L48" t="s">
-        <v>306</v>
-      </c>
-      <c r="M48" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="49" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D49" s="4" t="s">
         <v>52</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G49" s="9"/>
+      <c r="H49" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="I49" t="s">
+        <v>169</v>
+      </c>
       <c r="J49" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="K49" t="s">
-        <v>270</v>
+        <v>259</v>
+      </c>
+      <c r="L49" t="s">
+        <v>295</v>
       </c>
       <c r="M49" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="50" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D50" s="4" t="s">
         <v>52</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="I50" t="s">
-        <v>171</v>
-      </c>
-      <c r="J50" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="K50" s="9"/>
-      <c r="L50" s="9"/>
+        <v>54</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="G50" s="9"/>
+      <c r="H50" t="s">
+        <v>370</v>
+      </c>
+      <c r="J50" t="s">
+        <v>214</v>
+      </c>
+      <c r="K50" t="s">
+        <v>260</v>
+      </c>
       <c r="M50" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="51" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2440,27 +2658,38 @@
         <v>52</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="J51" t="s">
-        <v>224</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="H51" t="s">
+        <v>371</v>
+      </c>
+      <c r="I51" t="s">
+        <v>169</v>
+      </c>
+      <c r="J51" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="K51" s="9"/>
+      <c r="L51" s="9"/>
       <c r="M51" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="52" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D52" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="K52" t="s">
-        <v>271</v>
+        <v>56</v>
+      </c>
+      <c r="H52" t="s">
+        <v>372</v>
+      </c>
+      <c r="J52" t="s">
+        <v>216</v>
       </c>
       <c r="M52" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="53" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2468,166 +2697,171 @@
         <v>57</v>
       </c>
       <c r="E53" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H53" t="s">
+        <v>373</v>
+      </c>
+      <c r="K53" t="s">
+        <v>261</v>
+      </c>
+      <c r="M53" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D54" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E54" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F53" t="s">
-        <v>323</v>
-      </c>
-      <c r="L53" t="s">
-        <v>307</v>
-      </c>
-      <c r="M53" s="5" t="s">
+      <c r="F54" t="s">
+        <v>311</v>
+      </c>
+      <c r="L54" t="s">
+        <v>296</v>
+      </c>
+      <c r="M54" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="54" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D54" s="4" t="s">
+    <row r="55" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D55" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E54" s="5" t="s">
+      <c r="E55" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="M54" s="5" t="s">
+      <c r="M55" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="55" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D55" s="2"/>
-      <c r="E55" s="3"/>
-      <c r="M55" s="3"/>
-    </row>
-    <row r="56" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D56" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E56" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F56" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="G56" s="9"/>
-      <c r="I56" t="s">
-        <v>173</v>
-      </c>
-      <c r="J56" t="s">
-        <v>225</v>
-      </c>
-      <c r="K56" t="s">
-        <v>272</v>
-      </c>
-      <c r="L56" t="s">
-        <v>308</v>
-      </c>
-      <c r="M56" s="5" t="s">
-        <v>63</v>
-      </c>
+    <row r="56" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D56" s="2"/>
+      <c r="E56" s="3"/>
+      <c r="M56" s="3"/>
     </row>
     <row r="57" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="4" t="s">
         <v>62</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+      <c r="F57" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="G57" s="9"/>
+      <c r="I57" t="s">
+        <v>171</v>
       </c>
       <c r="J57" t="s">
-        <v>226</v>
+        <v>217</v>
+      </c>
+      <c r="K57" t="s">
+        <v>262</v>
+      </c>
+      <c r="L57" t="s">
+        <v>297</v>
       </c>
       <c r="M57" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="58" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="58" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="4" t="s">
         <v>62</v>
       </c>
       <c r="E58" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="J58" t="s">
+        <v>218</v>
+      </c>
+      <c r="M58" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="59" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D59" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E59" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="F58" t="s">
-        <v>287</v>
-      </c>
-      <c r="H58" t="s">
-        <v>160</v>
-      </c>
-      <c r="I58" t="s">
+      <c r="F59" t="s">
+        <v>277</v>
+      </c>
+      <c r="H59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I59" t="s">
+        <v>170</v>
+      </c>
+      <c r="J59" t="s">
+        <v>219</v>
+      </c>
+      <c r="K59" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="L59" s="9"/>
+      <c r="M59" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="60" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D60" s="2"/>
+      <c r="E60" s="3"/>
+      <c r="I60" t="s">
         <v>172</v>
       </c>
-      <c r="J58" t="s">
-        <v>227</v>
-      </c>
-      <c r="K58" s="9" t="s">
-        <v>273</v>
-      </c>
-      <c r="L58" s="9"/>
-      <c r="M58" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="59" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D59" s="2"/>
-      <c r="E59" s="3"/>
-      <c r="I59" t="s">
-        <v>174</v>
-      </c>
-      <c r="M59" s="3"/>
-    </row>
-    <row r="60" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D60" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="F60" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="G60" s="9"/>
-      <c r="I60" t="s">
-        <v>175</v>
-      </c>
-      <c r="J60" s="9" t="s">
-        <v>228</v>
-      </c>
-      <c r="K60" t="s">
-        <v>274</v>
-      </c>
-      <c r="M60" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="61" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M60" s="3"/>
+    </row>
+    <row r="61" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D61" s="4" t="s">
         <v>66</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="J61" t="s">
-        <v>229</v>
+        <v>67</v>
+      </c>
+      <c r="F61" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="G61" s="9" t="s">
+        <v>334</v>
+      </c>
+      <c r="H61" t="s">
+        <v>374</v>
+      </c>
+      <c r="I61" t="s">
+        <v>173</v>
+      </c>
+      <c r="J61" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="K61" t="s">
+        <v>264</v>
       </c>
       <c r="M61" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="62" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="62" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D62" s="4" t="s">
         <v>66</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="F62" t="s">
-        <v>289</v>
-      </c>
-      <c r="I62" t="s">
-        <v>176</v>
+        <v>68</v>
+      </c>
+      <c r="H62" t="s">
+        <v>375</v>
       </c>
       <c r="J62" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="M62" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="63" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2635,716 +2869,925 @@
         <v>66</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F63" s="9" t="s">
-        <v>288</v>
+        <v>69</v>
+      </c>
+      <c r="F63" t="s">
+        <v>279</v>
       </c>
       <c r="I63" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="J63" t="s">
-        <v>231</v>
-      </c>
-      <c r="K63" t="s">
-        <v>275</v>
-      </c>
-      <c r="L63" s="9" t="s">
-        <v>309</v>
+        <v>222</v>
       </c>
       <c r="M63" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="64" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="64" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D64" s="4" t="s">
         <v>66</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="F64" t="s">
-        <v>290</v>
-      </c>
-      <c r="G64" t="s">
-        <v>151</v>
+        <v>70</v>
+      </c>
+      <c r="F64" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="H64" t="s">
+        <v>376</v>
       </c>
       <c r="I64" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="J64" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="K64" t="s">
-        <v>276</v>
-      </c>
-      <c r="L64" t="s">
-        <v>310</v>
+        <v>265</v>
+      </c>
+      <c r="L64" s="9" t="s">
+        <v>298</v>
       </c>
       <c r="M64" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="65" spans="4:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="65" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D65" s="4" t="s">
         <v>66</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
+      </c>
+      <c r="F65" t="s">
+        <v>280</v>
       </c>
       <c r="G65" t="s">
-        <v>152</v>
+        <v>150</v>
+      </c>
+      <c r="H65" t="s">
+        <v>377</v>
       </c>
       <c r="I65" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="J65" t="s">
-        <v>233</v>
+        <v>224</v>
+      </c>
+      <c r="K65" t="s">
+        <v>266</v>
+      </c>
+      <c r="L65" t="s">
+        <v>299</v>
       </c>
       <c r="M65" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="66" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="66" spans="4:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D66" s="4" t="s">
         <v>66</v>
       </c>
       <c r="E66" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G66" t="s">
+        <v>151</v>
+      </c>
+      <c r="H66" t="s">
+        <v>159</v>
+      </c>
+      <c r="I66" t="s">
+        <v>177</v>
+      </c>
+      <c r="J66" t="s">
+        <v>225</v>
+      </c>
+      <c r="M66" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="67" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D67" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E67" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F66" t="s">
-        <v>291</v>
-      </c>
-      <c r="G66" t="s">
-        <v>153</v>
-      </c>
-      <c r="I66" t="s">
-        <v>180</v>
-      </c>
-      <c r="M66" s="5" t="s">
+      <c r="F67" t="s">
+        <v>281</v>
+      </c>
+      <c r="G67" t="s">
+        <v>152</v>
+      </c>
+      <c r="I67" t="s">
+        <v>178</v>
+      </c>
+      <c r="M67" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D67" s="2"/>
-      <c r="E67" s="3"/>
-      <c r="I67" t="s">
-        <v>181</v>
-      </c>
-      <c r="M67" s="3"/>
-    </row>
     <row r="68" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D68" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E68" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="G68" t="s">
-        <v>154</v>
-      </c>
-      <c r="J68" t="s">
-        <v>234</v>
-      </c>
-      <c r="K68" t="s">
-        <v>277</v>
-      </c>
-      <c r="L68" t="s">
-        <v>311</v>
-      </c>
-      <c r="M68" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="69" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D68" s="2"/>
+      <c r="E68" s="3"/>
+      <c r="I68" t="s">
+        <v>179</v>
+      </c>
+      <c r="M68" s="3"/>
+    </row>
+    <row r="69" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D69" s="4" t="s">
         <v>74</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="F69" t="s">
-        <v>135</v>
-      </c>
-      <c r="G69" t="s">
-        <v>155</v>
+        <v>75</v>
       </c>
       <c r="J69" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="K69" s="9" t="s">
-        <v>278</v>
-      </c>
-      <c r="L69" s="9" t="s">
-        <v>313</v>
+        <v>349</v>
+      </c>
+      <c r="K69" t="s">
+        <v>267</v>
       </c>
       <c r="M69" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="70" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="70" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D70" s="4" t="s">
         <v>74</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="I70" s="9" t="s">
-        <v>182</v>
+        <v>76</v>
+      </c>
+      <c r="F70" t="s">
+        <v>134</v>
+      </c>
+      <c r="G70" t="s">
+        <v>153</v>
+      </c>
+      <c r="J70" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="K70" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="L70" s="9" t="s">
+        <v>301</v>
       </c>
       <c r="M70" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="71" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="71" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D71" s="4" t="s">
         <v>74</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="F71" t="s">
-        <v>136</v>
-      </c>
-      <c r="H71" t="s">
-        <v>161</v>
-      </c>
-      <c r="I71" t="s">
-        <v>183</v>
+        <v>77</v>
+      </c>
+      <c r="I71" s="9" t="s">
+        <v>180</v>
       </c>
       <c r="J71" t="s">
-        <v>236</v>
-      </c>
-      <c r="K71" t="s">
-        <v>337</v>
+        <v>226</v>
       </c>
       <c r="M71" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="72" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="72" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D72" s="4" t="s">
         <v>74</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F72" t="s">
-        <v>137</v>
+        <v>135</v>
+      </c>
+      <c r="H72" t="s">
+        <v>159</v>
       </c>
       <c r="I72" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="J72" t="s">
-        <v>329</v>
-      </c>
-      <c r="K72" s="9" t="s">
-        <v>279</v>
-      </c>
-      <c r="L72" s="9" t="s">
-        <v>312</v>
+        <v>350</v>
+      </c>
+      <c r="K72" t="s">
+        <v>325</v>
+      </c>
+      <c r="L72" t="s">
+        <v>396</v>
       </c>
       <c r="M72" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="73" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="73" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D73" s="4" t="s">
         <v>74</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+      <c r="F73" t="s">
+        <v>136</v>
       </c>
       <c r="I73" t="s">
-        <v>185</v>
-      </c>
-      <c r="J73" s="9" t="s">
-        <v>237</v>
-      </c>
-      <c r="K73" s="9"/>
-      <c r="L73" s="9"/>
+        <v>182</v>
+      </c>
+      <c r="J73" t="s">
+        <v>317</v>
+      </c>
+      <c r="K73" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="L73" s="9" t="s">
+        <v>300</v>
+      </c>
       <c r="M73" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="74" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="74" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D74" s="4" t="s">
         <v>74</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="H74" t="s">
-        <v>162</v>
-      </c>
-      <c r="J74" t="s">
-        <v>238</v>
+        <v>80</v>
+      </c>
+      <c r="G74" t="s">
+        <v>335</v>
+      </c>
+      <c r="I74" t="s">
+        <v>183</v>
+      </c>
+      <c r="J74" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="K74" s="9"/>
+      <c r="L74" s="9" t="s">
+        <v>395</v>
       </c>
       <c r="M74" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="75" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D75" s="2"/>
-      <c r="E75" s="3"/>
-      <c r="I75" t="s">
-        <v>186</v>
-      </c>
-      <c r="M75" s="3"/>
-    </row>
-    <row r="76" spans="4:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D76" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E76" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="F76" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="G76" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="J76" t="s">
-        <v>239</v>
-      </c>
-      <c r="L76" t="s">
-        <v>314</v>
-      </c>
-      <c r="M76" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="77" spans="4:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D77" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E77" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F77" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="G77" s="9"/>
-      <c r="J77" t="s">
-        <v>240</v>
-      </c>
-      <c r="L77" t="s">
-        <v>315</v>
-      </c>
-      <c r="M77" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="78" spans="4:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D78" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E78" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="F78" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="G78" s="9"/>
-      <c r="H78" t="s">
-        <v>163</v>
-      </c>
-      <c r="I78" s="9" t="s">
-        <v>294</v>
-      </c>
-      <c r="J78" t="s">
-        <v>330</v>
-      </c>
-      <c r="M78" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="79" spans="4:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D79" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E79" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F79" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="G79" s="9"/>
-      <c r="H79" t="s">
-        <v>164</v>
-      </c>
-      <c r="J79" t="s">
-        <v>241</v>
-      </c>
-      <c r="L79" t="s">
-        <v>316</v>
-      </c>
-      <c r="M79" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="80" spans="4:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D80" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E80" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F80" t="s">
-        <v>142</v>
-      </c>
-      <c r="I80" t="s">
-        <v>187</v>
-      </c>
-      <c r="J80" t="s">
-        <v>242</v>
-      </c>
-      <c r="K80" t="s">
-        <v>280</v>
-      </c>
-      <c r="M80" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="81" spans="4:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D81" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E81" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F81" t="s">
-        <v>143</v>
-      </c>
-      <c r="I81" t="s">
-        <v>188</v>
-      </c>
-      <c r="J81" t="s">
-        <v>243</v>
-      </c>
-      <c r="M81" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="82" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D82" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E82" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="F82" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="G82" s="9"/>
-      <c r="I82" t="s">
-        <v>189</v>
-      </c>
-      <c r="J82" t="s">
-        <v>244</v>
-      </c>
-      <c r="M82" s="5" t="s">
-        <v>90</v>
-      </c>
+      <c r="D75" s="4"/>
+      <c r="E75" s="5"/>
+      <c r="J75" s="9" t="s">
+        <v>352</v>
+      </c>
+      <c r="K75" s="9"/>
+      <c r="L75" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="M75" s="5"/>
+    </row>
+    <row r="76" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D76" s="4"/>
+      <c r="E76" s="5"/>
+      <c r="J76" s="9" t="s">
+        <v>353</v>
+      </c>
+      <c r="K76" s="9"/>
+      <c r="L76" s="9" t="s">
+        <v>394</v>
+      </c>
+      <c r="M76" s="5"/>
+    </row>
+    <row r="77" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D77" s="4"/>
+      <c r="E77" s="5"/>
+      <c r="J77" s="9" t="s">
+        <v>354</v>
+      </c>
+      <c r="K77" s="9"/>
+      <c r="L77" s="9"/>
+      <c r="M77" s="5"/>
+    </row>
+    <row r="78" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D78" s="4"/>
+      <c r="E78" s="5"/>
+      <c r="J78" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="K78" s="9"/>
+      <c r="L78" s="9"/>
+      <c r="M78" s="5"/>
+    </row>
+    <row r="79" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D79" s="4"/>
+      <c r="E79" s="5"/>
+      <c r="J79" s="9" t="s">
+        <v>356</v>
+      </c>
+      <c r="K79" s="9"/>
+      <c r="L79" s="9"/>
+      <c r="M79" s="5"/>
+    </row>
+    <row r="80" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D80" s="4"/>
+      <c r="E80" s="5"/>
+      <c r="J80" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="K80" s="9"/>
+      <c r="L80" s="9"/>
+      <c r="M80" s="5"/>
+    </row>
+    <row r="81" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D81" s="4"/>
+      <c r="E81" s="5"/>
+      <c r="J81" s="9" t="s">
+        <v>353</v>
+      </c>
+      <c r="K81" s="9"/>
+      <c r="L81" s="9"/>
+      <c r="M81" s="5"/>
+    </row>
+    <row r="82" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D82" s="4"/>
+      <c r="E82" s="5"/>
+      <c r="J82" s="9" t="s">
+        <v>358</v>
+      </c>
+      <c r="K82" s="9"/>
+      <c r="L82" s="9"/>
+      <c r="M82" s="5"/>
     </row>
     <row r="83" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D83" s="2"/>
-      <c r="E83" s="3"/>
-      <c r="I83" t="s">
-        <v>296</v>
-      </c>
-      <c r="M83" s="3"/>
+      <c r="D83" s="4"/>
+      <c r="E83" s="5"/>
+      <c r="J83" s="9" t="s">
+        <v>351</v>
+      </c>
+      <c r="K83" s="9"/>
+      <c r="L83" s="9"/>
+      <c r="M83" s="5"/>
     </row>
     <row r="84" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D84" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H84" t="s">
+        <v>160</v>
+      </c>
+      <c r="J84" t="s">
+        <v>228</v>
+      </c>
+      <c r="M84" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="85" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D85" s="2"/>
+      <c r="E85" s="3"/>
+      <c r="I85" t="s">
+        <v>184</v>
+      </c>
+      <c r="M85" s="3"/>
+    </row>
+    <row r="86" spans="4:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D86" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F86" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="G86" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="J86" t="s">
+        <v>229</v>
+      </c>
+      <c r="L86" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="M86" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="87" spans="4:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D87" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E87" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F87" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="G87" s="9"/>
+      <c r="J87" t="s">
+        <v>230</v>
+      </c>
+      <c r="L87" t="s">
+        <v>303</v>
+      </c>
+      <c r="M87" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="88" spans="4:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D88" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F88" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="G88" s="9"/>
+      <c r="H88" t="s">
+        <v>161</v>
+      </c>
+      <c r="I88" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="J88" t="s">
+        <v>318</v>
+      </c>
+      <c r="M88" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="89" spans="4:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D89" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F89" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="G89" s="9" t="s">
+        <v>338</v>
+      </c>
+      <c r="H89" t="s">
+        <v>162</v>
+      </c>
+      <c r="J89" t="s">
+        <v>231</v>
+      </c>
+      <c r="L89" t="s">
+        <v>304</v>
+      </c>
+      <c r="M89" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="90" spans="4:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D90" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E90" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F90" t="s">
+        <v>141</v>
+      </c>
+      <c r="G90" t="s">
+        <v>337</v>
+      </c>
+      <c r="I90" t="s">
+        <v>185</v>
+      </c>
+      <c r="J90" t="s">
+        <v>232</v>
+      </c>
+      <c r="K90" t="s">
+        <v>270</v>
+      </c>
+      <c r="M90" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="91" spans="4:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D91" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F91" t="s">
+        <v>142</v>
+      </c>
+      <c r="G91" t="s">
+        <v>336</v>
+      </c>
+      <c r="I91" t="s">
+        <v>186</v>
+      </c>
+      <c r="J91" t="s">
+        <v>233</v>
+      </c>
+      <c r="M91" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="92" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D92" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E92" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F92" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="G92" s="9"/>
+      <c r="I92" t="s">
+        <v>187</v>
+      </c>
+      <c r="J92" t="s">
+        <v>234</v>
+      </c>
+      <c r="M92" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="93" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D93" s="2"/>
+      <c r="E93" s="3"/>
+      <c r="H93" t="s">
+        <v>379</v>
+      </c>
+      <c r="I93" t="s">
+        <v>286</v>
+      </c>
+      <c r="M93" s="3"/>
+    </row>
+    <row r="94" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D94" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E84" s="5" t="s">
+      <c r="E94" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="F84" t="s">
-        <v>145</v>
-      </c>
-      <c r="G84" t="s">
-        <v>157</v>
-      </c>
-      <c r="I84" t="s">
-        <v>190</v>
-      </c>
-      <c r="J84" t="s">
-        <v>245</v>
-      </c>
-      <c r="K84" t="s">
-        <v>295</v>
-      </c>
-      <c r="M84" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="85" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D85" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E85" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="M85" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="86" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D86" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E86" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="I86" t="s">
-        <v>191</v>
-      </c>
-      <c r="J86" t="s">
-        <v>246</v>
-      </c>
-      <c r="K86" t="s">
-        <v>281</v>
-      </c>
-      <c r="M86" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="87" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D87" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E87" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="F87" t="s">
-        <v>324</v>
-      </c>
-      <c r="I87" t="s">
-        <v>192</v>
-      </c>
-      <c r="J87" t="s">
-        <v>247</v>
-      </c>
-      <c r="K87" t="s">
-        <v>282</v>
-      </c>
-      <c r="L87" t="s">
-        <v>317</v>
-      </c>
-      <c r="M87" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="88" spans="4:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D88" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E88" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="M88" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="89" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D89" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E89" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="I89" t="s">
-        <v>193</v>
-      </c>
-      <c r="J89" t="s">
-        <v>248</v>
-      </c>
-      <c r="M89" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="90" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D90" s="2"/>
-      <c r="E90" s="3"/>
-      <c r="I90" t="s">
-        <v>333</v>
-      </c>
-      <c r="M90" s="3"/>
-    </row>
-    <row r="91" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D91" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="E91" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="M91" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="92" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D92" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="E92" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="F92" t="s">
-        <v>293</v>
-      </c>
-      <c r="J92" t="s">
-        <v>249</v>
-      </c>
-      <c r="K92" t="s">
-        <v>283</v>
-      </c>
-      <c r="L92" t="s">
-        <v>320</v>
-      </c>
-      <c r="M92" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="93" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D93" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="E93" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="F93" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="G93" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="J93" t="s">
-        <v>250</v>
-      </c>
-      <c r="K93" t="s">
-        <v>284</v>
-      </c>
-      <c r="L93" t="s">
-        <v>318</v>
-      </c>
-      <c r="M93" s="5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="94" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D94" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="E94" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="I94" s="9" t="s">
-        <v>194</v>
+      <c r="F94" t="s">
+        <v>144</v>
+      </c>
+      <c r="G94" t="s">
+        <v>155</v>
+      </c>
+      <c r="H94" t="s">
+        <v>378</v>
+      </c>
+      <c r="I94" t="s">
+        <v>188</v>
       </c>
       <c r="J94" t="s">
-        <v>251</v>
+        <v>235</v>
       </c>
       <c r="K94" t="s">
         <v>285</v>
       </c>
       <c r="M94" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="95" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D95" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E95" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="H95" t="s">
+        <v>380</v>
+      </c>
+      <c r="M95" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="96" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D96" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E96" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="I96" t="s">
+        <v>189</v>
+      </c>
+      <c r="J96" t="s">
+        <v>236</v>
+      </c>
+      <c r="K96" t="s">
+        <v>271</v>
+      </c>
+      <c r="M96" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="97" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D97" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E97" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F97" t="s">
+        <v>312</v>
+      </c>
+      <c r="H97" t="s">
+        <v>381</v>
+      </c>
+      <c r="I97" t="s">
+        <v>190</v>
+      </c>
+      <c r="J97" t="s">
+        <v>237</v>
+      </c>
+      <c r="K97" t="s">
+        <v>272</v>
+      </c>
+      <c r="L97" t="s">
+        <v>305</v>
+      </c>
+      <c r="M97" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="98" spans="4:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D98" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="H98" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="M98" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D99" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E99" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="H99" t="s">
+        <v>383</v>
+      </c>
+      <c r="I99" t="s">
+        <v>191</v>
+      </c>
+      <c r="J99" t="s">
+        <v>238</v>
+      </c>
+      <c r="M99" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="100" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D100" s="2"/>
+      <c r="E100" s="3"/>
+      <c r="I100" t="s">
+        <v>321</v>
+      </c>
+      <c r="M100" s="3"/>
+    </row>
+    <row r="101" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D101" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E101" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="M101" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="102" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D102" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E102" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F102" t="s">
+        <v>283</v>
+      </c>
+      <c r="G102" t="s">
+        <v>339</v>
+      </c>
+      <c r="H102" t="s">
+        <v>384</v>
+      </c>
+      <c r="J102" t="s">
+        <v>239</v>
+      </c>
+      <c r="K102" t="s">
+        <v>273</v>
+      </c>
+      <c r="L102" t="s">
+        <v>308</v>
+      </c>
+      <c r="M102" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="103" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D103" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E103" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F103" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="G103" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="J103" t="s">
+        <v>240</v>
+      </c>
+      <c r="K103" t="s">
+        <v>274</v>
+      </c>
+      <c r="L103" t="s">
+        <v>306</v>
+      </c>
+      <c r="M103" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="104" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D104" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E104" s="5" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="95" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D95" s="4" t="s">
+      <c r="H104" s="9" t="s">
+        <v>385</v>
+      </c>
+      <c r="I104" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="J104" t="s">
+        <v>241</v>
+      </c>
+      <c r="K104" t="s">
+        <v>275</v>
+      </c>
+      <c r="M104" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="105" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D105" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E95" s="5" t="s">
+      <c r="E105" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="F95" t="s">
-        <v>146</v>
-      </c>
-      <c r="I95" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="K95" t="s">
-        <v>286</v>
-      </c>
-      <c r="L95" t="s">
+      <c r="F105" t="s">
+        <v>145</v>
+      </c>
+      <c r="H105" t="s">
+        <v>386</v>
+      </c>
+      <c r="I105" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="K105" t="s">
+        <v>276</v>
+      </c>
+      <c r="L105" t="s">
+        <v>307</v>
+      </c>
+      <c r="M105" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="106" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="L106" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="107" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="F107" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="108" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="J108" t="s">
         <v>319</v>
       </c>
-      <c r="M95" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="98" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J98" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="100" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="K100" t="s">
-        <v>338</v>
+    </row>
+    <row r="110" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="J110" t="s">
+        <v>359</v>
+      </c>
+      <c r="K110" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="111" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="J111" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="112" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="J112" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="113" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J113" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="114" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J114" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="115" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J115" t="s">
+        <v>364</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="F18" r:id="rId1" xr:uid="{F0B0DE59-DA83-4C12-86F8-32FF2B1DA60A}"/>
-    <hyperlink ref="F79" r:id="rId2" xr:uid="{271D87EF-FE75-4435-92F0-B7C42F80D97B}"/>
-    <hyperlink ref="F82" r:id="rId3" xr:uid="{D1B3712C-9998-452C-A666-F08A0C006BA6}"/>
+    <hyperlink ref="F89" r:id="rId2" xr:uid="{271D87EF-FE75-4435-92F0-B7C42F80D97B}"/>
+    <hyperlink ref="F92" r:id="rId3" xr:uid="{D1B3712C-9998-452C-A666-F08A0C006BA6}"/>
     <hyperlink ref="F12" r:id="rId4" xr:uid="{D2F7C913-C7F7-4312-8F91-1AA5D7271530}"/>
     <hyperlink ref="F11" r:id="rId5" xr:uid="{2A4AF34E-315F-4EDD-8729-D0E1F5DF7C57}"/>
     <hyperlink ref="F13" r:id="rId6" xr:uid="{80E83750-08C2-48C7-A1D3-65C2345C8FEE}"/>
     <hyperlink ref="F14" r:id="rId7" xr:uid="{B0B065DB-6FB3-4424-B095-6EE5E7304B93}"/>
     <hyperlink ref="F20" r:id="rId8" xr:uid="{38A3E9EE-76E1-47EF-9707-5FE2A8E77F9C}"/>
     <hyperlink ref="F22" r:id="rId9" xr:uid="{942D8DE3-DFD7-46BC-976E-6F2F4FCC9D02}"/>
-    <hyperlink ref="F26" r:id="rId10" xr:uid="{3FB93EA1-EE6D-4F02-9FD5-A05F7DDDB7D1}"/>
-    <hyperlink ref="F31" r:id="rId11" xr:uid="{25D4F6C4-B46F-497B-BF24-33C9AC171B81}"/>
-    <hyperlink ref="F33" r:id="rId12" xr:uid="{39833C68-0968-45C8-8399-2B41E42C29A0}"/>
-    <hyperlink ref="F38" r:id="rId13" xr:uid="{7D306272-7814-4438-BA51-7EC4EC0A0263}"/>
-    <hyperlink ref="F39" r:id="rId14" xr:uid="{1708FE19-42CF-439F-A054-74076BDCFB31}"/>
-    <hyperlink ref="F40" r:id="rId15" xr:uid="{6EC2A991-B639-4F28-B084-7FD868EBC97B}"/>
-    <hyperlink ref="F43" r:id="rId16" xr:uid="{C660C1FA-F167-4FFA-BD40-731399EAEFE3}"/>
-    <hyperlink ref="F46" r:id="rId17" xr:uid="{BDD0178F-0648-4572-A133-A5E735F9A719}"/>
-    <hyperlink ref="F48" r:id="rId18" xr:uid="{A6E53AAA-1E50-4090-B34B-9F87DB2CE138}"/>
-    <hyperlink ref="F49" r:id="rId19" xr:uid="{F1340F25-1CE1-4A96-AB21-10821F8050FA}"/>
-    <hyperlink ref="F56" r:id="rId20" xr:uid="{B87BED42-9B54-4B78-9DEB-BD28B530DA1B}"/>
-    <hyperlink ref="F60" r:id="rId21" xr:uid="{9D4DB46C-D914-46AE-8B8E-CC1C300FDA98}"/>
-    <hyperlink ref="F76" r:id="rId22" xr:uid="{AC0778F0-1F7B-41B3-813B-1245E10BFE52}"/>
+    <hyperlink ref="F27" r:id="rId10" xr:uid="{3FB93EA1-EE6D-4F02-9FD5-A05F7DDDB7D1}"/>
+    <hyperlink ref="F32" r:id="rId11" xr:uid="{25D4F6C4-B46F-497B-BF24-33C9AC171B81}"/>
+    <hyperlink ref="F34" r:id="rId12" xr:uid="{39833C68-0968-45C8-8399-2B41E42C29A0}"/>
+    <hyperlink ref="F39" r:id="rId13" xr:uid="{7D306272-7814-4438-BA51-7EC4EC0A0263}"/>
+    <hyperlink ref="F40" r:id="rId14" xr:uid="{1708FE19-42CF-439F-A054-74076BDCFB31}"/>
+    <hyperlink ref="F41" r:id="rId15" xr:uid="{6EC2A991-B639-4F28-B084-7FD868EBC97B}"/>
+    <hyperlink ref="F44" r:id="rId16" xr:uid="{C660C1FA-F167-4FFA-BD40-731399EAEFE3}"/>
+    <hyperlink ref="F47" r:id="rId17" xr:uid="{BDD0178F-0648-4572-A133-A5E735F9A719}"/>
+    <hyperlink ref="F49" r:id="rId18" xr:uid="{A6E53AAA-1E50-4090-B34B-9F87DB2CE138}"/>
+    <hyperlink ref="F50" r:id="rId19" xr:uid="{F1340F25-1CE1-4A96-AB21-10821F8050FA}"/>
+    <hyperlink ref="F57" r:id="rId20" xr:uid="{B87BED42-9B54-4B78-9DEB-BD28B530DA1B}"/>
+    <hyperlink ref="F61" r:id="rId21" xr:uid="{9D4DB46C-D914-46AE-8B8E-CC1C300FDA98}"/>
+    <hyperlink ref="F86" r:id="rId22" xr:uid="{AC0778F0-1F7B-41B3-813B-1245E10BFE52}"/>
     <hyperlink ref="F7" r:id="rId23" xr:uid="{387C584A-278C-450E-820B-6D592CD9B542}"/>
     <hyperlink ref="F8" r:id="rId24" xr:uid="{231440AF-B43B-4790-9E97-F51A5021CA9A}"/>
     <hyperlink ref="F9" r:id="rId25" xr:uid="{75397D25-F535-4596-87C1-6CE4AF75CB9C}"/>
     <hyperlink ref="F10" r:id="rId26" xr:uid="{01187902-B213-47A1-B0AB-38BC026033E3}"/>
-    <hyperlink ref="F78" r:id="rId27" xr:uid="{AE505ADC-5D84-4887-8B45-D1B047108302}"/>
-    <hyperlink ref="F77" r:id="rId28" xr:uid="{4B851A94-480D-4562-A61A-EB57C6B36F7F}"/>
-    <hyperlink ref="I70" r:id="rId29" display="https://www.ozon.ru/product/makfa-lyubitelskaya-vermishel-dlinnaya-spagetti-500-g-140800360/?asb=PiXAxdUD%252Fb8Q6qcfNBYgYZSa74CfvsYST7VXIKCqsI4%253D&amp;asb2=oFSDihkMWoB8nWmHdebLJHz0vIatpYbUNfq2HRXzEndDi0EfZLepBYnsQxQRgmua&amp;ectx=1&amp;keywords=%D0%BC%D0%B0%D0%BA%D1%84%D0%B0&amp;miniapp=supermarket&amp;sh=K5xV8WIg-g" xr:uid="{E76EC934-5688-487D-8CEB-7EECD8297302}"/>
+    <hyperlink ref="F88" r:id="rId27" xr:uid="{AE505ADC-5D84-4887-8B45-D1B047108302}"/>
+    <hyperlink ref="F87" r:id="rId28" xr:uid="{4B851A94-480D-4562-A61A-EB57C6B36F7F}"/>
+    <hyperlink ref="I71" r:id="rId29" display="https://www.ozon.ru/product/makfa-lyubitelskaya-vermishel-dlinnaya-spagetti-500-g-140800360/?asb=PiXAxdUD%252Fb8Q6qcfNBYgYZSa74CfvsYST7VXIKCqsI4%253D&amp;asb2=oFSDihkMWoB8nWmHdebLJHz0vIatpYbUNfq2HRXzEndDi0EfZLepBYnsQxQRgmua&amp;ectx=1&amp;keywords=%D0%BC%D0%B0%D0%BA%D1%84%D0%B0&amp;miniapp=supermarket&amp;sh=K5xV8WIg-g" xr:uid="{E76EC934-5688-487D-8CEB-7EECD8297302}"/>
     <hyperlink ref="I9" r:id="rId30" display="https://www.ozon.ru/product/pelmeni-imperator-tsezar-zamorozhennye-800-g-360092984/?asb=qjxJOzyaP5eiIp3dFFhocI2vC%252B0BwHzNexEcZ6ME9vI%253D&amp;asb2=kIq6DZcBFl2HVot5SyrOtbinVyUMRC8Yhi57ws0_MSIKiAv1lBgKMWLbe0sKN4G1&amp;ectx=1&amp;keywords=%D1%86%D0%B5%D0%B7%D0%B0%D1%80%D1%8C&amp;miniapp=supermarket&amp;sh=K5xV8Uep1Q" xr:uid="{2ECD4382-FE90-4913-80D1-5C2CD19FDA74}"/>
     <hyperlink ref="I10" r:id="rId31" xr:uid="{715D8978-E09F-4537-A640-856992E7F8CB}"/>
-    <hyperlink ref="I95" r:id="rId32" display="https://www.ozon.ru/product/syr-brest-litovsk-klassicheskiy-45-150-g-152141663/?asb=Tdv9tczfDa0PTKhltcp1Q6PBJg4kEMxiQyThzh5iKbU%253D&amp;asb2=gf9xWzcVUAeRvGgIa54q929unGEPpy48EadGcnul4r-wPb6gcWYx1GFdDzqUI3ln&amp;ectx=1&amp;keywords=%D0%91%D1%80%D0%B5%D1%81%D1%82+%D0%9B%D0%B8%D1%82%D0%BE%D0%B2%D1%81%D0%BA&amp;miniapp=supermarket&amp;sh=K5xV8Y4_HQ" xr:uid="{EA030594-B44A-4F70-BE65-1EAA753D15CB}"/>
-    <hyperlink ref="I94" r:id="rId33" display="https://www.ozon.ru/product/brest-litovsk-maslo-sladko-slivochnoe-nesolenoe-82-5-180-g-145923184/?asb=jIkcWaZ8F2DraHiq9EkWSqHPHpJGeby2dptq6D3zZMw%253D&amp;asb2=jU54E3oIkNKIgSViutQjlT_4Mgd1c3ms7hb00oP7TOiu8wiJapREib7WfJBxMz2F&amp;ectx=1&amp;keywords=%D0%91%D1%80%D0%B5%D1%81%D1%82+%D0%9B%D0%B8%D1%82%D0%BE%D0%B2%D1%81%D0%BA&amp;miniapp=supermarket&amp;sh=K5xV8Xe3Fg" xr:uid="{B8E2B196-F6B7-4B8D-B1DC-360FE9199845}"/>
+    <hyperlink ref="I105" r:id="rId32" display="https://www.ozon.ru/product/syr-brest-litovsk-klassicheskiy-45-150-g-152141663/?asb=Tdv9tczfDa0PTKhltcp1Q6PBJg4kEMxiQyThzh5iKbU%253D&amp;asb2=gf9xWzcVUAeRvGgIa54q929unGEPpy48EadGcnul4r-wPb6gcWYx1GFdDzqUI3ln&amp;ectx=1&amp;keywords=%D0%91%D1%80%D0%B5%D1%81%D1%82+%D0%9B%D0%B8%D1%82%D0%BE%D0%B2%D1%81%D0%BA&amp;miniapp=supermarket&amp;sh=K5xV8Y4_HQ" xr:uid="{EA030594-B44A-4F70-BE65-1EAA753D15CB}"/>
+    <hyperlink ref="I104" r:id="rId33" display="https://www.ozon.ru/product/brest-litovsk-maslo-sladko-slivochnoe-nesolenoe-82-5-180-g-145923184/?asb=jIkcWaZ8F2DraHiq9EkWSqHPHpJGeby2dptq6D3zZMw%253D&amp;asb2=jU54E3oIkNKIgSViutQjlT_4Mgd1c3ms7hb00oP7TOiu8wiJapREib7WfJBxMz2F&amp;ectx=1&amp;keywords=%D0%91%D1%80%D0%B5%D1%81%D1%82+%D0%9B%D0%B8%D1%82%D0%BE%D0%B2%D1%81%D0%BA&amp;miniapp=supermarket&amp;sh=K5xV8Xe3Fg" xr:uid="{B8E2B196-F6B7-4B8D-B1DC-360FE9199845}"/>
     <hyperlink ref="H9" r:id="rId34" xr:uid="{018BC0E8-7D36-4FDC-B01F-961CF1BAB866}"/>
     <hyperlink ref="G7" r:id="rId35" display="https://lavka.yandex.ru/213/good/b01a29d7997948658686098667c64a1e000300010000?searchQuery=%D0%A6%D0%B5%D0%B7%D0%B0%D1%80%D1%8C%20%D0%B3%D0%BE%D1%81%D1%83%D0%B4%D0%B0%D1%80%D1%8C%20%D0%B8%D0%BC%D0%BF%D0%B5%D1%80%D0%B0%D1%82%D0%BE%D1%80%20800%20%D0%B3&amp;searchPosition=-1" xr:uid="{E1D5F1F2-7D41-4892-BB76-421E3FAE8527}"/>
     <hyperlink ref="G12" r:id="rId36" xr:uid="{AF577DF4-4728-48AF-A65A-2285548B425E}"/>
-    <hyperlink ref="J14" r:id="rId37" xr:uid="{E3ADEC76-6366-47CD-B97C-D6EF83C1141B}"/>
-    <hyperlink ref="J17" r:id="rId38" xr:uid="{28F53E34-2BE7-45DE-A4C8-DE5703380BA0}"/>
-    <hyperlink ref="J42" r:id="rId39" xr:uid="{7B711258-2660-4291-8B28-70B42D0DCF9C}"/>
-    <hyperlink ref="J50" r:id="rId40" xr:uid="{C121E486-6DC5-4AB8-BDD6-D4F32794A3A4}"/>
-    <hyperlink ref="J69" r:id="rId41" xr:uid="{7F316388-2C20-4908-B372-14903C2E8EAA}"/>
-    <hyperlink ref="J73" r:id="rId42" xr:uid="{851CBC7D-F6E3-4C94-816D-5E4B54BC54F2}"/>
-    <hyperlink ref="K12" r:id="rId43" xr:uid="{06AD9E37-3909-452B-AF07-1A08C94977D7}"/>
-    <hyperlink ref="K46" r:id="rId44" xr:uid="{96CAC567-3F0E-49CA-8DEC-F36C45823856}"/>
-    <hyperlink ref="J60" r:id="rId45" xr:uid="{159BA102-A07E-4CCA-B39C-0649E37DABAB}"/>
-    <hyperlink ref="F63" r:id="rId46" xr:uid="{02308EB3-0D4F-43E5-B4E2-B6F6C09AEFBB}"/>
-    <hyperlink ref="K7" r:id="rId47" xr:uid="{12963AA2-BE9C-48F6-ADD3-656C6E23B39C}"/>
-    <hyperlink ref="H48" r:id="rId48" xr:uid="{8E5E12B2-C9E3-4CE9-A709-1339EBF59243}"/>
-    <hyperlink ref="K10" r:id="rId49" xr:uid="{A00C7BE9-6CBD-4A4B-AB12-2C62A70BE084}"/>
-    <hyperlink ref="K58" r:id="rId50" xr:uid="{7593D602-EECA-4B89-A6ED-6CF677EB1C0D}"/>
-    <hyperlink ref="K72" r:id="rId51" xr:uid="{46977EFB-3B7E-4A69-822A-E021388A83CE}"/>
-    <hyperlink ref="L63" r:id="rId52" xr:uid="{A6E2704C-7779-416A-BF8F-0168747F4B17}"/>
+    <hyperlink ref="J43" r:id="rId37" xr:uid="{7B711258-2660-4291-8B28-70B42D0DCF9C}"/>
+    <hyperlink ref="J51" r:id="rId38" xr:uid="{C121E486-6DC5-4AB8-BDD6-D4F32794A3A4}"/>
+    <hyperlink ref="J70" r:id="rId39" xr:uid="{7F316388-2C20-4908-B372-14903C2E8EAA}"/>
+    <hyperlink ref="J74" r:id="rId40" xr:uid="{851CBC7D-F6E3-4C94-816D-5E4B54BC54F2}"/>
+    <hyperlink ref="K12" r:id="rId41" xr:uid="{06AD9E37-3909-452B-AF07-1A08C94977D7}"/>
+    <hyperlink ref="K47" r:id="rId42" xr:uid="{96CAC567-3F0E-49CA-8DEC-F36C45823856}"/>
+    <hyperlink ref="J61" r:id="rId43" xr:uid="{159BA102-A07E-4CCA-B39C-0649E37DABAB}"/>
+    <hyperlink ref="F64" r:id="rId44" xr:uid="{02308EB3-0D4F-43E5-B4E2-B6F6C09AEFBB}"/>
+    <hyperlink ref="K7" r:id="rId45" xr:uid="{12963AA2-BE9C-48F6-ADD3-656C6E23B39C}"/>
+    <hyperlink ref="H49" r:id="rId46" xr:uid="{8E5E12B2-C9E3-4CE9-A709-1339EBF59243}"/>
+    <hyperlink ref="K10" r:id="rId47" xr:uid="{A00C7BE9-6CBD-4A4B-AB12-2C62A70BE084}"/>
+    <hyperlink ref="K59" r:id="rId48" xr:uid="{7593D602-EECA-4B89-A6ED-6CF677EB1C0D}"/>
+    <hyperlink ref="K73" r:id="rId49" xr:uid="{46977EFB-3B7E-4A69-822A-E021388A83CE}"/>
+    <hyperlink ref="L64" r:id="rId50" xr:uid="{A6E2704C-7779-416A-BF8F-0168747F4B17}"/>
+    <hyperlink ref="J9" r:id="rId51" xr:uid="{008C7D2B-E38E-4E27-B175-93EF66E5BA88}"/>
+    <hyperlink ref="J69" r:id="rId52" xr:uid="{4039C487-EB12-4F7C-9DE7-06EA042FFD2D}"/>
+    <hyperlink ref="J78" r:id="rId53" xr:uid="{6B7D29C3-52C4-4049-AA04-92C5CACA0D6B}"/>
+    <hyperlink ref="H98" r:id="rId54" xr:uid="{43050494-654D-45F2-AE59-7C5313A00FC2}"/>
+    <hyperlink ref="H104" r:id="rId55" xr:uid="{E230078A-0B3B-4E54-9A65-52FAB8048042}"/>
+    <hyperlink ref="L7" r:id="rId56" xr:uid="{3F898277-AC53-489C-B199-74F51F108BD6}"/>
+    <hyperlink ref="L86" r:id="rId57" xr:uid="{32241EFA-8502-4F0D-9CC4-A1E387DB2156}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId53"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId58"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new update for db
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mihail\PycharmProjects\parce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BACCFAA9-A311-46E5-BB84-566ABE6DE35A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E058AB-5DF2-4958-BF45-2872EBC5CF22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{FFE27364-2778-47AC-8397-2059D7069E9C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="498">
   <si>
     <t>Бренд</t>
   </si>
@@ -369,9 +369,6 @@
     <t>https://www.perekrestok.ru/cat/417/p/pelmeni-cezar-imperator-800g-3669807</t>
   </si>
   <si>
-    <t>https://www.ozon.ru/product/pelmeni-zamorozhennye-tsezar-tsarskoe-zastole-750-g-167975764/?sh=K5xV8cKooA</t>
-  </si>
-  <si>
     <t>https://www.perekrestok.ru/cat/417/p/pelmeni-cezar-gordost-sibiri-800g-3666702</t>
   </si>
   <si>
@@ -429,27 +426,9 @@
     <t>https://www.perekrestok.ru/cat/396/p/muka-makfa-vyssego-sorta-2kg-91304</t>
   </si>
   <si>
-    <t>https://www.perekrestok.ru/cat/443/p/zubnaa-pasta-splat-biokalcij-100ml-2104916</t>
-  </si>
-  <si>
-    <t>https://www.perekrestok.ru/cat/443/p/zubnaa-pasta-splat-professianal-bioaktivnaa-lecebnye-travy-100ml-2172628</t>
-  </si>
-  <si>
     <t>https://www.perekrestok.ru/cat/471/p/gel-dla-stirki-biomio-bio-sensitive-dla-delikatnyh-tkanej-1-5l-3694702</t>
   </si>
   <si>
-    <t>https://www.perekrestok.ru/cat/471/p/porosok-stiralnyj-biomio-bio-color-ekologicnyj-dla-cvetnogo-bela-koncentrat-1-5kg-3418106</t>
-  </si>
-  <si>
-    <t>https://www.perekrestok.ru/cat/470/p/sredstvo-dla-myta-posudy-ovosej-fruktov-biomio-maslo-mandarina-450ml-3446820</t>
-  </si>
-  <si>
-    <t>https://www.perekrestok.ru/cat/474/p/tabletki-biomio-bio-total-s-maslom-evkalipta-30st-3418093</t>
-  </si>
-  <si>
-    <t>https://www.perekrestok.ru/cat/478/p/sprej-biomio-bio-cleaner-dla-cistki-stekol-plastika-zerkal-s-ekstraktom-hlopka-500ml-3978984</t>
-  </si>
-  <si>
     <t>https://www.perekrestok.ru/cat/437/p/krem-mylo-zidkoe-usastyj-nan-s-olivkovym-maslom-i-aloe-vera-300ml-3379451</t>
   </si>
   <si>
@@ -507,81 +486,18 @@
     <t>https://online.metro-cc.ru/category/kosmetika/uhod-za-zubami/pasty-opolaskivateli/zubnaya-splat-medical-herbs-lechebnye-travy-100-ml</t>
   </si>
   <si>
-    <t>https://www.ozon.ru/product/pelmeni-gordost-sibiri-tsezar-zamorozhennye-800-g-360093003/?asb=iO0WhjLtHsaObm%252BFSQ49xqF5SE3LfrJ%252BtDHCTsLL62k%253D&amp;asb2=1OHd1rato9_m0nY8jZvTcRr8tqoEcgxVAs1HVyeOHNP526sZWaGCJ_U4N1H1xAkh&amp;ectx=1&amp;keywords=%D0%A6%D0%B5%D0%B7%D0%B0%D1%80%D1%8C+%D0%B3%D0%BE%D1%80%D0%B4%D0%BE%D1%81%D1%82%D1%8C+%D0%A1%D0%B8%D0%B1%D0%B8%D1%80%D0%B8+800+%D0%B3&amp;miniapp=supermarket&amp;sh=K5xV8Zjotw</t>
-  </si>
-  <si>
-    <t>https://www.ozon.ru/product/blinchiki-s-myasom-morozko-zamorozhennye-420-g-188564195/?asb=rNu1awsHR1Bl8LVivr24A%252BON8Geo5FL7woe9kaCrBSM%253D&amp;asb2=ZcfXEO64xYNiAXZR44S47Z4d1woYYoBXY097_NTMdHbXrf0LNlSag7FFr1CkooXN&amp;ectx=1&amp;keywords=%D0%91%D0%BB%D0%B8%D0%BD%D1%8B+%D0%9C%D0%BE%D1%80%D0%BE%D0%B7%D0%BA%D0%BE+%D1%81+%D0%B2%D0%B5%D1%82%D1%87%D0%B8%D0%BD%D0%BE%D0%B9+%D0%B8+%D1%81%D1%8B%D1%80%D0%BE%D0%BC+420%D0%B3&amp;miniapp=supermarket&amp;sh=K5xV8Q-72A</t>
-  </si>
-  <si>
-    <t>https://www.ozon.ru/product/blinchiki-zamorozhennye-morozko-s-tvorogom-420-g-188564196/?asb=YK%252FKpMHCru3dEMbjQJz1DmtwSvdLyMcSzmb0YmMq7uc%253D&amp;asb2=EztbBqGeYkh6Q6u1uueiNmRWpXN--L6rhAFyFtL4hIw9uf_hbFExbROBYehBr90d&amp;ectx=1&amp;keywords=%D0%91%D0%BB%D0%B8%D0%BD%D1%8B+%D0%9C%D0%BE%D1%80%D0%BE%D0%B7%D0%BA%D0%BE+%D1%81+%D0%B2%D0%B5%D1%82%D1%87%D0%B8%D0%BD%D0%BE%D0%B9+%D0%B8+%D1%81%D1%8B%D1%80%D0%BE%D0%BC+420%D0%B3&amp;miniapp=supermarket&amp;sh=K5xV8ZoiVg</t>
-  </si>
-  <si>
-    <t>https://www.ozon.ru/product/pitstsa-la-trattoria-s-vetchinoy-i-gribami-335-g-162288239/?asb=G%252FdevnP7%252Fe2EShnBqBIWXxe2v9MHeYNVMNqVaZIX61U%253D&amp;asb2=PuqAsdiuuI1c7kzU2825XVwvCdTlnU-ZFtTKFmjFb2MVAVBnc0TV2nBIl61wyBs-&amp;ectx=1&amp;keywords=%D0%9F%D0%B8%D1%86%D1%86%D0%B0+La+Trattoria+%D0%B2%D0%B5%D1%82%D1%87%D0%B8%D0%BD%D0%B0+%D0%B3%D1%80%D0%B8%D0%B1%D1%8B+335%D0%B3&amp;miniapp=supermarket&amp;sh=K5xV8R9aZw</t>
-  </si>
-  <si>
-    <t>https://www.ozon.ru/product/kruassany-la-reine-zamorozhennye-420-g-360089439/?asb=tE9ELMdvljQoBoiGDaDp9BjrOQRGieGFbAeOUA7%252FXjw%253D&amp;asb2=TKVWjRPuSNBTdfzJKvKSZIFKCTheBj870sMMvXC5Utd_1-m6ldNgrOCyJyp-TGxK&amp;ectx=1&amp;keywords=%D0%9A%D1%80%D1%83%D0%B0%D1%81%D1%81%D0%B0%D0%BD%D1%8B+La+Reine+%D0%B1%D0%B5%D0%B7+%D0%BD%D0%B0%D1%87%D0%B8%D0%BD%D0%BA%D0%B8+6%D1%88%D1%82+420%D0%B3&amp;miniapp=supermarket&amp;sh=K5xV8YTL-Q</t>
-  </si>
-  <si>
     <t>https://www.ozon.ru/product/sytoedov-kurinye-grudki-v-teste-s-sousom-syuprem-i-kartofelnym-pyure-350-g-145717884/?asb=lzYGustVQh62byGX0SKJelXailmDgq5mfShBQESTOB4%253D&amp;asb2=pN4jdD2F4UfChXK9D1QidiH3pgDSFstzWQLH9L2pgIjWxYzNlxmGNkvcQdI4OYXx&amp;ectx=1&amp;keywords=%D0%A8%D0%BD%D0%B8%D1%86%D0%B5%D0%BB%D1%8C+%D1%81+%D0%BA%D0%B0%D1%80%D1%82%D0%BE%D1%84%D0%B5%D0%BB%D1%8C%D0%BD%D1%8B%D0%BC+%D0%BF%D1%8E%D1%80%D0%B5+%D0%BF%D0%BE%D0%B4+%D0%BA%D1%80%D0%B0%D1%81%D0%BD%D1%8B%D0%BC+%D1%81%D0%BE%D1%83%D1%81%D0%BE%D0%BC%2C+%C2%AB%D0%A1%D1%8B%D1%82%D0%BE%D0%95%D0%B4%D0%BE%D0%B2%C2%BB%2C+350+%D0%B3%D1%80&amp;miniapp=supermarket&amp;sh=K5xV8WvoLA</t>
   </si>
   <si>
-    <t>https://www.ozon.ru/product/mayonez-ryaba-provansal-olivkovyy-67-372-g-526017350/?asb=rX6WVWzvYWdGeNz94g7JomCfU5hVOCPfk9zpzNLtIHE%253D&amp;asb2=NzwGV6mAX_IKn7dTx08kombFknEv7-FXlbR0FYvp3dYh6i9eAUA0lfrqRD5rLux6&amp;keywords=%D1%80%D1%8F%D0%B1%D0%B0+%D0%BC%D0%B0%D0%B9%D0%BE%D0%BD%D0%B5%D0%B7+372&amp;sh=K5xV8dUXEg</t>
-  </si>
-  <si>
     <t>https://www.ozon.ru/product/voda-pitevaya-chernogolovka-negazirovannaya-5-l-pet-2-sht-175639647/?asb=huObhMtYldQT24n2JQ69ax8kL7wiV4epyV3E9sL5qSc%253D&amp;asb2=YRwjf1Oz111ma1Zr5eNr_h_-LuDKJ4cO9eAxZkOGrO7K4TA1-7VP0OULEO75-_Xg&amp;keywords=%D0%92%D0%BE%D0%B4%D0%B0+%22%D0%A7%D0%B5%D1%80%D0%BD%D0%BE%D0%B3%D0%BE%D0%BB%D0%BE%D0%B2%D0%BA%D0%B0%22+5+%D0%BB.&amp;sh=K5xV8em7NQ</t>
   </si>
   <si>
-    <t>https://www.ozon.ru/product/kokosovoe-maslo-delicato-otbelennoe-0-45-l-249231484/?_bctx=CAMQ0oKVKA&amp;asb=Y7DypC4Qoubn4onROrBldKn1ZpDJRQUqDzsrkwjhk0U%253D&amp;asb2=iuGZItK-pYZ39qk6o-kQ8M1Oh3sOBfKsc4S7B6J2ldE0VsLU8VncocP9GbjZqw3s&amp;sh=K5xV8fCVWQ</t>
-  </si>
-  <si>
     <t>https://www.ozon.ru/product/voda-pitevaya-chernogolovka-vkusnaya-artezianskaya-mineralnaya-negazirovannaya-6-sht-po-1-5-l-176107612/?asb=XlA3hALCpdVTxNnyzGR5KXGZLbBsVgPSu7FEZj0f5fw%253D&amp;asb2=gjIZZeT5DEOdLFMTy0W3uYfK59CC7wRxihIDWT8O1EDCA5HbM0er4JqCKvdzzjLJ&amp;keywords=%D1%87%D0%B5%D1%80%D0%BD%D0%BE%D0%B3%D0%BE%D0%BB%D0%BE%D0%B2%D0%BA%D0%B0+%D0%B2%D0%BE%D0%B4%D0%B0&amp;sh=K5xV8aum-Q</t>
   </si>
   <si>
     <t>https://www.ozon.ru/product/limonad-chernogolovka-originalnyy-1-25-l-pet-6-sht-217851416/?asb=vr4KeACAeqtLZWrLt9siySyK1f%252BlmlV2KtL19XBQKMw%253D&amp;asb2=KWL3d8ibFg-WxjWh_vp3a61gxkD0nEZr4xgnmYBrB6GUh-XuBCubA1AeYBHs8QQL&amp;keywords=%D1%87%D0%B5%D1%80%D0%BD%D0%BE%D0%B3%D0%BE%D0%BB%D0%BE%D0%B2%D0%BA%D0%B0+1.25&amp;sh=K5xV8dmCXw</t>
   </si>
   <si>
-    <t>https://www.ozon.ru/product/sen-soy-soevyy-sous-klassicheskiy-220-ml-138134144/?asb=euBRRKziDaNknsdVEEaqT4YgEechDRXhfc0cSfoCNjA%253D&amp;asb2=mI7UqsG_G1eBJv3a7fKwCpm0Q_FJJrNF1kyecOgdTQtS0Mxm8zObjVNBoOd_7lIb&amp;keywords=%D0%A1%D0%BE%D0%B5%D0%B2%D1%8B%D0%B9+%D1%81%D0%BE%D1%83%D1%81+%C2%AB%D0%9A%D0%BB%D0%B0%D1%81%D1%81%D0%B8%D1%87%D0%B5%D1%81%D0%BA%D0%B8%D0%B9%C2%BB%2C+220+%D0%BC%D0%BB.&amp;sh=K5xV8UluZQ</t>
-  </si>
-  <si>
-    <t>https://www.ozon.ru/product/sen-soy-premium-lapsha-yaichnaya-egg-noodles-300-g-138134384/?asb=0%252BXxHLtUWwUIT68ZA2dkTPDfiFlUiLygj7iTNhKy%252Fhs%253D&amp;asb2=WcEXKLr2x6bYoPlUPwua0InDEDAIi4F95c5Rp6ooYMvk_epDiJsOl3xPc-0Nqj7N&amp;keywords=EGG+NOODLES&amp;sh=K5xV8YfMIQ</t>
-  </si>
-  <si>
-    <t>https://www.ozon.ru/product/sen-soy-premium-lapsha-pshenichnaya-udon-300-g-138134382/?asb=Y1dmqdnZhiWwCJEYBq6cOqaykf77%252FMRfOnipTwP%252F77s%253D&amp;asb2=CjpLelAJwts_R8X7ydC44evA4BD6TG1jz7r_zJ1Op0qQcH0RnzTVe5igW41K7FGO&amp;keywords=%D1%83%D0%B4%D0%BE%D0%BD&amp;sh=K5xV8WB3ww</t>
-  </si>
-  <si>
-    <t>https://www.ozon.ru/product/sen-soy-premium-lapsha-grechnevaya-soba-300-g-138134380/?asb=TceGDLwPZ5NxmROzFd4ZsfRDt9k1zm4q%252FgmHOpOVsME%253D&amp;asb2=wfjmaNYEPGycX_UF-dF6vz3wMjM38itwG9Ifs7M6pLLwBo4jM3b_EBAPq6IS9uDj&amp;keywords=soba&amp;sh=K5xV8c7YOw</t>
-  </si>
-  <si>
-    <t>https://www.ozon.ru/product/sen-soy-vermishel-funchoza-200-g-138134379/?asb=Q1y%252Fh7QU8m%252FsvJW%252FTf6vntnOG1OPNO2irUETVpT1ZSw%253D&amp;asb2=0HjSCyBYFQPlSbYZy29iQHkXoO28cNvvy_YmYS4asnMF5_1Nz3d5481DRaT90s-W&amp;keywords=%D1%84%D1%83%D0%BD%D1%87%D0%BE%D0%B7%D0%B0&amp;sh=K5xV8UnqvA</t>
-  </si>
-  <si>
-    <t>https://www.ozon.ru/product/sen-soy-funchoza-pod-yaponskim-sousom-teriyaki-125-g-142813280/?asb=Rg%252FrmAuxrqMKlInHUXrjKYKLGy%252F9gMTkTZkZ4udcxck%253D&amp;asb2=RHd2fkCvPNJUnAvCkx7aFxahyI5xmNdBvOzdIed9P_Z9pBlHvT87oc0Tn6Fip0dK&amp;keywords=%D1%84%D1%83%D0%BD%D1%87%D0%BE%D0%B7%D0%B0&amp;sh=K5xV8fOPfA</t>
-  </si>
-  <si>
-    <t>https://www.ozon.ru/product/makfa-lyubitelskaya-vermishel-dlinnaya-spagetti-500-g-140800360/?asb=PiXAxdUD%252Fb8Q6qcfNBYgYZSa74CfvsYST7VXIKCqsI4%253D&amp;asb2=oFSDihkMWoB8nWmHdebLJHz0vIatpYbUNfq2HRXzEndDi0EfZLepBYnsQxQRgmua&amp;ectx=1&amp;keywords=%D0%BC%D0%B0%D0%BA%D1%84%D0%B0&amp;miniapp=supermarket&amp;sh=K5xV8WIg-g</t>
-  </si>
-  <si>
-    <t>https://www.ozon.ru/product/makfa-vermishel-pautinka-400-g-140800364/?asb=K5k%252BgOq3qgZghuvKBxCOqG0BJp%252Fmb9Wq8vAjJopa4Yw%253D&amp;asb2=54CVI2_yaNQwXDx8I8hygOa6E-Fkjlc0_7JhQWWXdHS9EuBxV9qQhK0Fi7hGPy-4&amp;keywords=%D0%BC%D0%B0%D0%BA%D1%84%D0%B0+%D0%BF%D0%B0%D1%83%D1%82%D0%B8%D0%BD%D0%BA%D0%B0&amp;sh=K5xV8WY13w</t>
-  </si>
-  <si>
-    <t>https://www.ozon.ru/product/makaronnye-izdeliya-makfa-bantiki-a-vysshiy-sort-400g-komplekt-iz-8-sht-447489354/?asb=sBKs%252Fzn2Gt59BvixPRiGWsMd2C0eTlqNxsCOLu44YTU%253D&amp;asb2=GozNEyfSHItVtL5VM_Icr7XO8aqs0_vnKq72vHVjk7YrZSuXKXrwUlOzN3OCcqvVVrnsO1gs6eH3-SqeHxJDcA&amp;keywords=%D0%BC%D0%B0%D0%BA%D1%84%D0%B0+%D0%B1%D0%B0%D0%BD%D1%82%D0%B8%D0%BA%D0%B8&amp;sh=K5xV8QfZow</t>
-  </si>
-  <si>
-    <t>https://www.ozon.ru/product/makfa-hlopya-gerkules-traditsionnyy-400-g-140800403/?asb=URtDxEY6%252F2LNjpCkmI%252BXJ7A4PptVvMtu5HPTuqoc%252FeI%253D&amp;asb2=XDSsXHVGRizDkslwdk2E36nMsCAAUMNDi05FORKwjipYfbtESstPtR2QSYKRRmPx&amp;keywords=%D0%B3%D0%B5%D1%80%D0%BA%D1%83%D0%BB%D0%B5%D1%81+%D1%82%D1%80%D0%B0%D0%B4%D0%B8%D1%86%D0%B8%D0%BE%D0%BD%D0%BD%D1%8B%D0%B9+15+%D0%BC%D0%B8%D0%BD%D0%B8&amp;sh=K5xV8WkwHQ</t>
-  </si>
-  <si>
-    <t>https://www.ozon.ru/product/biomio-ekologichnyy-gel-dlya-stirki-delikatnyh-tkaney-bio-sensitive-bez-zapaha-1-5-l-275671748/?asb=ncPCrnTbHUuIWCvcIbLsJqD3F%252FDLTXGEj4vTj13m4To%253D&amp;asb2=VicgGbfDAYfrr5REKKrgyZmjqSl1byRDxamz4gH_4fx7B_kAuYIqAUB10czaImwR&amp;keywords=%D0%AD%D0%BA%D0%BE%D0%BB%D0%BE%D0%B3%D0%B8%D1%87%D0%BD%D1%8B%D0%B9+%D0%B3%D0%B5%D0%BB%D1%8C+++%D0%B4%D0%BB%D1%8F+%D0%B4%D0%B5%D0%BB%D0%B8%D0%BA%D0%B0%D1%82%D0%BD%D1%8B%D1%85+%D1%82%D0%BA%D0%B0%D0%BD%D0%B5%D0%B9+BioMio%C2%AE+BIO-SENSITIVE+1%2C5+%D0%BB.&amp;sh=K5xV8XHVNg</t>
-  </si>
-  <si>
-    <t>https://www.ozon.ru/product/biomio-ekologichnyy-stiralnyy-poroshok-bio-color-dlya-tsvetnogo-belya-s-ekstraktom-hlopka-1-5-kg-158316972/?fromSku=26431434&amp;sh=K5xV8Tt8SA</t>
-  </si>
-  <si>
-    <t>https://www.ozon.ru/product/biomio-ekologichnoe-sredstvo-dlya-mytya-posudy-ovoshchey-i-fruktov-bio-care-bez-zapaha-450-ml-26431422/?asb=ERqDx3N%252B3XaJqlYdrUOv50bqRXMpcn%252FDm%252F9Ea0s0eH0%253D&amp;asb2=QrllhsWNJ6re4htULZqdeyEFLjROBZYSwpLePPXS0Pyigc34wr3pMyqjZWyxV4dk&amp;keywords=%D1%81%D1%80%D0%B5%D0%B4%D1%81%D1%82%D0%B2%D0%BE+%D0%B4%D0%BB%D1%8F+%D0%BC%D1%8B%D1%82%D1%8C%D1%8F+%D0%BF%D0%BE%D1%81%D1%83%D0%B4%D1%8B%2C+%D0%BE%D0%B2%D0%BE%D1%89%D0%B5%D0%B9+%D0%B8+%D1%84%D1%80%D1%83%D0%BA%D1%82%D0%BE%D0%B2+BioMio%C2%AE+BIO-CARE%2C+450+%D0%BC%D0%BB&amp;sh=K5xV8ZE-Gg</t>
-  </si>
-  <si>
-    <t>https://www.ozon.ru/product/biomio-ekologichnoe-chistyashchee-sredstvo-dlya-stekol-zerkal-plastika-bio-glass-cleaner-bez-zapaha-147577585/?asb=z4TqFNrAWCwUTbgpOZEhsTe4WDv5bl0LaZ5Bm88en0A%253D&amp;asb2=O5TFSRttjbZd-AXtQMEIis57QE_fuXJzNMDWrTMnF_nwyNxaMGpwNOby174cWL0b&amp;keywords=%D1%87%D0%B8%D1%81%D1%82%D1%8F%D1%89%D0%B8%D0%B9+%D1%81%D0%BF%D1%80%D0%B5%D0%B9+%D0%B4%D0%BB%D1%8F+%D1%81%D1%82%D0%B5%D0%BA%D0%BE%D0%BB+BioMio%C2%AE+BIO-CLEANER%2C+%D0%B1%D0%B5%D0%B7+%D0%B7%D0%B0%D0%BF%D0%B0%D1%85%D0%B0%2C+500+%D0%BC%D0%BB.&amp;sh=K5xV8bgtMQ</t>
-  </si>
-  <si>
     <t>https://www.ozon.ru/product/ushastyy-nyan-zhidkoe-krem-mylo-detskoe-s-dozatorom-dlya-ruk-i-tela-s-olivkovym-maslom-i-ekstraktom-303353378/?asb=0ZXpIQ1DaE47IGGRiNNAfp6yDw%252F8jge0wv8hXYA3PtY%253D&amp;asb2=3Eh0g3FguD215NhhA-XU6cQYDxQXz9IxRv1e5DU5_YS3FaE8MXdJxBY4wxtR1Xjr&amp;keywords=%D0%96%D0%B8%D0%B4%D0%BA%D0%BE%D0%B5+%D0%BA%D1%80%D0%B5%D0%BC-%D0%BC%D1%8B%D0%BB%D0%BE+%22%D0%A3%D1%88%D0%B0%D1%81%D1%82%D1%8B%D0%B9+%D0%BD%D1%8F%D0%BD%D1%8C%22+%D1%81+%D0%B0%D0%BB%D0%BE%D1%8D+%D0%B2%D0%B5%D1%80%D0%B0%2C+300+%D0%BC%D0%BB.&amp;sh=K5xV8ZHVMA</t>
   </si>
   <si>
@@ -591,9 +507,6 @@
     <t>https://www.ozon.ru/product/stiralnyy-poroshok-detskiy-ushastyy-nyan-gipoallergennyy-0-2-4-kg-172622421/?asb=m6mKjPTymXCcI2Or18lU0oJvTQ0QJiKq6q53A71Opaw%253D&amp;asb2=eM-rr3bGfQ9lNcdnbdf6ngawAaZtgkCxzc7-E228u9mF2QUyNYNzNqIBRQQF1f3b&amp;keywords=%D0%A1%D1%82%D0%B8%D1%80%D0%B0%D0%BB%D1%8C%D0%BD%D1%8B%D0%B9+%D0%BF%D0%BE%D1%80%D0%BE%D1%88%D0%BE%D0%BA+%D0%B4%D0%BB%D1%8F+%D0%B4%D0%B5%D1%82%D1%81%D0%BA%D0%BE%D0%B3%D0%BE+%D0%B1%D0%B5%D0%BB%D1%8C%D1%8F+%C2%AB%D0%A3%D1%88%D0%B0%D1%81%D1%82%D1%8B%D0%B9+%D0%BD%D1%8F%D0%BD%D1%8C%C2%BB%2C+2%2C4+%D0%BA%D0%B3.&amp;sh=K5xV8Tp3GQ</t>
   </si>
   <si>
-    <t>https://www.ozon.ru/product/brest-litovsk-maslo-sladko-slivochnoe-nesolenoe-82-5-180-g-145923184/?asb=jIkcWaZ8F2DraHiq9EkWSqHPHpJGeby2dptq6D3zZMw%253D&amp;asb2=jU54E3oIkNKIgSViutQjlT_4Mgd1c3ms7hb00oP7TOiu8wiJapREib7WfJBxMz2F&amp;ectx=1&amp;keywords=%D0%91%D1%80%D0%B5%D1%81%D1%82+%D0%9B%D0%B8%D1%82%D0%BE%D0%B2%D1%81%D0%BA&amp;miniapp=supermarket&amp;sh=K5xV8Xe3Fg</t>
-  </si>
-  <si>
     <t>https://www.ozon.ru/product/syr-brest-litovsk-klassicheskiy-45-150-g-152141663/?asb=Tdv9tczfDa0PTKhltcp1Q6PBJg4kEMxiQyThzh5iKbU%253D&amp;asb2=gf9xWzcVUAeRvGgIa54q929unGEPpy48EadGcnul4r-wPb6gcWYx1GFdDzqUI3ln&amp;ectx=1&amp;keywords=%D0%91%D1%80%D0%B5%D1%81%D1%82+%D0%9B%D0%B8%D1%82%D0%BE%D0%B2%D1%81%D0%BA&amp;miniapp=supermarket&amp;sh=K5xV8Y4_HQ</t>
   </si>
   <si>
@@ -615,9 +528,6 @@
     <t>https://www.utkonos.ru/item/3057261/bliny-morozko-s-mjasom-zamorozhennye-420-g</t>
   </si>
   <si>
-    <t>https://www.utkonos.ru/item/3325041/kotlety-morozko-green-ovoshhnye-zamorozhennye</t>
-  </si>
-  <si>
     <t>https://www.utkonos.ru/item/3396152/kotlety-morozko-iz-govjadiny-zamorozhennye-330-g</t>
   </si>
   <si>
@@ -711,9 +621,6 @@
     <t>https://www.utkonos.ru/item/3227951/stiralnyj-poroshok-biomio-bio-color-ekologichnyj-dlja-cvetnogo-belja-1-5-kg</t>
   </si>
   <si>
-    <t>https://www.utkonos.ru/item/3224637/sredstvo-dlja-mytja-posudy-ovoshhej-i-fruktov-biomio-bio-care-bez-zapakha-450-ml</t>
-  </si>
-  <si>
     <t>https://www.utkonos.ru/item/3227930/sredstvo-dlja-mytja-posudy-v-posudomoechnoj-mashine-biomio-bio-total-7-v-1-s-efirnym-maslom-evkalipta-v-tabletkakh-30-shtuk</t>
   </si>
   <si>
@@ -867,15 +774,9 @@
     <t>https://www.perekrestok.ru/cat/376/p/maslo-sladkoslivocnoe-brest-litovsk-nesolenoe-vyssego-sorta-82-5-180g-3413519</t>
   </si>
   <si>
-    <t>https://www.ozon.ru/product/zubnaya-pasta-splat-professional-biocalcium-biokaltsiy-100-ml-14125564/?asb=DQh2d2CXCPJhOsLCUsKD7IeWYbVtyE1bN1bmh1qFJlQ%253D&amp;asb2=iKz35uWcXwnGVyZZt_GtV2MjRDj33vLNg5IhYFtxx5UrJwueCIfZPJ--SPmerBuL&amp;keywords=splat+%D0%B7%D1%83%D0%B1%D0%BD%D0%B0%D1%8F+%D0%BF%D0%B0%D1%81%D1%82%D0%B0&amp;sh=K5xV8fHweA</t>
-  </si>
-  <si>
     <t>https://www.auchan.ru/product/krem-mylo-ushastyy-nyan-s-olivkovym-maslom-i-aloe-vera-300-ml/</t>
   </si>
   <si>
-    <t>https://www.ozon.ru/product/biomio-ekologichnye-tabletki-dlya-posudomoechnoy-mashiny-7-v-1-bio-total-s-efirnym-maslom-evkalipta-26431435/?asb=DouF%252BVPCQamL9FhU692H1xqffhfk67OyVWjBHhMBhXhh%252FRzlSVLDnfPd0lA%252F9DIx&amp;asb2=77vgEV7r0eqKtmB55MlP472Q4qSngYJQ2Lcd7rlQzehyQNscwQ51rabPiyNdxmg6LV_n0HO6xdRHUCWCX1ynGfERYVh1WRVhIJP8lvQtjvxecsEfKNejMBmVqr26bBKn&amp;keywords=%D0%A2%D0%B0%D0%B1%D0%BB%D0%B5%D1%82%D0%BA%D0%B8+%D0%B4%D0%BB%D1%8F+%D0%BF%D0%BE%D1%81%D1%83%D0%B4%D0%BE%D0%BC%D0%BE%D0%B5%D1%87%D0%BD%D0%BE%D0%B9+%D0%BC%D0%B0%D1%88%D0%B8%D0%BD%D1%8B+BioMio+BIO-TOTAL+7-%D0%B2-1+%D1%8D%D0%B2%D0%BA%D0%B0%D0%BB%D0%B8%D0%BF%D1%82%2C+30+%D1%88%D1%82&amp;sh=K5xV8fdMzQ</t>
-  </si>
-  <si>
     <t>Дикси</t>
   </si>
   <si>
@@ -924,9 +825,6 @@
     <t>https://dostavka.dixy.ru/catalog/gigiena_i_kosmetika/ukhod_za_polostyu_rta/133318/</t>
   </si>
   <si>
-    <t>https://dostavka.dixy.ru/catalog/gigiena_i_kosmetika/ukhod_za_polostyu_rta/132837/</t>
-  </si>
-  <si>
     <t>https://dostavka.dixy.ru/catalog/bytovaya_khimiya/stirka_i_ukhod_za_belem/226821/</t>
   </si>
   <si>
@@ -1204,6 +1102,432 @@
   </si>
   <si>
     <t>https://dostavka.dixy.ru/catalog/gigiena_i_kosmetika/salfetki_i_nosovye_platki/308089/</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/471/p/porosok-stiralnyj-biomio-bio-white-dla-belogo-bela-1-5kg-3418107</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/471/p/patnovyvoditel-biomio-universalnyj-750ml-3954300</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/471/p/kondicioner-dla-bela-biomio-mandarin-koncentrat-1l-3975846</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/441/p/mylo-biomio-bio-soap-s-efirnym-maslom-cajnogo-dereva-antibakterialnoe-300ml-4090601</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/474/p/tabletki-biomio-bio-total-dla-posudomoecnoj-masiny-s-maslom-evkalipta-60st-4163731</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/479/p/sredstvo-biomio-melissa-dla-myta-polov-750ml-3978982</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/473/p/sredstvo-cistasee-biomio-bio-bathroom-cleaner-grejpfrut-dla-vannoj-i-tualeta-500ml-3954301</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/470/p/sredstvo-dla-myta-posudy-biomio-bio-care-ru-cis-20-ekstrakt-hlopka-iony-serebra-bez-zapaha-l-4104185</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/443/p/zubnaa-pasta-splat-otbelivanie-plus-100ml-2172627</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/443/p/zubnaa-pasta-splat-professianal-sensitiv-100ml-3480375</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/443/p/zubnaa-pasta-splat-aktiv-100ml-2104917</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/443/p/zubnaa-pasta-detskaa-splat-kids-bioaktivnaa-zemlanika-visna-50ml-3489655</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/443/p/zubnaa-setka-splat-professional-whitening-medium-srednej-zestkosti-3298563</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/443/p/zubnaa-setka-splat-professional-ultra-complete-srednej-zestkosti-4080489</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/443/p/zubnaa-setka-splat-professional-whitening-hard-zestkaa-3329901</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/443/p/zubnaa-setka-splat-professional-ultra-sensitive-soft-s-magkoj-setinoj-3966333</t>
+  </si>
+  <si>
+    <t>https://www.perekrestok.ru/cat/443/p/zubnaa-setka-detskaa-splat-kids-magkaa-v-assortimente-3376273</t>
+  </si>
+  <si>
+    <t>https://lavka.yandex.ru/213/good/ae8cc776b4e3408c836dd1e90deef59f000100010001?searchQuery=BioMio&amp;searchPosition=-1</t>
+  </si>
+  <si>
+    <t>https://lavka.yandex.ru/213/good/cebd8ee8a29e49ba8e180ebeee64da4c000200010001?searchQuery=BioMio&amp;searchPosition=-1</t>
+  </si>
+  <si>
+    <t>https://lavka.yandex.ru/213/good/67bc7a96f1b84a0aa3ae02a413dcc571000300010000?searchQuery=splat&amp;searchPosition=-1</t>
+  </si>
+  <si>
+    <t>https://lavka.yandex.ru/213/good/367d3ec2830d4920bfac76e13fdfa0a0000100010001?searchQuery=splat&amp;searchPosition=-1</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3396149/vareniki-cezar-s-kartofelem-i-zharenym-luchkom-600-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3226799/stiralnyj-poroshok-biomio-bio-white-ekologichnyj-dlja-belogo-belja-1-5-kg</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3360773/kondicioner-dlja-belja-biomio-bio-soft-s-aromatom-evkalipta-i-khlopka-1-l</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3428014/mylo-biomio-bio-soap-khozjajstvennoe-pjatnovyvoditel-ekologichnoe-bez-zapakha-200-g</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3516873/credstvo-dlja-mytja-posudy-biomio-bio-care-refill-ekologichnoe-s-ekstraktom-khlopka-i-ionami-serebra-koncentrat-500-ml</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3401361/sredstvo-dlja-mytja-detskoj-posudy-biomio-baby-bio-balm-romashka-i-ilang-ilang-eko-balzam-450-ml</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3401365/sredstvo-chistjashhee-dlja-posudomoechnoj-mashiny-biomio-bio-salt-sol-1-kg</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3510965/opolaskivatel-dlja-posudomoechnoj-mashiny-biomio-bio-rinse-ekologichnyj-750-ml</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3361972/sredstvo-dlja-mytja-pola-biomio-bio-floor-cleaner-melissa-ekologichnoe-zhidkoe-750-ml</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3399571/mylo-zhidkoe-dlja-ruk-biomio-bio-soap-s-maslom-abrikosa-300-ml</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/gigiena_i_kosmetika/ukhod_za_polostyu_rta/133317/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/gigiena_i_kosmetika/ukhod_za_polostyu_rta/191303/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/gigiena_i_kosmetika/ukhod_za_polostyu_rta/264062/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/gigiena_i_kosmetika/ukhod_za_polostyu_rta/134781/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/tovary_dlya_detey/gigiena_i_ukhod/230785/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/tovary_dlya_detey/gigiena_i_ukhod/302596/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/gigiena_i_kosmetika/ukhod_za_polostyu_rta/309050/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/gigiena_i_kosmetika/ukhod_za_polostyu_rta/303639/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/tovary_dlya_detey/gigiena_i_ukhod/302603/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/gigiena_i_kosmetika/ukhod_za_polostyu_rta/133074/</t>
+  </si>
+  <si>
+    <t>https://dostavka.dixy.ru/catalog/gigiena_i_kosmetika/ukhod_za_polostyu_rta/302604/</t>
+  </si>
+  <si>
+    <t>https://online.metro-cc.ru/category/bytovaya-himiya/sredstva-dlya-stirki/stiralnye-poroshki/stiralnyj-poroshok-bio-mio-dlya-cvetnogo-belya-s-ekstraktom-hlopka-15kg</t>
+  </si>
+  <si>
+    <t>https://online.metro-cc.ru/category/bytovaya-himiya/sredstva-dlya-stirki/uhod-za-tkanyami/15l-koncentrat-delik-tkanej</t>
+  </si>
+  <si>
+    <t>https://online.metro-cc.ru/category/bytovaya-himiya/sredstva-dlya-stirki/zhidkie-sredstva-dlya-stirki/art_63343</t>
+  </si>
+  <si>
+    <t>https://online.metro-cc.ru/category/bytovaya-himiya/sredstva-dlya-mytya-posudy/dlya-posudomoechnyh-mashin/biomio-bio-salt-ekologichnaya-sol-biomio-bio-salt-eco-dish-washer-salt-1000-g</t>
+  </si>
+  <si>
+    <t>https://online.metro-cc.ru/category/bytovaya-himiya/chistyaschie-sredstva/universalnye-chistyashchie-sredstva/sprej-bez-zapaha-bio-mio-7v1-350ml</t>
+  </si>
+  <si>
+    <t>https://online.metro-cc.ru/category/kosmetika/uhod-za-zubami/pasty-opolaskivateli/zubnaya-splat-white-plus-otbelivanie-plyus-100-ml</t>
+  </si>
+  <si>
+    <t>https://online.metro-cc.ru/category/kosmetika/uhod-za-zubami/pasty-opolaskivateli/zubnaya-splat-sensitive-sensitiv-antibakterialnaya-100-ml</t>
+  </si>
+  <si>
+    <t>https://online.metro-cc.ru/category/kosmetika/uhod-za-zubami/pasty-opolaskivateli/zubnaya-splat-active-aktiv-100-ml</t>
+  </si>
+  <si>
+    <t>https://online.metro-cc.ru/category/kosmetika/uhod-za-zubami/pasty-opolaskivateli/zubnaya-splat-ultracomplex-ultrakompleks-antibakterialnaya-100-ml</t>
+  </si>
+  <si>
+    <t>https://online.metro-cc.ru/category/kosmetika/uhod-za-zubami/shchetki-114003002/zubnaya-splat-ultra-sensitive-myagkaya</t>
+  </si>
+  <si>
+    <t>https://online.metro-cc.ru/category/kosmetika/uhod-za-zubami/shchetki-114003002/z-sch-splat-ultra-complete-srednyaya</t>
+  </si>
+  <si>
+    <t>https://online.metro-cc.ru/category/kosmetika/uhod-za-zubami/shchetki-114003002/zubnaya-splat-whitening-zhestkaya</t>
+  </si>
+  <si>
+    <t>https://online.metro-cc.ru/category/kosmetika/uhod-za-zubami/shchetki-114003002/zubnaya-splat-otbelivayuschaya-srednej-zhestkosti</t>
+  </si>
+  <si>
+    <t>https://online.metro-cc.ru/category/kosmetika/uhod-za-zubami/shchetki-114003002/detskaya-zubnaya-schetka-splat-kids-antibakterialnaya-myagkaya</t>
+  </si>
+  <si>
+    <t>https://online.metro-cc.ru/category/kosmetika/uhod-za-zubami/shchetki-114003002/zubnaya-splat-junior-myagkaya</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3105647/zubnaja-pasta-splat-professional-otbelivanie-pljus-100-ml</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3281505/zubnaja-pasta-splat-sensitive-antibakterialnaja-vosstanovlenie-emali-100-ml</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3105598/zubnaja-pasta-splat-professional-aktiv-kompleksnyj-ukhod-100-ml</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3105644/zubnaja-pasta-splat-ultrakompleks-antibakterialnaja-otbelivajushhaja-100-ml</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3320919/zubnaja-pasta-detskaja-splat-junior-babl-gam-s-6-do-11-let-55-ml</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3501923/zubnaja-shhetka-splat-professional-ultra-komplit-srednjaja-zhestkost-zelenaja</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3173968/zubnaja-shhetka-splat-professional-whitening-srednjaja-zhestkost</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3173994/zubnaja-shhetka-splat-professional-whitening-zhestkaja</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3421812/zubnaja-shhetka-detskaja-splat-kids-mjagkaja-cvet-zheltyj-s-2-do-8-let</t>
+  </si>
+  <si>
+    <t>https://www.utkonos.ru/item/3401712/zubnaja-shhetka-detskaja-splat-junior-so-happy-s-ionami-serebra-mjagkaja-zheltaja-s-4-let</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/pelmeni-tsezar-klassika-800-g-162288229/?asb=kuSwhXEyi7%252F%252BdSmYvl9Sid7EmX%252FQou4lwb8KQkvzEc0%253D&amp;asb2=C32LR2cB7pPbjRtboKeHS4ovSQtrZHpKDA8QTSUpcjpwuFyaX3xvdTAaKJj_WNLP&amp;ectx=1&amp;keywords=%D1%86%D0%B5%D0%B7%D0%B0%D1%80%D1%8C&amp;miniapp=supermarket&amp;sh=K5xV8Q13sQ</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/pelmeni-gordost-sibiri-tsezar-zamorozhennye-800-g-360093003/?asb=42nQZAJ1ITGn1VHElT2cqfyk%252FJMPpZ276K%252Bdr%252FRLPsU%253D&amp;asb2=e1svIVBTpzR_wpAa3G_zoesJtpxA4GmtJ9Z7vMxskORlZbKYKHM36Rdp2LsnMZUa&amp;ectx=1&amp;keywords=%D1%86%D0%B5%D0%B7%D0%B0%D1%80%D1%8C+%D0%BF%D0%B5%D0%BB%D1%8C%D0%BC%D0%B5%D0%BD%D0%B8&amp;miniapp=supermarket&amp;sh=K5xV8XnkXQ</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/testo-sloenoe-bezdrozhzhevoe-morozko-400-g-483915621/?asb=lS%252FDdgWY7qcQ8QLDKyjchUkhgLK7ishgApYHBHjA0WU%253D&amp;asb2=bSo5EOa9Q-T0hzu9qCojO1Gx50VQ8tY40e5Gcy43d_L0B-Nr45fAevSLKm9iueIi&amp;ectx=1&amp;keywords=%D0%BC%D0%BE%D1%80%D0%BE%D0%B7%D0%BA%D0%BE+%D1%82%D0%B5%D1%81%D1%82%D0%BE&amp;miniapp=supermarket&amp;sh=K5xV8SetZA</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/testo-sloenoe-drozhzhevoe-morozko-400-g-483915632/?asb=e0YrAYZuJdmIJL2sIWNqfg6l%252F%252FOa4EkFuv8R4qtACd0%253D&amp;asb2=bmKGLT9--T_6w_UWuy6YvTXpu0RJ7Nmc2DX_eNj_SQvtt_pjoq0rgY0yVjuq0vcZ&amp;ectx=1&amp;keywords=%D0%BC%D0%BE%D1%80%D0%BE%D0%B7%D0%BA%D0%BE+%D1%82%D0%B5%D1%81%D1%82%D0%BE&amp;miniapp=supermarket&amp;sh=K5xV8SJ5Hg</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/testo-sloenoe-morozko-bezdrozhzhevoe-legkoe-500-g-162288234/?asb=NFW66R79e6QSQI0DvP5oT0f5XoqyyZsv8FrVr2CHRPo%253D&amp;asb2=1faM-rd0BE3FT49TVwL-_a5Ua_EoADL7YDfsCEji3Ht3J0ggzUSWrwmYdojhsZll&amp;ectx=1&amp;keywords=%D0%BC%D0%BE%D1%80%D0%BE%D0%B7%D0%BA%D0%BE+%D1%82%D0%B5%D1%81%D1%82%D0%BE&amp;miniapp=supermarket&amp;sh=K5xV8XZfLQ</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/kruassany-la-reine-zamorozhennye-420-g-360089439/?asb=HI2JSZXCwRR1ISXay0DmlvNZzFkK7gTDu5ZURfBfnfQ%253D&amp;asb2=c-smRLozWsBFWpxZgLy_h_yjALldslTwTbOVEZt2eEqyNxPx0zfcEpzc7d_VOIl_&amp;ectx=1&amp;keywords=la+reine&amp;miniapp=supermarket&amp;sh=K5xV8dnKig</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/kruassany-s-shokoladom-la-reine-zamorozhennye-420-g-360089424/?asb=Wn7bvGoaCDRibLOl7rHdEyAJPwToUkvS6A0GxF5cJqw%253D&amp;asb2=Gpcuspc5Mr9j6x1V1S6OhY7FROiOe_kRFpTqAj0iMfYPs0zBGKT01q9iULy5WdME&amp;ectx=1&amp;keywords=la+reine&amp;miniapp=supermarket&amp;sh=K5xV8WxRPg</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/blinchiki-s-myasom-morozko-zamorozhennye-420-g-188564195/?asb=%252FY%252BdpCo8oB7w5%252B5iNOWKZzbJNcpdnouaYwNYtu9AzlE%253D&amp;asb2=-EL4O0womKU9xpDE8JZb2xvM9IeJvz4gx7mqDQpOnjaoKD63kpyc8QVEj3EWPk0Q&amp;ectx=1&amp;keywords=%D0%BC%D0%BE%D1%80%D0%BE%D0%B7%D0%BA%D0%BE+%D0%B1%D0%BB%D0%B8%D0%BD%D1%8B&amp;miniapp=supermarket&amp;sh=K5xV8UKVOg</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/blinchiki-tsezar-s-telyatinoy-450-g-162288230/?asb=R0D9ivjnN%252B%252FVuD%252BNPlGO%252FSBw3fdRV3hgIb%252BJzuxsxrY%253D&amp;asb2=vFNUSY0eIHMhxq_k4pfG_gCo2BOnil3AUBWOoyv5T-VpW9Nvewh0TQ3Anq0qB9Dw&amp;ectx=1&amp;keywords=%D1%86%D0%B5%D0%B7%D0%B0%D1%80%D1%8C+%D0%B1%D0%BB%D0%B8%D0%BD%D1%8B&amp;miniapp=supermarket&amp;sh=K5xV8eoSOg</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/blinchiki-s-derevenskim-tvorogom-tsezar-450-g-483915587/?asb=Y4NrCwLEL84snk%252BWWEUHYjlzZerOmyG96uaH0aPcLeU%253D&amp;asb2=hRCE69ABKgkGWGcpbhSOj04-eAkClbi-lMSSZ8uNzOXN1l4Dpr7Pb9xGeWJNPUe7&amp;ectx=1&amp;keywords=%D1%86%D0%B5%D0%B7%D0%B0%D1%80%D1%8C+%D0%B1%D0%BB%D0%B8%D0%BD%D1%8B&amp;miniapp=supermarket&amp;sh=K5xV8cVkIg</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/cheburek-s-myasom-bogatyr-zharenki-180-g-420019067/?asb=95e0KF5YXuj%252FDY7eG4yJVNzbW8vFPYiEoFzE9xXtki0%253D&amp;asb2=8mqAaCaO8qdqnv5pFcNo1g8n1g9_NxNkBEo9IPavT9ACSbPS4iRxjvwYDVRPE6pg&amp;keywords=%D0%B6%D0%B0%D1%80%D0%B5%D0%BD%D0%BA%D0%B8&amp;sh=K5xV8UsSOg</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/pitstsa-s-vetchinoy-i-gribami-tsezar-420-g-483915605/?asb=5dzsJ8hYLoNdBSnLbHl676o0t2UqbFgK%252BO7tFUj%252B52A%253D&amp;asb2=KdZ9JTXEX_hCVPnNcOsaw18fjqTFeNzlSPCGxdGPhul877G-eXX7BpM8hgxwgIl-&amp;ectx=1&amp;keywords=%D1%86%D0%B5%D0%B7%D0%B0%D1%80%D1%8C+%D0%BF%D0%B8%D1%86%D1%86%D0%B0&amp;miniapp=supermarket&amp;sh=K5xV8bQg6w</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/pitstsa-kvartet-tsezar-420-g-483915614/?asb=7E80NcrWIg%252FnbM0pL7wMOqJXyIBDSosG%252Bcqqjtr6tIo%253D&amp;asb2=5oKTb6OqrqsStSNSRb5k__FFJJPqhpCSnH1wB1MHWoZ81q3aHHaNaH6lGBshlZfr&amp;ectx=1&amp;keywords=%D1%86%D0%B5%D0%B7%D0%B0%D1%80%D1%8C+%D0%BF%D0%B8%D1%86%D1%86%D0%B0&amp;miniapp=supermarket&amp;sh=K5xV8Tq5Og</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/pitstsa-la-trattoria-assorti-335-g-162288237/?asb=C7LYwSdb5qCOLYevCMv4UTHARvUvwJoGn879pS9VrAE%253D&amp;asb2=utQEWGkwndZEPn5eO8scGFPZFdY7ksgo1-bh4g_w5LA9YEqyIgcXVJtyfTHl-PMa&amp;ectx=1&amp;keywords=la+trattoria+%D0%BF%D0%B8%D1%86%D1%86%D0%B0&amp;miniapp=supermarket&amp;sh=K5xV8XVDbw</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/pitstsa-la-trattoria-s-motsarelloy-335-g-162288240/?asb=p8YEQCMOfp%252BvN9cQzE%252BsInuZlyxF2qxzDPrgrfXgnx8%253D&amp;asb2=_ozuhIGp8-yJ99HVO4wfUEMV7cupb95pn11q-abfSuqBZdMDGSN7CpS9szBRsqUw&amp;ectx=1&amp;keywords=la+trattoria+%D0%BF%D0%B8%D1%86%D1%86%D0%B0&amp;miniapp=supermarket&amp;sh=K5xV8Zc55Q</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/vareniki-tsezar-s-kartofelem-i-belymi-gribami-600-g-343734927/?asb=PLOiP1my4kkrydmiFYbLjZD26eqeoim%252BlbuN%252FpN3Imk%253D&amp;asb2=RGShrj5dP8PRswOOnfyLEIWhCrSV4UtKJ7DNoenrW3K7828arp7z8B74eYpDsYAX&amp;ectx=1&amp;keywords=%D1%86%D0%B5%D0%B7%D0%B0%D1%80%D1%8C+%D0%B2%D0%B0%D1%80%D0%B5%D0%BD%D0%B8%D0%BA%D0%B8&amp;miniapp=supermarket&amp;sh=K5xV8RhqZg</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/vareniki-tsezar-s-kartofelem-i-zharenym-luchkom-600-g-343734928/?asb=1xfssvQUAKtW82fFPuG5Q1uaD7mqJGQSjFRV7kjmTsE%253D&amp;asb2=umhukP1OpuUqiLMQni7Zyxhq9FppIrWC9J_VRqGdfXg7t_mMSFyszAhKtbb7sPX-&amp;ectx=1&amp;keywords=%D1%86%D0%B5%D0%B7%D0%B0%D1%80%D1%8C+%D0%B2%D0%B0%D1%80%D0%B5%D0%BD%D0%B8%D0%BA%D0%B8&amp;miniapp=supermarket&amp;sh=K5xV8SYVUA</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/naggetsy-kurinye-morozko-zamorozhennye-300-g-349268240/?asb=3XKC0ndMn12X4Usz4Ko4stpcUhwNdLqJbhyErE2Ic5k%253D&amp;asb2=3-Asga7Z_YWv_kzJp5_LGa7lSyrIuK9T_nBD-PgFMZfrC4BD3KJPTAH4QYt20m4R&amp;ectx=1&amp;keywords=%D0%BC%D0%BE%D1%80%D0%BE%D0%B7%D0%BA%D0%BE+%D0%BD%D0%B0%D0%B3%D0%B3%D0%B5%D1%82%D1%81%D1%8B&amp;miniapp=supermarket&amp;sh=K5xV8ViBmA</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/sous-mayoneznyy-astoriya-syrnyy-233g-562470584/?asb=qAD2v%252FMsk19UuDJvyEwS4j7gvJn5oz8dUUvxanPR44s%253D&amp;asb2=7hji0afT-BXcmytAnuBgOBAkzjTdqE163F1fcRcletu9Zft-LtnKZbmNYJiJkDq0&amp;ectx=1&amp;keywords=%D0%B0%D1%81%D1%82%D0%BE%D1%80%D0%B8%D1%8F&amp;miniapp=supermarket&amp;sh=K5xV8TjLvA</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/sous-mayoneznyy-astoriya-slivochno-chesnochnyy-233g-562470076/?asb=rnw4LFcYV52VJpeeY3TugAALsOxwjSyG59NwS4ysSxo%253D&amp;asb2=M2ej8d_LQtWowW_joZVU7wwbklUmM5rsm2qXvnxPayY5S__64lUGO_QtKZdY1VBv&amp;ectx=1&amp;keywords=%D0%B0%D1%81%D1%82%D0%BE%D1%80%D0%B8%D1%8F&amp;miniapp=supermarket&amp;sh=K5xV8YUL1w</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/ketchup-astoriya-shashlychnyy-330g-562450468/?asb=MU5XEu7eMoanRqizKwkhZjeKu9mhruNsW1iJ31Pihek%253D&amp;asb2=qDcbXVC6spvN-MnlCbbyeoMceygV8RdSVgdXULx01ALnJzicbtp29sZrDPlQeYp2&amp;ectx=1&amp;keywords=%D0%B0%D1%81%D1%82%D0%BE%D1%80%D0%B8%D1%8F&amp;miniapp=supermarket&amp;sh=K5xV8fcbFw</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/ketchup-astoriya-tomatnyy-330g-562450450/?asb=i0rgH00t2b8ShBvUGiOMsaWRY5FyrB6X8D9B%252Bk6Wj%252BU%253D&amp;asb2=9orDZu1Lf9FgHbBbQIRV_Oyuevr2pc4lwSTVXmM1m4lTaXHWlMZle_t1NZNZP9WY&amp;ectx=1&amp;keywords=%D0%B0%D1%81%D1%82%D0%BE%D1%80%D0%B8%D1%8F&amp;miniapp=supermarket&amp;sh=K5xV8cPdtg</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/sen-soy-soevyy-sous-klassicheskiy-220-ml-138134144/?asb=zw%252F6N5F25vgpEcCbGsKVRIAkAvKiNL8ZY1iV4j5lwXI%253D&amp;asb2=xvJI3j7V9fhSwQjlfS-792xcPJRaH0rUzRvEzia4Wz3-9TO6PM5PjyC1dbFo-nwF&amp;keywords=sen+soy+%D1%81%D0%BE%D1%83%D1%81&amp;sh=K5xV8XFefQ</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/sen-soy-premium-lapsha-yaichnaya-egg-noodles-300-g-138134384/?asb=5vWHdYaNOyfVMMQif58kS%252F4x5Dwh4vHEZ3gqL2rTi9s%253D&amp;asb2=OmdzGQAW7PS4rrpDUzKp_g1dF4imRTYcvkoAcRFRWMVxNonpyPFO94FXcYTsugzA&amp;keywords=sen+soy&amp;sh=K5xV8RHgBA</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/lapsha-grechnevaya-sen-soy-premium-soba-300-g-532187446/?asb=WGjRjmJEAfXIKbdEHtIMX0RQMeXGzsg9shj2zwuDxsnwVCNx9wpUeFwyulfIzky6&amp;asb2=sWMFFZTuPPIIZMWLRHUEIf_I4StshxUO_I-psuorSJvUuj0-oBrgTnOehIcrQD4-XGiirUWNogcNlI2iGS048y-EsaYsplQ5gVS4vY62yt0YG4z8o0vvH_XD_GNVxjjA9w-zunyPmbL5CvzZlR5bXg&amp;keywords=sen+soy&amp;sh=K5xV8UClvw</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/sen-soy-premium-lapsha-pshenichnaya-udon-300-g-138134382/?asb=JCd48%252F92AEyQJ2p7B7cWsvMT5H8%252F%252FJA6DOJDs%252F7eMqE%253D&amp;asb2=gew3OwFAFw9gdJTNW6Aj3AdKeDl3RExgCABy_K-v0cWuMSXqqfHwCqJXzycEoRhO&amp;ectx=1&amp;keywords=sen+soy+udon&amp;miniapp=supermarket&amp;sh=K5xV8WRs5A</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/sen-soy-vermishel-funchoza-200-g-138134379/?asb=NeQ2LqHLLd9sFt9VSEqt%252FjNnYcabgZe7XsBRhlZ%252F02Q%253D&amp;asb2=dxPPJkgTcnPJxtAIz4gzOczuxNMivf2XpOFjjQBRZinAQwDnTtvE7m0bcifJbeXC&amp;ectx=1&amp;keywords=sen+soy+%D1%84%D1%83%D0%BD%D1%87%D0%BE%D0%B7%D0%B0&amp;miniapp=supermarket&amp;sh=K5xV8fmUVA</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/sen-soy-funchoza-pod-yaponskim-sousom-teriyaki-125-g-142813280/?asb=1x96jVkgRFeC7AF7%252FpPTBR82KBYed4ftAmzDKeMhT7I%253D&amp;asb2=xkXAcIUvIA1ONsquj-ULDOUqfCoxCjqu4LBebnofTNCrNDQhXohzYc-bQrKskncf&amp;ectx=1&amp;keywords=sen+soy+%D1%84%D1%83%D0%BD%D1%87%D0%BE%D0%B7%D0%B0&amp;miniapp=supermarket&amp;sh=K5xV8dJTAg</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/sup-sen-soy-pho-bo-s-risovoy-lapshoy-125-g-151438743/?asb=lIQlXA5uqTlzCs4r5st0P%252BcQhI%252FlL8xA9MnehqbXSvI%253D&amp;asb2=-vEUF8IfPWCucm1izYwYtvros6UxJupq9UEbQA3g4MierKMBxZvixOhJRz2eRZ7g&amp;ectx=1&amp;keywords=sen+soy+%D1%84%D0%BE+%D0%B1%D0%BE&amp;miniapp=supermarket&amp;sh=K5xV8Zwy0Q</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/makfa-spirali-400-g-140800394/?asb=N4xXme8mUT%252BdHV%252F7J12Kb7YQ144tA4g1k%252BSA4LURrIM%253D&amp;asb2=XH9njwGpDRoPTN1-Wz3MQeTU7wwv5mG1LZ2tm02QwhCNEyCEbmMh0f9YNA_RcUd8&amp;ectx=1&amp;keywords=makfa+%D1%81%D0%BF%D0%B8%D1%80%D0%B0%D0%BB%D0%B8&amp;miniapp=supermarket&amp;sh=K5xV8eCN1g</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/makfa-perya-lyubitelskie-400-g-140800382/?asb=nhf60h0rEpO0i3Qh8m4fTZfA9hEsUoCUFn%252BeSMiZXq0%253D&amp;asb2=yYcya1mJ0kj4kXuKdkYa9ysDBnHn_Zbu7AMxQ2bIvLD7KnDjsaa02dilMsNdVFdQ&amp;ectx=1&amp;keywords=makfa+%D0%BF%D0%B5%D1%80%D1%8C%D1%8F&amp;miniapp=supermarket&amp;sh=K5xV8brqYw</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/makfa-vitki-400-g-140800365/?asb=7O5PtIBn7LHach7IVKw%252B2NUPaU521Oy9biOKqjDhyho%253D&amp;asb2=znw0jVtWWouiIGjuLSbheihn34fGFfQz2GF8Obv5ZB4mRrdXZJ5dHEhOHWKoU89t&amp;ectx=1&amp;keywords=makfa+%D0%B2%D0%B8%D1%82%D0%BA%D0%B8&amp;miniapp=supermarket&amp;sh=K5xV8Ruq2w</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/muka-makfa-pshenichnaya-hlebopekarnaya-vysshiy-sort-2-kg-140723110/?asb=rXAAbxOGoteSz5Qr%252BFt2FZGdlTfcSBQJ6Xdu7Zlz5VY%253D&amp;asb2=fUDx4_CGIQryIj3hT6jLcwD8KzzzdCpCTWq7AvrUEgeVqHKpBzwqDM-Mc_XHiVHl&amp;ectx=1&amp;keywords=makfa+%D0%BC%D1%83%D0%BA%D0%B0&amp;miniapp=supermarket&amp;sh=K5xV8XV-aQ</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/makfa-grechnevaya-yadritsa-800-g-140800411/?asb=hDltkwri85jewP0jqCjwYJLW%252FzZb%252Fg%252BUqIxpDkmli14%253D&amp;asb2=Hktu5DsgNibM5RSm4eiwXaJQU18OwLj4EgOqW9SDUVZbXQx6xvgmarMnHcSrtee4&amp;ectx=1&amp;keywords=makfa+%D0%BA%D1%80%D1%83%D0%BF%D0%B0&amp;miniapp=supermarket&amp;sh=K5xV8WJgbA</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/makfa-makaronnye-izdeliya-livingood-lg-energy-pasta-fusilli-400-g-h-3-upakovki-346647048/?asb=tk7%252F1yubIY98qg9yH6npCSVGgE67IqP1iz7mb6UKgkw%253D&amp;asb2=xKVQtw8ZU4KDTND1YUh6bDCDW6jXkLor0sCPhPz5T2QKb-ptdEZTh88KZUtTgvZe&amp;keywords=%D1%8D%D0%B4%D0%BF+energy+pasta+fusilli+400+%D0%B3%D1%80&amp;sh=K5xV8aFK4A</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/makfa-makaronnye-izdeliya-livingood-lg-energy-pasta-spaghetti-400-g-h-3-upakovki-346880201/?asb=aTQkZudSS%252BTLALFQllmrWxp0lLdD7qTh5W1sm2XIhHE%253D&amp;asb2=K5o4Qil_c712FovVJ2jYd53VO2186vbCL3AxWTF0Zz1hUeOO_WmSQOkrmyIcHh_c&amp;keywords=%D1%8D%D0%B4%D0%BF+energy+pasta+spaghetti+400+%D0%B3%D1%80&amp;sh=K5xV8S24rQ</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/hlopya-makfa-5-zlaka-400g-567098277/?asb=1HnYX6xNJH7QyIgAu%252FZoJ940fQbo03Y%252FBlnVaMWUufw%253D&amp;asb2=663ki1ENpWYcyx7yXyOlmAPcrCGX9sr09Gw1i_iHAnNomvcCzjhI0IJyCmo__9jq&amp;keywords=%D0%BC%D0%B0%D0%BA%D1%84%D0%B0+%D1%85%D0%BB%D0%BE%D0%BF%D1%8C%D1%8F+5+%D0%B7%D0%BB%D0%B0%D0%BA%D0%BE%D0%B2&amp;sh=K5xV8RbIlw</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/hlopya-makfa-4-zlaka-400g-594443440/?asb=QVdKTO0kw%252Bagr%252FM0%252BhSZFVpYn0moMe2Xi17msVoOiKU%253D&amp;asb2=4r-uMr_UxSeAYyPJ6N35cBFF27WbYoOcN5aClTTYulbFq5QYIY3-TeWpuw7IcmeI&amp;keywords=%D0%BC%D0%B0%D0%BA%D1%84%D0%B0+4+%D0%B7%D0%BB%D0%B0%D0%BA%D0%B0&amp;sh=K5xV8d9UZQ</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/makfa-hlopya-gerkules-traditsionnyy-400-g-140800403/?asb=LzEoiRP2NAQrp6eCvRK1c03tT34XWEoWq4aTvr0Dp5I%253D&amp;asb2=mKnsWj_X2qeEAjjRW-Be4wLchkURoJiIudw8darRG05zgH28TrhUkip_HAeguJxX&amp;keywords=%D0%BC%D0%B0%D0%BA%D1%84%D0%B0+%D0%BE%D0%B2%D1%81%D1%8F%D0%BD%D1%8B%D0%B5+%D1%85%D0%BB%D0%BE%D0%BF%D1%8C%D1%8F&amp;sh=K5xV8YTjMg</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/makfa-hlopya-ovsyanye-400-g-140800405/?asb=yNQoNTidBbmxy%252Fld52EuHlsr35GUW2IGNRRwqQK%252Bi2M%253D&amp;asb2=WTCImwarosJtcJ3J-KE7WLeUov9TnoNG9NcgAg1AVOUmtAMDKKhnn7sEqAjITDQg&amp;keywords=%D0%BC%D0%B0%D0%BA%D1%84%D0%B0+%D0%BE%D0%B2%D1%81%D1%8F%D0%BD%D1%8B%D0%B5+%D1%85%D0%BB%D0%BE%D0%BF%D1%8C%D1%8F&amp;sh=K5xV8f4DhA</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/biomio-ekologichnyy-stiralnyy-poroshok-bio-color-dlya-tsvetnogo-belya-s-ekstraktom-hlopka-1-5-kg-26431434/?asb=bZCupQ8IdpnGmQFdk98sG0P4ufLPiksLAicJYJ6bdpk%253D&amp;asb2=GGTFjDxVc8eBJlZ2x5vRPpxUpnXzgie398QpoB8QwtZCIQvWc-82V-Dj6GwBywfx&amp;keywords=BioMio&amp;sh=K5xV8VoUEA</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/biomio-ekologichnyy-stiralnyy-poroshok-bio-white-dlya-belogo-belya-s-ekstraktom-hlopka-1-5-kg-26431433/?asb=cmwryBtTNsRird5eB1cjuU7LGb0cUOssYAIxIh8ml4c%253D&amp;asb2=mM-Zt2gdoCAqxU7tsAZQWQhb474q9CKyHO-M6lp1byYUioLKBIkvW5wkFlkAgvty&amp;keywords=BioMio&amp;sh=K5xV8TlF7A</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/biomio-ekologichnyy-gel-dlya-stirki-delikatnyh-tkaney-bio-sensitive-bez-zapaha-1-5-l-147577588/?asb=22LIFV1eqj7pNFHU%252BvnWAiFlJa3RpdQGOpE6QsIXFdA%253D&amp;asb2=LX3XmwM8moWL3idwha9Jpr5XqPpcp0C9zXLOTRUkJPR1QErgCUkxeBtbRjEkScjk&amp;keywords=BioMio&amp;sh=K5xV8Wo_GQ</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/biomio-ekologichnyy-gel-i-pyatnovyvoditel-bio-2-in-1-dlya-stirki-belya-1-5-l-147577582/?asb=tUDKc6hYZaVakHTUdbVHC4%252FTtRC%252B8k5B7FIUO8GwmL8%253D&amp;asb2=RLX6iLWCN6n6juisoULokoCF9bzhDpnSWFhB0U0BdIKsFJplNwdgPtBb36ykoEum&amp;keywords=BioMio&amp;sh=K5xV8focKw</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/biomio-ekologichnyy-konditsioner-dlya-belya-bio-soft-s-efirnym-maslom-evkalipta-kontsentrat-1-l-147577592/?asb=Y8H9FZgUwygeK7d1s7X0Wf3YvcSlsnoroKAYoMNnUi4%253D&amp;asb2=HgINcNzk-iW36-PE6DtLBJfq19iNp0j7oXdasXXmTSdhrBmF7HosU1dTWXnNJN6s&amp;keywords=BioMio&amp;sh=K5xV8UCBKQ</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/mylo-hozyaystvennoe-biomio-bio-soap-pyatnovyvoditel-ekologichnoe-200-g-2-sht-208541230/?asb=NVSzmxaSi%252FfOwTMoxj%252Fa0%252FWbnNxOddeHToZLDF0ko2Y%253D&amp;asb2=mT1fnfKCSWtbVuVYsqn5GgddhvJUJBzTwE8VemvSI_MApqXT7-ZdEPRmL88rISsl&amp;keywords=BioMio+%D0%BC%D1%8B%D0%BB%D0%BE&amp;sh=K5xV8bd64w</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/biomio-ekologichnoe-sredstvo-dlya-mytya-posudy-ovoshchey-i-fruktov-bio-care-bez-zapaha-450-ml-26431422/?asb=BfXewQqRe4Fc4CPx5gmm0LCvF%252BF5oUF9p0q3mQdKPS8%253D&amp;asb2=OTzaWF9QMqlJqaja8rPZfcJCUiPFZf3n5qUfHLQWY0kPN5cNm-_QofeNC6mOkApW&amp;keywords=BioMio&amp;sh=K5xV8Sd_Vg</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/biomio-ekologichnoe-sredstvo-dlya-mytya-posudy-ovoshchey-i-fruktov-bio-care-antibakterialnoe-26431428/?asb=irCU9OWnZyOBdTo0Rx%252F5L4tfJ6s8Y28UOgw%252BUq0XLEc%253D&amp;asb2=8RgQf6_DaRKfkLX5Xu9FEPzEZ_gQXf8y8r5_nL1oMNdpKYp9tAikrHaiU6HM4MS1&amp;keywords=biomio+%D1%81%D1%80%D0%B5%D0%B4%D1%81%D1%82%D0%B2%D0%BE+%D0%B4%D0%BB%D1%8F+%D0%BC%D1%8B%D1%82%D1%8C%D1%8F+%D0%BF%D0%BE%D1%81%D1%83%D0%B4%D1%8B&amp;sh=K5xV8QrQCQ</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/balzam-dlya-mytya-detskoy-posudy-biomio-baby-bio-balm-romashka-i-ilang-ilang-170280096/?asb=rNnP76YFVaqXpAzGeE5mRBm8YsKrUyfxOG9fJ37DIrU%253D&amp;asb2=aidPw712h7uNHszB1FCx_ZZ21U2Rm_sCUpYr6FH7YUNR73FusvR423pmvaZ1rknN&amp;keywords=biomio+%D0%B1%D0%B0%D0%BB%D1%8C%D0%B7%D0%B0%D0%BC&amp;sh=K5xV8cbhmg</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/ekologichnaya-pena-biomio-bio-foam-dlya-mytya-posudy-s-efirnym-maslom-lemongrassa-350ml-355651498/?asb=yGIS1N63Ft2Z2dFotMj1lHdVxrLVUfFrGf66WRAw9kw%253D&amp;asb2=GcPeg_fCOuLf_-bRpDxd4sPHkTrMpT6yX0a3t5WTToAsBs5X1ufgLKOXYPGFCfL3&amp;keywords=biomio+%D0%BF%D0%B5%D0%BD%D0%B0&amp;sh=K5xV8QlqOw</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/biomio-ekologichnye-tabletki-dlya-posudomoechnoy-mashiny-7-v-1-bio-total-s-efirnym-maslom-evkalipta-26431435/?asb=w1BvSPg5rQA3pPDpjw9H1bv5tsb6pkpribgq7BO9Qls%253D&amp;asb2=05-s2w7wTtFw6xnSvSRu2Ckz2qWzoKe95Y2ALqjIbX95TsRFRgxg6WwXQDH7p95q&amp;keywords=biomio+%D1%82%D0%B0%D0%B1%D0%BB%D0%B5%D1%82%D0%BA%D0%B8&amp;sh=K5xV8f0SWA</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/sol-dlya-posudomoechnyh-mashin-biomio-bio-salt-1-kg-165148319/?asb=GEbzgAAJb7PWss7m4BpCyjEydOSjrg6GtwTnAWyw%252BAE%253D&amp;asb2=EKCf1myn9KZvbOlNmUzCrW71RSS8CUSQblZz4LYPxjSEKd70wpNoON62HpdwJyGa&amp;keywords=biomio+%D1%81%D0%BE%D0%BB%D1%8C&amp;sh=K5xV8emTjw</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/opolaskivatel-dlya-posudomoechnoy-mashiny-biomio-bio-rinse-ekologichnyy-750-ml-315439203/?asb=EyjlqyZvnx%252Fv6YW6Cldj%252BtKOw527FhR0fu7oGhOu9JY%253D&amp;asb2=IdTQAbZI3kBHVWEMt9ixob08wsf205z4JxrvVFOW_dzNNyK8yYzx6g5R00NEoCfq&amp;keywords=biomio+%D0%BE%D0%BF%D0%BE%D0%BB%D0%B0%D1%81%D0%BA%D0%B8%D0%B2%D0%B0%D1%82%D0%B5%D0%BB%D1%8C+%D0%B4%D0%BB%D1%8F+%D0%BF%D0%BE%D1%81%D1%83%D0%B4%D0%BE%D0%BC%D0%BE%D0%B5%D1%87%D0%BD%D0%BE%D0%B9+%D0%BC%D0%B0%D1%88%D0%B8%D0%BD%D1%8B&amp;sh=K5xV8U_IBw</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/universalnoe-chistyashchee-sredstvo-biomio-bio-multi-purpose-cleaner-ekologichnoe-sprey-bez-zapaha-289873990/?asb=k3LQf1S7YIYGFhxG8IDR2nAzAYps5jxJQ4y7kX8GWhY%253D&amp;asb2=-XYbY0sgY1HMHz1neWTreel3ZVzPIHCH_G9oCUTGlYhPm3gMBZC7bsJKYRPkGOa8&amp;keywords=biomio+Bio-cleaner&amp;sh=K5xV8TJ44w</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/biomio-ekologichnoe-chistyashchee-sredstvo-dlya-stekol-zerkal-plastika-bio-glass-cleaner-bez-zapaha-147577585/?asb=ANuoAosNi%252Bknovdfv9luHM9Sin%252Bpnd45yJY8Gv3YuvE%253D&amp;asb2=sMR7X72eHTB0GnG_bU8fw2yJorxmRi-zKcUB38Jnrnrkbn5uRoD28GJl5b1ei1ed&amp;keywords=biomio+Bio-cleaner+glass&amp;sh=K5xV8WF6IA</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/biomio-bio-floor-cleaner-antibakterialnoe-chistyashchee-sredstvo-dlya-pola-s-efirnym-maslom-melissy-147577584/?asb=c%252Fwb%252F6iVzi%252F8uH1fqd%252F%252FisO87e2KzzsWvCL8bVoRv%252B8%253D&amp;asb2=_8h8FWM7V20uoj3Yi6sFXNA2_8xh3Aoz6QaVaLGIhGrm_JazBKBVOTYXzT6IQGTP&amp;keywords=biomio+Bio-cleaner+floor&amp;sh=K5xV8R5_HA</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/biomio-ekologichnoe-antibakterialnoe-chistyashchee-sredstva-dlya-vannoy-komnaty-bio-bathroom-cleaner-147577583/?asb=kd6p7lK%252Fz2VmPOl%252F4lwZsFdvoF%252Bm6W9fO6Yg0S8Gdds%253D&amp;asb2=grtl16_RdqBdHO4b6D7McJVUz6TJmJnx9Pp4coHcSweiW6awYgOtx5bOHDuBExgH&amp;keywords=biomio+Bio+bathroom&amp;sh=K5xV8ZAymg</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/splat-professional-zubnaya-pasta-white-plus-otbelivanie-plyus-40-ml-27937119/?asb=Xxl1pSw%252B%252FeJmQN%252FuVm58WRUQYKEOmDER%252BOBBvbNbVDw%253D&amp;asb2=bvRoC0YQ10NsSXnzOpatXscaNdUjrreTsq_AhxfJm2d7U42ZzD_w0k_8oZ01vDMH&amp;keywords=splat+white+plus&amp;sh=K5xV8V2cjQ</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/zubnaya-pasta-splat-professional-biocalcium-biokaltsiy-100-ml-14125564/?asb=X5YvIVPDHuKAciDQIUZXTzvT4lcJl71F3sLRaALXb%252B8%253D&amp;asb2=rvFC2EHCSdpTAZPdRYcW09dj_ASpJRhV7dj5pJg8GKtXOOOpRaGKi-Nhrj7mEd1I&amp;keywords=splat&amp;sh=K5xV8QyVJw</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/zubnaya-pasta-splat-professional-sensitive-sensitiv-dlya-snizheniya-chuvstvitelnosti-zubov-i-208799454/?asb=%252FwxRy%252BfsXF%252B5JEIqQ%252B8kXuLqqEHTBaXa3Lf3qdm99%252BM%253D&amp;asb2=d8jXdkPgORvEqiQEaLR7HzMomh3WOWb5Ny1AFC9K3WbNfm6LAUVxICMtJTUuc_LO&amp;keywords=splat+sensitive&amp;sh=K5xV8eTg8w</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/zubnaya-pasta-splat-professional-medical-herbs-lechebnye-travy-100-ml-14125567/?asb=mTwdbMZ0cveafY6Li7JdP6hAsMKkqs9oQwidYtIA4pI%253D&amp;asb2=W6Eo0QGXkI_bALqwR64MkTwVrz6DUg0tR8Lq3hYWcprGiHTDGlpOqhSfstlzC1XH&amp;keywords=splat+%D0%BB%D0%B5%D1%87%D0%B5%D0%B1%D0%BD%D1%8B%D0%B5+%D1%82%D1%80%D0%B0%D0%B2%D1%8B&amp;sh=K5xV8WiPvA</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/otbelivayushchaya-antibakterialnaya-zubnaya-pasta-splat-ultracomplex-kompleksnyy-uhod-bez-ftora-dlya-14125571/?asb=lYZ4RqmYrtCG%252FO0%252FLqHTM2lGjsFaO9xDnEKFeYJIXhM%253D&amp;asb2=VaMDvyB73FqC6BAYcbk2gLwGTNvfx9Kj-iGE7x4RfWwTzH_BR41cD_XQTRYnwwqU&amp;keywords=splat+%D1%83%D0%BB%D1%8C%D1%82%D1%80%D0%B0%D0%BA%D0%BE%D0%BC%D0%BF%D0%BB%D0%B5%D0%BA%D1%81&amp;sh=K5xV8ZeEaQ</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/splat-zubnaya-pasta-detskaya-zemlyanika-vishnya-antibakterialnaya-ot-2-do-6-let-50-ml-135516747/?asb=h1D5JTMGFWNekO1bcdqZu3v%252FUfxECVcSb69tZdHMIl0%253D&amp;asb2=_Y-Rt7rTFDCDVRNax0xdanb9H6m7zohu3S6eN3zRWVFEIV3MOcb6-sgIDB-c9xpL&amp;keywords=splat+%D0%B7%D0%B5%D0%BC%D0%BB%D1%8F%D0%BD%D0%B8%D0%BA%D0%B0&amp;sh=K5xV8W4wMw</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/splat-zubnaya-pasta-detskaya-junior-babl-gam-73-g-139577058/?asb=VuG1XMYTtJYxpJu%252B9h1qAil9hafd1O%252FLrM%252BRJbILv24%253D&amp;asb2=3tM1OwFXZyv6AVxsxmEalsyPrDjRXrHBX95Wi5hD4A1-UTNa3NtrdkM-Qbwjxdbv&amp;keywords=splat+%D0%B1%D0%B0%D0%B1%D0%BB+%D0%B3%D0%B0%D0%BC&amp;sh=K5xV8STMSQ</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/zubnaya-shchetka-splat-professional-ultra-sensitive-soft-5-sht-340184934/?asb=gzJC7W8iaNl%252BJVsZieyU4WYirVovz81ss5%252BWphlNy6k%253D&amp;asb2=O6J6OmUt4R8fvF0RwE2aqjOV7sdMGrWTUJ5zDuzKHFg8e8PF9I-fcyHFzPYoBaZJ&amp;keywords=SPLAT+ULTRA+SENSITIVE+Soft+%2F+%D0%A3%D0%9B%D0%AC%D0%A2%D0%A0%D0%90+%D0%A1%D0%95%D0%9D%D0%A1%D0%98%D0%A2%D0%98%D0%92+%D0%9C%D1%8F%D0%B3%D0%BA%D0%B0%D1%8F&amp;sh=K5xV8RAfcw</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/zubnaya-shchetka-splat-professional-clinic-care-medium-srednyaya-zelenaya-235409443/?asb=R2T9HCYrzrEbZMOx8WfcfJxsK0IAZUeqP7c%252FGW8TJok%253D&amp;asb2=-EF55Kv6-d8kJIWDy6FM_ZrLgpGOlRy8eB88GMbRhzyNvVFKAcHRIOrASA8ptyeV&amp;keywords=splat+clinic+care+medium+%D1%81%D1%80%D0%B5%D0%B4%D0%BD%D1%8F%D1%8F&amp;sh=K5xV8awfGg</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/zubnaya-shchetka-splat-professional-ultra-complete-srednyaya-zheltaya-235409461/?asb=pesXgDzYf9Xck73dwSMpQJ%252BUHZugCL7scFjDyKECAfw%253D&amp;asb2=a1Qp2TcmPLdGllgch_tBhAN4D6-wZahgpkuYX-2DMdHwhc2uaj0iE7bSyZnpZmW3&amp;keywords=SPLAT+ULTRA+COMPLETE+Medium+%2F+%D0%A3%D0%9B%D0%AC%D0%A2%D0%A0%D0%90+%D0%9A%D0%9E%D0%9C%D0%9F%D0%9B%D0%98%D0%A2+%D0%A1%D1%80%D0%B5%D0%B4%D0%BD%D1%8F%D1%8F&amp;sh=K5xV8Vb3rA</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/splat-zubnaya-shchetka-whitening-otbelivayushchaya-srednyaya-v-assortimente-143769283/?asb=k8hNW3tRj3ltAqfp70pXdzagMTX6r6BZQ2%252BVOnpnUaE%253D&amp;asb2=CrIxaOnvXX-DcoFeIheyXez_jSPORS81f3-OLxFZTAu3gCVZWTfMZICjyOLNE2Cb&amp;keywords=SPLAT+WHITENING+Medium+%2F+%D0%9E%D0%A2%D0%91%D0%95%D0%9B%D0%98%D0%92%D0%90%D0%AE%D0%A9%D0%90%D0%AF+%D0%A1%D1%80%D0%B5%D0%B4%D0%BD%D1%8F%D1%8F+%28%D0%BF%D1%80%D0%BE%D0%B8%D0%B7%D0%B2%D0%BE%D0%B4%D1%81%D1%82%D0%B2%D0%BE+%D0%A0%D0%A4%29&amp;sh=K5xV8UYvyQ</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/splat-zubnaya-shchetka-whitening-otbelivayushchaya-zhestkaya-tsvet-zelenyy-143769280/?asb=MJCt3hB%252BFfg8M7AMX%252FGVdKpc8FdYnEKPmCjaWvvGFLM%253D&amp;asb2=7pOMfFZKrc4x-7dZ5S_Wqxe5Gq2_tySKVoLsBztaCbw8Ni4X4nP_XW5YF7fI45vr&amp;keywords=SPLAT+WHITENING+Hard+%2F+%D0%9E%D0%A2%D0%91%D0%95%D0%9B%D0%98%D0%92%D0%90%D0%AE%D0%A9%D0%90%D0%AF+%D0%96%D1%91%D1%81%D1%82%D0%BA%D0%B0%D1%8F+%28%D0%BF%D1%80%D0%BE%D0%B8%D0%B7%D0%B2%D0%BE%D0%B4%D1%81%D1%82%D0%B2%D0%BE+%D0%A0%D0%A4%29&amp;sh=K5xV8WtidA</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/zubnaya-shchetka-biomed-mineral-hard-490277279/?asb=NyzKxgfl3Qaf38PkCU5P7pLd8rE4f18yjDB5t977sHE%253D&amp;asb2=7OH_NG15r7RfUdXzj08z-ICCZW4kVyiCJjXD5QYilKqcYPf_w_XfQC_yFGoMET9p&amp;keywords=%D0%97%D1%83%D0%B1%D0%BD%D0%B0%D1%8F+%D1%89%D0%B5%D1%82%D0%BA%D0%B0+BIOMED+MINERAL+HARD&amp;sh=K5xV8RFBtw</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/zubnaya-shchetka-splat-kids-detskaya-myagkaya-1204-02-02-zheltyy-163606532/?asb=z0Lp%252FwU0EUpPydg71yEWa7QkltiYwgWv9swvBs3JpKQ%253D&amp;asb2=L-LG5mq2bZNmoJh4nCy3g8ofRoo5H64-UDeJkjx7IihR3tEgWcrBcPGkIKOCdem7&amp;keywords=SPLAT+KIDS+%D0%B4%D0%B5%D1%82%D1%81%D0%BA%D0%B0%D1%8F+%D0%B7%D1%83%D0%B1%D0%BD%D0%B0%D1%8F+%D1%89%D0%B5%D1%82%D0%BA%D0%B0&amp;sh=K5xV8dPCPA</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/splat-junior-zubnaya-shchetka-s-ionami-serebra-myagkie-shchetinki-dlya-detey-ot-4-let-biryuzovyy-163606529/?asb=b7I2oJk9tDszk4eyfaHbXbTla6gO1HQnTdtaNSB0D54%253D&amp;asb2=_mB9mYF1UDlpb-UFtx9N8X1Ktv-MyBJ8KOq7RLQgkmW65BKi2eHtdXrXHeR5oOmg&amp;keywords=SPLAT+JUNIOR+%D0%B4%D0%B5%D1%82%D1%81%D0%BA%D0%B0%D1%8F+%D0%B7%D1%83%D0%B1%D0%BD%D0%B0%D1%8F+%D1%89%D0%B5%D1%82%D0%BA%D0%B0&amp;sh=K5xV8aVbbQ</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/brest-litovsk-maslo-sladko-slivochnoe-nesolenoe-82-5-180-g-145923184/?asb=zKHL5xgxfT99qqDSwhkl0%252BM9sbMai2TqZFnyKSsgAdo%253D&amp;asb2=tW7AUVLOvTmJeiz_V4tx1BXh8yTgJraTyb_pT71juaFxL-XxUCjDvd0NC-bxrrTg&amp;ectx=1&amp;keywords=%D0%B1%D1%80%D0%B5%D1%81%D1%82+%D0%BB%D0%B8%D1%82%D0%BE%D0%B2%D1%81%D0%BA&amp;miniapp=supermarket&amp;sh=K5xV8Wnabw</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/vatnye-diski-aura-beauty-s-verevochkoy-120-sht-324469602/?asb=bAcQm3t72e5wO1oiqka9MTO02J3OU5BVMCRhN75Op%252BQ%253D&amp;asb2=q__UVChAFjnUAOg-5XA0kEY4U0PLAQ9mzXcn7JryVjc50pB5B6MSRdbMHDeEXIJx&amp;keywords=aura+%D0%B2%D0%B0%D1%82%D0%BD%D1%8B%D0%B5+%D0%B4%D0%B8%D1%81%D0%BA%D0%B8+120+%D0%BF%D1%8D+%D1%81+%D0%B2%D0%B5%D1%80%D0%B5%D0%B2%D0%BE%D1%87%D0%BA%D0%BE%D0%B9+120%D1%88%D1%82&amp;sh=K5xV8UHp-g</t>
+  </si>
+  <si>
+    <t>https://www.ozon.ru/product/vatnye-palochki-ya-samaya-original-4607068620957-300-sht-202009511/?asb=zDcRJhsdcxXYYrvPRyPmLZlWOoRWZrX5AMcj6tKOHsM%253D&amp;asb2=lXgqXQe7SBYSfbT3Om9mz4FUS_K29jQErCfD693gTAHsE4Q6Tli4v8AMPyyOoEb-&amp;keywords=%D1%8F+%D1%81%D0%B0%D0%BC%D0%B0%D1%8F+%D0%B2%D0%B0%D1%82%D0%BD%D1%8B%D0%B5+%D0%B4%D0%B8%D1%81%D0%BA%D0%B8+original+%D0%BF%D1%8D+100%D1%88%D1%82&amp;sh=K5xV8bOvDA</t>
   </si>
 </sst>
 </file>
@@ -1245,7 +1569,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1261,6 +1585,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1390,7 +1720,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1426,6 +1756,12 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -1741,10 +2077,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF1A69E3-A9E5-424F-8F16-B76B324D2ACC}">
-  <dimension ref="D5:M115"/>
+  <dimension ref="D5:M153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F75" sqref="F75"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1770,7 +2106,7 @@
         <v>106</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="H6" s="11" t="s">
         <v>107</v>
@@ -1779,13 +2115,13 @@
         <v>108</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>187</v>
+        <v>158</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>235</v>
+        <v>204</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>280</v>
+        <v>247</v>
       </c>
       <c r="M6" s="13" t="s">
         <v>1</v>
@@ -1802,16 +2138,19 @@
         <v>110</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>141</v>
+        <v>134</v>
+      </c>
+      <c r="I7" t="s">
+        <v>423</v>
       </c>
       <c r="J7" t="s">
-        <v>188</v>
+        <v>159</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>236</v>
+        <v>205</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>380</v>
+        <v>346</v>
       </c>
       <c r="M7" s="5" t="s">
         <v>3</v>
@@ -1825,19 +2164,22 @@
         <v>4</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>320</v>
+        <v>286</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>323</v>
+        <v>289</v>
       </c>
       <c r="H8" t="s">
-        <v>358</v>
+        <v>324</v>
+      </c>
+      <c r="I8" t="s">
+        <v>424</v>
       </c>
       <c r="J8" t="s">
-        <v>333</v>
+        <v>299</v>
       </c>
       <c r="K8" t="s">
-        <v>237</v>
+        <v>206</v>
       </c>
       <c r="M8" s="6" t="s">
         <v>4</v>
@@ -1851,23 +2193,23 @@
         <v>5</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="9" t="s">
         <v>109</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>313</v>
+        <v>279</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>189</v>
+        <v>160</v>
       </c>
       <c r="K9" t="s">
-        <v>238</v>
+        <v>207</v>
       </c>
       <c r="L9" t="s">
-        <v>281</v>
+        <v>248</v>
       </c>
       <c r="M9" s="5" t="s">
         <v>5</v>
@@ -1883,16 +2225,16 @@
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="I10" s="9" t="s">
-        <v>111</v>
+        <v>425</v>
       </c>
       <c r="J10" t="s">
-        <v>190</v>
+        <v>161</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>239</v>
+        <v>208</v>
       </c>
       <c r="L10" s="9" t="s">
-        <v>381</v>
+        <v>347</v>
       </c>
       <c r="M10" s="5" t="s">
         <v>6</v>
@@ -1906,23 +2248,23 @@
         <v>8</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G11" s="9"/>
       <c r="H11" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="I11" t="s">
-        <v>157</v>
+        <v>426</v>
       </c>
       <c r="J11" t="s">
-        <v>191</v>
+        <v>162</v>
       </c>
       <c r="K11" t="s">
-        <v>240</v>
+        <v>209</v>
       </c>
       <c r="L11" t="s">
-        <v>382</v>
+        <v>348</v>
       </c>
       <c r="M11" s="5" t="s">
         <v>8</v>
@@ -1936,19 +2278,22 @@
         <v>9</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>142</v>
+        <v>135</v>
+      </c>
+      <c r="I12" t="s">
+        <v>427</v>
       </c>
       <c r="J12" t="s">
-        <v>192</v>
+        <v>163</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>241</v>
+        <v>210</v>
       </c>
       <c r="L12" s="9" t="s">
-        <v>383</v>
+        <v>349</v>
       </c>
       <c r="M12" s="5" t="s">
         <v>9</v>
@@ -1963,8 +2308,11 @@
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
+      <c r="I13" t="s">
+        <v>428</v>
+      </c>
       <c r="J13" t="s">
-        <v>338</v>
+        <v>304</v>
       </c>
       <c r="M13" s="5" t="s">
         <v>10</v>
@@ -1979,19 +2327,19 @@
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9" t="s">
-        <v>324</v>
+        <v>290</v>
       </c>
       <c r="H14" t="s">
-        <v>359</v>
+        <v>325</v>
       </c>
       <c r="I14" t="s">
-        <v>158</v>
+        <v>429</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>335</v>
+        <v>301</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>242</v>
+        <v>211</v>
       </c>
       <c r="L14" s="9"/>
       <c r="M14" s="5" t="s">
@@ -2006,19 +2354,19 @@
         <v>13</v>
       </c>
       <c r="F15" t="s">
-        <v>321</v>
+        <v>287</v>
       </c>
       <c r="G15" t="s">
-        <v>325</v>
+        <v>291</v>
       </c>
       <c r="H15" t="s">
-        <v>360</v>
+        <v>326</v>
       </c>
       <c r="I15" t="s">
-        <v>159</v>
+        <v>430</v>
       </c>
       <c r="J15" t="s">
-        <v>336</v>
+        <v>302</v>
       </c>
       <c r="M15" s="5" t="s">
         <v>13</v>
@@ -2032,16 +2380,16 @@
         <v>15</v>
       </c>
       <c r="G16" t="s">
-        <v>326</v>
+        <v>292</v>
       </c>
       <c r="I16" t="s">
-        <v>160</v>
+        <v>431</v>
       </c>
       <c r="J16" t="s">
-        <v>334</v>
+        <v>300</v>
       </c>
       <c r="L16" t="s">
-        <v>384</v>
+        <v>350</v>
       </c>
       <c r="M16" s="5" t="s">
         <v>15</v>
@@ -2055,10 +2403,13 @@
         <v>16</v>
       </c>
       <c r="H17" t="s">
-        <v>361</v>
+        <v>327</v>
+      </c>
+      <c r="I17" t="s">
+        <v>432</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>339</v>
+        <v>305</v>
       </c>
       <c r="K17" s="9"/>
       <c r="L17" s="9"/>
@@ -2076,10 +2427,13 @@
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
       <c r="H18" t="s">
-        <v>362</v>
+        <v>328</v>
+      </c>
+      <c r="I18" t="s">
+        <v>433</v>
       </c>
       <c r="J18" t="s">
-        <v>193</v>
+        <v>377</v>
       </c>
       <c r="L18" s="9"/>
       <c r="M18" s="5" t="s">
@@ -2093,8 +2447,11 @@
       <c r="E19" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="I19" t="s">
+        <v>434</v>
+      </c>
       <c r="J19" t="s">
-        <v>194</v>
+        <v>164</v>
       </c>
       <c r="M19" s="5" t="s">
         <v>18</v>
@@ -2109,8 +2466,11 @@
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
+      <c r="I20" t="s">
+        <v>435</v>
+      </c>
       <c r="J20" t="s">
-        <v>340</v>
+        <v>306</v>
       </c>
       <c r="M20" s="5" t="s">
         <v>19</v>
@@ -2123,11 +2483,14 @@
       <c r="E21" s="5" t="s">
         <v>20</v>
       </c>
+      <c r="I21" t="s">
+        <v>436</v>
+      </c>
       <c r="J21" t="s">
-        <v>337</v>
+        <v>303</v>
       </c>
       <c r="K21" t="s">
-        <v>243</v>
+        <v>212</v>
       </c>
       <c r="M21" s="5" t="s">
         <v>20</v>
@@ -2141,14 +2504,17 @@
         <v>22</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G22" s="9"/>
+      <c r="I22" t="s">
+        <v>437</v>
+      </c>
       <c r="J22" t="s">
-        <v>195</v>
+        <v>165</v>
       </c>
       <c r="K22" t="s">
-        <v>244</v>
+        <v>213</v>
       </c>
       <c r="M22" s="5" t="s">
         <v>22</v>
@@ -2159,13 +2525,19 @@
       <c r="E23" s="5"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
+      <c r="I23" t="s">
+        <v>438</v>
+      </c>
       <c r="M23" s="5"/>
     </row>
     <row r="24" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D24" s="2"/>
       <c r="E24" s="3"/>
+      <c r="I24" t="s">
+        <v>439</v>
+      </c>
       <c r="J24" t="s">
-        <v>341</v>
+        <v>307</v>
       </c>
       <c r="M24" s="3"/>
     </row>
@@ -2179,13 +2551,13 @@
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
       <c r="I25" t="s">
-        <v>161</v>
+        <v>440</v>
       </c>
       <c r="J25" t="s">
-        <v>196</v>
+        <v>166</v>
       </c>
       <c r="K25" t="s">
-        <v>316</v>
+        <v>282</v>
       </c>
       <c r="M25" s="5" t="s">
         <v>24</v>
@@ -2199,13 +2571,13 @@
         <v>25</v>
       </c>
       <c r="J26" t="s">
-        <v>197</v>
+        <v>167</v>
       </c>
       <c r="K26" t="s">
-        <v>317</v>
+        <v>283</v>
       </c>
       <c r="L26" t="s">
-        <v>282</v>
+        <v>249</v>
       </c>
       <c r="M26" s="5" t="s">
         <v>25</v>
@@ -2219,11 +2591,11 @@
         <v>26</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G27" s="9"/>
       <c r="J27" t="s">
-        <v>198</v>
+        <v>168</v>
       </c>
       <c r="M27" s="5" t="s">
         <v>26</v>
@@ -2236,6 +2608,9 @@
       <c r="E28" s="5" t="s">
         <v>28</v>
       </c>
+      <c r="I28" t="s">
+        <v>150</v>
+      </c>
       <c r="M28" s="5" t="s">
         <v>28</v>
       </c>
@@ -2281,11 +2656,14 @@
         <v>33</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G32" s="9"/>
+      <c r="I32" t="s">
+        <v>441</v>
+      </c>
       <c r="L32" t="s">
-        <v>283</v>
+        <v>250</v>
       </c>
       <c r="M32" s="5" t="s">
         <v>33</v>
@@ -2298,6 +2676,9 @@
       <c r="E33" s="8" t="s">
         <v>35</v>
       </c>
+      <c r="I33" t="s">
+        <v>442</v>
+      </c>
       <c r="M33" s="8" t="s">
         <v>35</v>
       </c>
@@ -2310,17 +2691,20 @@
         <v>36</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G34" s="9"/>
+      <c r="I34" t="s">
+        <v>444</v>
+      </c>
       <c r="J34" t="s">
-        <v>306</v>
+        <v>272</v>
       </c>
       <c r="K34" t="s">
-        <v>245</v>
+        <v>214</v>
       </c>
       <c r="L34" t="s">
-        <v>284</v>
+        <v>251</v>
       </c>
       <c r="M34" s="5" t="s">
         <v>36</v>
@@ -2333,11 +2717,14 @@
       <c r="E35" s="5" t="s">
         <v>37</v>
       </c>
+      <c r="I35" t="s">
+        <v>443</v>
+      </c>
       <c r="J35" t="s">
-        <v>307</v>
+        <v>273</v>
       </c>
       <c r="L35" t="s">
-        <v>315</v>
+        <v>281</v>
       </c>
       <c r="M35" s="5" t="s">
         <v>37</v>
@@ -2351,10 +2738,10 @@
         <v>39</v>
       </c>
       <c r="J36" t="s">
-        <v>308</v>
+        <v>274</v>
       </c>
       <c r="K36" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="M36" s="5" t="s">
         <v>39</v>
@@ -2367,11 +2754,8 @@
       <c r="E37" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="I37" t="s">
-        <v>162</v>
-      </c>
       <c r="J37" t="s">
-        <v>309</v>
+        <v>275</v>
       </c>
       <c r="M37" s="5" t="s">
         <v>40</v>
@@ -2390,14 +2774,14 @@
         <v>42</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G39" s="9"/>
       <c r="J39" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="K39" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="M39" s="5" t="s">
         <v>42</v>
@@ -2411,14 +2795,14 @@
         <v>43</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G40" s="9"/>
       <c r="J40" t="s">
-        <v>200</v>
+        <v>170</v>
       </c>
       <c r="K40" t="s">
-        <v>248</v>
+        <v>217</v>
       </c>
       <c r="M40" s="5" t="s">
         <v>43</v>
@@ -2432,16 +2816,16 @@
         <v>44</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="J41" t="s">
-        <v>203</v>
+        <v>173</v>
       </c>
       <c r="L41" t="s">
-        <v>285</v>
+        <v>252</v>
       </c>
       <c r="M41" s="5" t="s">
         <v>44</v>
@@ -2455,13 +2839,13 @@
         <v>45</v>
       </c>
       <c r="F42" t="s">
-        <v>302</v>
+        <v>268</v>
       </c>
       <c r="J42" t="s">
-        <v>204</v>
+        <v>174</v>
       </c>
       <c r="K42" t="s">
-        <v>249</v>
+        <v>218</v>
       </c>
       <c r="M42" s="5" t="s">
         <v>45</v>
@@ -2475,7 +2859,7 @@
         <v>46</v>
       </c>
       <c r="J43" s="9" t="s">
-        <v>201</v>
+        <v>171</v>
       </c>
       <c r="K43" s="9"/>
       <c r="L43" s="9"/>
@@ -2491,11 +2875,11 @@
         <v>47</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G44" s="9"/>
       <c r="J44" t="s">
-        <v>202</v>
+        <v>172</v>
       </c>
       <c r="M44" s="5" t="s">
         <v>47</v>
@@ -2514,13 +2898,13 @@
         <v>49</v>
       </c>
       <c r="F46" t="s">
-        <v>303</v>
+        <v>269</v>
       </c>
       <c r="K46" t="s">
-        <v>251</v>
+        <v>220</v>
       </c>
       <c r="L46" t="s">
-        <v>286</v>
+        <v>253</v>
       </c>
       <c r="M46" s="5" t="s">
         <v>49</v>
@@ -2534,17 +2918,17 @@
         <v>50</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G47" s="9"/>
       <c r="J47" t="s">
-        <v>205</v>
+        <v>175</v>
       </c>
       <c r="K47" s="9" t="s">
-        <v>250</v>
+        <v>219</v>
       </c>
       <c r="L47" s="9" t="s">
-        <v>287</v>
+        <v>254</v>
       </c>
       <c r="M47" s="5" t="s">
         <v>50</v>
@@ -2570,23 +2954,20 @@
         <v>53</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G49" s="9"/>
       <c r="H49" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="I49" t="s">
-        <v>163</v>
+        <v>122</v>
       </c>
       <c r="J49" t="s">
-        <v>206</v>
+        <v>176</v>
       </c>
       <c r="K49" t="s">
-        <v>252</v>
+        <v>221</v>
       </c>
       <c r="L49" t="s">
-        <v>288</v>
+        <v>255</v>
       </c>
       <c r="M49" s="5" t="s">
         <v>53</v>
@@ -2600,17 +2981,17 @@
         <v>54</v>
       </c>
       <c r="F50" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G50" s="9"/>
       <c r="H50" t="s">
-        <v>363</v>
+        <v>329</v>
       </c>
       <c r="J50" t="s">
-        <v>207</v>
+        <v>177</v>
       </c>
       <c r="K50" t="s">
-        <v>253</v>
+        <v>222</v>
       </c>
       <c r="M50" s="5" t="s">
         <v>54</v>
@@ -2624,13 +3005,10 @@
         <v>55</v>
       </c>
       <c r="H51" t="s">
-        <v>364</v>
-      </c>
-      <c r="I51" t="s">
-        <v>163</v>
+        <v>330</v>
       </c>
       <c r="J51" s="9" t="s">
-        <v>208</v>
+        <v>178</v>
       </c>
       <c r="K51" s="9"/>
       <c r="L51" s="9"/>
@@ -2646,10 +3024,10 @@
         <v>56</v>
       </c>
       <c r="H52" t="s">
-        <v>365</v>
+        <v>331</v>
       </c>
       <c r="J52" t="s">
-        <v>209</v>
+        <v>179</v>
       </c>
       <c r="M52" s="5" t="s">
         <v>56</v>
@@ -2663,10 +3041,10 @@
         <v>58</v>
       </c>
       <c r="H53" t="s">
-        <v>366</v>
+        <v>332</v>
       </c>
       <c r="K53" t="s">
-        <v>254</v>
+        <v>223</v>
       </c>
       <c r="M53" s="5" t="s">
         <v>58</v>
@@ -2680,10 +3058,10 @@
         <v>59</v>
       </c>
       <c r="F54" t="s">
-        <v>304</v>
+        <v>270</v>
       </c>
       <c r="L54" t="s">
-        <v>289</v>
+        <v>256</v>
       </c>
       <c r="M54" s="5" t="s">
         <v>59</v>
@@ -2713,20 +3091,17 @@
         <v>63</v>
       </c>
       <c r="F57" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G57" s="9"/>
-      <c r="I57" t="s">
-        <v>165</v>
-      </c>
       <c r="J57" t="s">
-        <v>210</v>
+        <v>180</v>
       </c>
       <c r="K57" t="s">
-        <v>255</v>
+        <v>224</v>
       </c>
       <c r="L57" t="s">
-        <v>290</v>
+        <v>257</v>
       </c>
       <c r="M57" s="5" t="s">
         <v>63</v>
@@ -2740,7 +3115,7 @@
         <v>64</v>
       </c>
       <c r="J58" t="s">
-        <v>211</v>
+        <v>181</v>
       </c>
       <c r="M58" s="5" t="s">
         <v>64</v>
@@ -2754,19 +3129,19 @@
         <v>65</v>
       </c>
       <c r="F59" t="s">
-        <v>270</v>
+        <v>239</v>
       </c>
       <c r="H59" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="I59" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="J59" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="K59" s="9" t="s">
-        <v>256</v>
+        <v>225</v>
       </c>
       <c r="L59" s="9"/>
       <c r="M59" s="5" t="s">
@@ -2777,7 +3152,7 @@
       <c r="D60" s="2"/>
       <c r="E60" s="3"/>
       <c r="I60" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="M60" s="3"/>
     </row>
@@ -2789,22 +3164,22 @@
         <v>67</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G61" s="9" t="s">
-        <v>327</v>
+        <v>293</v>
       </c>
       <c r="H61" t="s">
-        <v>367</v>
+        <v>333</v>
       </c>
       <c r="I61" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="J61" s="9" t="s">
-        <v>213</v>
+        <v>183</v>
       </c>
       <c r="K61" t="s">
-        <v>257</v>
+        <v>226</v>
       </c>
       <c r="M61" s="5" t="s">
         <v>67</v>
@@ -2818,10 +3193,10 @@
         <v>68</v>
       </c>
       <c r="H62" t="s">
-        <v>368</v>
+        <v>334</v>
       </c>
       <c r="J62" t="s">
-        <v>214</v>
+        <v>184</v>
       </c>
       <c r="M62" s="5" t="s">
         <v>68</v>
@@ -2835,13 +3210,13 @@
         <v>69</v>
       </c>
       <c r="F63" t="s">
-        <v>272</v>
+        <v>241</v>
       </c>
       <c r="I63" t="s">
-        <v>168</v>
+        <v>445</v>
       </c>
       <c r="J63" t="s">
-        <v>215</v>
+        <v>185</v>
       </c>
       <c r="M63" s="5" t="s">
         <v>69</v>
@@ -2855,22 +3230,22 @@
         <v>70</v>
       </c>
       <c r="F64" s="9" t="s">
-        <v>271</v>
+        <v>240</v>
       </c>
       <c r="H64" t="s">
-        <v>369</v>
+        <v>335</v>
       </c>
       <c r="I64" t="s">
-        <v>169</v>
+        <v>446</v>
       </c>
       <c r="J64" t="s">
-        <v>216</v>
+        <v>186</v>
       </c>
       <c r="K64" t="s">
+        <v>227</v>
+      </c>
+      <c r="L64" s="9" t="s">
         <v>258</v>
-      </c>
-      <c r="L64" s="9" t="s">
-        <v>291</v>
       </c>
       <c r="M64" s="5" t="s">
         <v>70</v>
@@ -2884,25 +3259,25 @@
         <v>71</v>
       </c>
       <c r="F65" t="s">
-        <v>273</v>
+        <v>242</v>
       </c>
       <c r="G65" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="H65" t="s">
-        <v>370</v>
+        <v>336</v>
       </c>
       <c r="I65" t="s">
-        <v>170</v>
+        <v>448</v>
       </c>
       <c r="J65" t="s">
-        <v>217</v>
+        <v>187</v>
       </c>
       <c r="K65" t="s">
+        <v>228</v>
+      </c>
+      <c r="L65" t="s">
         <v>259</v>
-      </c>
-      <c r="L65" t="s">
-        <v>292</v>
       </c>
       <c r="M65" s="5" t="s">
         <v>71</v>
@@ -2916,16 +3291,16 @@
         <v>72</v>
       </c>
       <c r="G66" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="H66" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="I66" t="s">
-        <v>171</v>
+        <v>447</v>
       </c>
       <c r="J66" t="s">
-        <v>218</v>
+        <v>188</v>
       </c>
       <c r="M66" s="5" t="s">
         <v>72</v>
@@ -2939,13 +3314,13 @@
         <v>73</v>
       </c>
       <c r="F67" t="s">
-        <v>274</v>
+        <v>243</v>
       </c>
       <c r="G67" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="I67" t="s">
-        <v>172</v>
+        <v>449</v>
       </c>
       <c r="M67" s="5" t="s">
         <v>73</v>
@@ -2955,7 +3330,7 @@
       <c r="D68" s="2"/>
       <c r="E68" s="3"/>
       <c r="I68" t="s">
-        <v>173</v>
+        <v>450</v>
       </c>
       <c r="M68" s="3"/>
     </row>
@@ -2966,11 +3341,14 @@
       <c r="E69" s="5" t="s">
         <v>75</v>
       </c>
+      <c r="I69" t="s">
+        <v>451</v>
+      </c>
       <c r="J69" s="9" t="s">
-        <v>342</v>
+        <v>308</v>
       </c>
       <c r="K69" t="s">
-        <v>260</v>
+        <v>229</v>
       </c>
       <c r="M69" s="5" t="s">
         <v>75</v>
@@ -2984,19 +3362,22 @@
         <v>76</v>
       </c>
       <c r="F70" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G70" t="s">
-        <v>147</v>
+        <v>140</v>
+      </c>
+      <c r="I70" t="s">
+        <v>452</v>
       </c>
       <c r="J70" s="9" t="s">
-        <v>219</v>
+        <v>189</v>
       </c>
       <c r="K70" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="L70" s="9" t="s">
         <v>261</v>
-      </c>
-      <c r="L70" s="9" t="s">
-        <v>294</v>
       </c>
       <c r="M70" s="5" t="s">
         <v>76</v>
@@ -3010,10 +3391,7 @@
         <v>77</v>
       </c>
       <c r="I71" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="J71" t="s">
-        <v>219</v>
+        <v>453</v>
       </c>
       <c r="M71" s="5" t="s">
         <v>77</v>
@@ -3027,19 +3405,16 @@
         <v>78</v>
       </c>
       <c r="H72" t="s">
-        <v>153</v>
-      </c>
-      <c r="I72" t="s">
-        <v>175</v>
+        <v>146</v>
       </c>
       <c r="J72" t="s">
-        <v>343</v>
+        <v>309</v>
       </c>
       <c r="K72" t="s">
-        <v>318</v>
+        <v>284</v>
       </c>
       <c r="L72" t="s">
-        <v>388</v>
+        <v>354</v>
       </c>
       <c r="M72" s="5" t="s">
         <v>78</v>
@@ -3053,19 +3428,16 @@
         <v>79</v>
       </c>
       <c r="F73" t="s">
-        <v>130</v>
-      </c>
-      <c r="I73" t="s">
-        <v>176</v>
+        <v>129</v>
       </c>
       <c r="J73" t="s">
-        <v>310</v>
+        <v>276</v>
       </c>
       <c r="K73" s="9" t="s">
-        <v>262</v>
+        <v>231</v>
       </c>
       <c r="L73" s="9" t="s">
-        <v>293</v>
+        <v>260</v>
       </c>
       <c r="M73" s="5" t="s">
         <v>79</v>
@@ -3079,14 +3451,17 @@
         <v>80</v>
       </c>
       <c r="G74" t="s">
-        <v>328</v>
+        <v>294</v>
+      </c>
+      <c r="I74" t="s">
+        <v>454</v>
       </c>
       <c r="J74" s="9" t="s">
-        <v>220</v>
+        <v>190</v>
       </c>
       <c r="K74" s="9"/>
       <c r="L74" s="9" t="s">
-        <v>387</v>
+        <v>353</v>
       </c>
       <c r="M74" s="5" t="s">
         <v>80</v>
@@ -3095,32 +3470,41 @@
     <row r="75" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D75" s="4"/>
       <c r="E75" s="5"/>
+      <c r="I75" t="s">
+        <v>455</v>
+      </c>
       <c r="J75" s="9" t="s">
-        <v>345</v>
+        <v>311</v>
       </c>
       <c r="K75" s="9"/>
       <c r="L75" s="9" t="s">
-        <v>385</v>
+        <v>351</v>
       </c>
       <c r="M75" s="5"/>
     </row>
     <row r="76" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D76" s="4"/>
       <c r="E76" s="5"/>
+      <c r="I76" t="s">
+        <v>456</v>
+      </c>
       <c r="J76" s="9" t="s">
-        <v>346</v>
+        <v>312</v>
       </c>
       <c r="K76" s="9"/>
       <c r="L76" s="9" t="s">
-        <v>386</v>
+        <v>352</v>
       </c>
       <c r="M76" s="5"/>
     </row>
     <row r="77" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D77" s="4"/>
       <c r="E77" s="5"/>
+      <c r="I77" t="s">
+        <v>457</v>
+      </c>
       <c r="J77" s="9" t="s">
-        <v>347</v>
+        <v>313</v>
       </c>
       <c r="K77" s="9"/>
       <c r="L77" s="9"/>
@@ -3129,8 +3513,11 @@
     <row r="78" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D78" s="4"/>
       <c r="E78" s="5"/>
+      <c r="I78" t="s">
+        <v>458</v>
+      </c>
       <c r="J78" s="9" t="s">
-        <v>348</v>
+        <v>314</v>
       </c>
       <c r="K78" s="9"/>
       <c r="L78" s="9"/>
@@ -3139,8 +3526,11 @@
     <row r="79" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D79" s="4"/>
       <c r="E79" s="5"/>
+      <c r="I79" t="s">
+        <v>459</v>
+      </c>
       <c r="J79" s="9" t="s">
-        <v>349</v>
+        <v>315</v>
       </c>
       <c r="K79" s="9"/>
       <c r="L79" s="9"/>
@@ -3149,8 +3539,11 @@
     <row r="80" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D80" s="4"/>
       <c r="E80" s="5"/>
+      <c r="I80" t="s">
+        <v>461</v>
+      </c>
       <c r="J80" s="9" t="s">
-        <v>350</v>
+        <v>316</v>
       </c>
       <c r="K80" s="9"/>
       <c r="L80" s="9"/>
@@ -3159,8 +3552,11 @@
     <row r="81" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D81" s="4"/>
       <c r="E81" s="5"/>
+      <c r="I81" t="s">
+        <v>460</v>
+      </c>
       <c r="J81" s="9" t="s">
-        <v>346</v>
+        <v>312</v>
       </c>
       <c r="K81" s="9"/>
       <c r="L81" s="9"/>
@@ -3169,8 +3565,11 @@
     <row r="82" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D82" s="4"/>
       <c r="E82" s="5"/>
+      <c r="I82" t="s">
+        <v>462</v>
+      </c>
       <c r="J82" s="9" t="s">
-        <v>351</v>
+        <v>317</v>
       </c>
       <c r="K82" s="9"/>
       <c r="L82" s="9"/>
@@ -3180,7 +3579,7 @@
       <c r="D83" s="4"/>
       <c r="E83" s="5"/>
       <c r="J83" s="9" t="s">
-        <v>344</v>
+        <v>310</v>
       </c>
       <c r="K83" s="9"/>
       <c r="L83" s="9"/>
@@ -3194,10 +3593,10 @@
         <v>81</v>
       </c>
       <c r="H84" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="J84" t="s">
-        <v>221</v>
+        <v>191</v>
       </c>
       <c r="M84" s="5" t="s">
         <v>81</v>
@@ -3206,545 +3605,927 @@
     <row r="85" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D85" s="2"/>
       <c r="E85" s="3"/>
-      <c r="I85" t="s">
-        <v>177</v>
+      <c r="J85" t="s">
+        <v>194</v>
+      </c>
+      <c r="L85" t="s">
+        <v>263</v>
       </c>
       <c r="M85" s="3"/>
     </row>
-    <row r="86" spans="4:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D86" s="4" t="s">
+    <row r="86" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D86" s="15"/>
+      <c r="E86" s="16"/>
+      <c r="F86" t="s">
+        <v>356</v>
+      </c>
+      <c r="J86" t="s">
+        <v>378</v>
+      </c>
+      <c r="L86" t="s">
+        <v>387</v>
+      </c>
+      <c r="M86" s="3"/>
+    </row>
+    <row r="87" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D87" s="15"/>
+      <c r="E87" s="16"/>
+      <c r="F87" t="s">
+        <v>130</v>
+      </c>
+      <c r="G87" t="s">
+        <v>374</v>
+      </c>
+      <c r="H87" t="s">
+        <v>398</v>
+      </c>
+      <c r="J87" t="s">
+        <v>277</v>
+      </c>
+      <c r="L87" t="s">
+        <v>262</v>
+      </c>
+      <c r="M87" s="3"/>
+    </row>
+    <row r="88" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D88" s="15"/>
+      <c r="E88" s="16"/>
+      <c r="G88" t="s">
+        <v>373</v>
+      </c>
+      <c r="H88" t="s">
+        <v>337</v>
+      </c>
+      <c r="J88" t="s">
+        <v>379</v>
+      </c>
+      <c r="L88" t="s">
+        <v>388</v>
+      </c>
+      <c r="M88" s="3"/>
+    </row>
+    <row r="89" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D89" s="15"/>
+      <c r="E89" s="16"/>
+      <c r="F89" t="s">
+        <v>358</v>
+      </c>
+      <c r="H89" t="s">
+        <v>399</v>
+      </c>
+      <c r="J89" t="s">
+        <v>380</v>
+      </c>
+      <c r="L89" t="s">
+        <v>389</v>
+      </c>
+      <c r="M89" s="3"/>
+    </row>
+    <row r="90" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D90" s="15"/>
+      <c r="E90" s="16"/>
+      <c r="F90" t="s">
+        <v>357</v>
+      </c>
+      <c r="H90" t="s">
+        <v>400</v>
+      </c>
+      <c r="J90" t="s">
+        <v>381</v>
+      </c>
+      <c r="L90" t="s">
+        <v>390</v>
+      </c>
+      <c r="M90" s="3"/>
+    </row>
+    <row r="91" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D91" s="15"/>
+      <c r="E91" s="16"/>
+      <c r="H91" t="s">
+        <v>401</v>
+      </c>
+      <c r="J91" t="s">
+        <v>382</v>
+      </c>
+      <c r="L91" t="s">
+        <v>391</v>
+      </c>
+      <c r="M91" s="3"/>
+    </row>
+    <row r="92" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D92" s="15"/>
+      <c r="E92" s="16"/>
+      <c r="F92" t="s">
+        <v>363</v>
+      </c>
+      <c r="H92" t="s">
+        <v>402</v>
+      </c>
+      <c r="J92" t="s">
+        <v>195</v>
+      </c>
+      <c r="L92" t="s">
+        <v>392</v>
+      </c>
+      <c r="M92" s="3"/>
+    </row>
+    <row r="93" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D93" s="15"/>
+      <c r="E93" s="16"/>
+      <c r="H93" t="s">
+        <v>403</v>
+      </c>
+      <c r="J93" t="s">
+        <v>383</v>
+      </c>
+      <c r="L93" t="s">
+        <v>393</v>
+      </c>
+      <c r="M93" s="3"/>
+    </row>
+    <row r="94" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D94" s="15"/>
+      <c r="E94" s="16"/>
+      <c r="H94" t="s">
+        <v>148</v>
+      </c>
+      <c r="I94" t="s">
+        <v>463</v>
+      </c>
+      <c r="J94" t="s">
+        <v>384</v>
+      </c>
+      <c r="L94" t="s">
+        <v>394</v>
+      </c>
+      <c r="M94" s="3"/>
+    </row>
+    <row r="95" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D95" s="15"/>
+      <c r="E95" s="16"/>
+      <c r="H95" t="s">
+        <v>404</v>
+      </c>
+      <c r="I95" t="s">
+        <v>464</v>
+      </c>
+      <c r="J95" t="s">
+        <v>196</v>
+      </c>
+      <c r="L95" t="s">
+        <v>395</v>
+      </c>
+      <c r="M95" s="3"/>
+    </row>
+    <row r="96" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D96" s="15"/>
+      <c r="E96" s="16"/>
+      <c r="H96" t="s">
+        <v>405</v>
+      </c>
+      <c r="I96" t="s">
+        <v>465</v>
+      </c>
+      <c r="J96" t="s">
+        <v>385</v>
+      </c>
+      <c r="L96" t="s">
+        <v>396</v>
+      </c>
+      <c r="M96" s="3"/>
+    </row>
+    <row r="97" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D97" s="15"/>
+      <c r="E97" s="16"/>
+      <c r="H97" t="s">
+        <v>406</v>
+      </c>
+      <c r="I97" t="s">
+        <v>466</v>
+      </c>
+      <c r="J97" t="s">
+        <v>386</v>
+      </c>
+      <c r="L97" t="s">
+        <v>397</v>
+      </c>
+      <c r="M97" s="3"/>
+    </row>
+    <row r="98" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D98" s="15"/>
+      <c r="E98" s="16"/>
+      <c r="F98" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="H98" t="s">
+        <v>407</v>
+      </c>
+      <c r="I98" t="s">
+        <v>467</v>
+      </c>
+      <c r="J98" t="s">
+        <v>413</v>
+      </c>
+      <c r="M98" s="3"/>
+    </row>
+    <row r="99" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D99" s="15"/>
+      <c r="E99" s="16"/>
+      <c r="F99" t="s">
+        <v>361</v>
+      </c>
+      <c r="H99" t="s">
+        <v>408</v>
+      </c>
+      <c r="J99" t="s">
+        <v>192</v>
+      </c>
+      <c r="M99" s="3"/>
+    </row>
+    <row r="100" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D100" s="15"/>
+      <c r="E100" s="16"/>
+      <c r="F100" t="s">
+        <v>362</v>
+      </c>
+      <c r="H100" t="s">
+        <v>410</v>
+      </c>
+      <c r="I100" t="s">
+        <v>468</v>
+      </c>
+      <c r="M100" s="3"/>
+    </row>
+    <row r="101" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D101" s="15"/>
+      <c r="E101" s="16"/>
+      <c r="F101" t="s">
+        <v>359</v>
+      </c>
+      <c r="G101" t="s">
+        <v>376</v>
+      </c>
+      <c r="H101" t="s">
+        <v>409</v>
+      </c>
+      <c r="I101" t="s">
+        <v>469</v>
+      </c>
+      <c r="J101" t="s">
+        <v>414</v>
+      </c>
+      <c r="M101" s="3"/>
+    </row>
+    <row r="102" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D102" s="15"/>
+      <c r="E102" s="16"/>
+      <c r="F102" t="s">
+        <v>364</v>
+      </c>
+      <c r="H102" t="s">
+        <v>411</v>
+      </c>
+      <c r="I102" t="s">
+        <v>470</v>
+      </c>
+      <c r="J102" t="s">
+        <v>415</v>
+      </c>
+      <c r="M102" s="3"/>
+    </row>
+    <row r="103" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D103" s="15"/>
+      <c r="E103" s="16"/>
+      <c r="F103" t="s">
+        <v>365</v>
+      </c>
+      <c r="G103" t="s">
+        <v>375</v>
+      </c>
+      <c r="H103" t="s">
+        <v>412</v>
+      </c>
+      <c r="I103" t="s">
+        <v>471</v>
+      </c>
+      <c r="J103" t="s">
+        <v>193</v>
+      </c>
+      <c r="M103" s="3"/>
+    </row>
+    <row r="104" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D104" s="15"/>
+      <c r="E104" s="16"/>
+      <c r="F104" t="s">
+        <v>366</v>
+      </c>
+      <c r="I104" t="s">
+        <v>472</v>
+      </c>
+      <c r="J104" t="s">
+        <v>416</v>
+      </c>
+      <c r="M104" s="3"/>
+    </row>
+    <row r="105" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D105" s="15"/>
+      <c r="E105" s="16"/>
+      <c r="I105" t="s">
+        <v>473</v>
+      </c>
+      <c r="J105" t="s">
+        <v>417</v>
+      </c>
+      <c r="M105" s="3"/>
+    </row>
+    <row r="106" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D106" s="15"/>
+      <c r="E106" s="16"/>
+      <c r="F106" t="s">
+        <v>367</v>
+      </c>
+      <c r="I106" t="s">
+        <v>474</v>
+      </c>
+      <c r="J106" t="s">
+        <v>418</v>
+      </c>
+      <c r="M106" s="3"/>
+    </row>
+    <row r="107" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D107" s="15"/>
+      <c r="E107" s="16"/>
+      <c r="F107" s="16" t="s">
+        <v>371</v>
+      </c>
+      <c r="I107" t="s">
+        <v>475</v>
+      </c>
+      <c r="J107" t="s">
+        <v>419</v>
+      </c>
+      <c r="M107" s="3"/>
+    </row>
+    <row r="108" spans="4:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D108" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E86" s="5" t="s">
+      <c r="E108" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="F86" s="9" t="s">
+      <c r="F108" s="9" t="s">
+        <v>369</v>
+      </c>
+      <c r="G108" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="I108" t="s">
+        <v>476</v>
+      </c>
+      <c r="J108" t="s">
+        <v>420</v>
+      </c>
+      <c r="L108" s="9"/>
+      <c r="M108" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="109" spans="4:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D109" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E109" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F109" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="G109" s="9"/>
+      <c r="I109" t="s">
+        <v>477</v>
+      </c>
+      <c r="J109" t="s">
+        <v>421</v>
+      </c>
+      <c r="M109" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="110" spans="4:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D110" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E110" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F110" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="G110" s="9"/>
+      <c r="H110" t="s">
+        <v>148</v>
+      </c>
+      <c r="I110" s="9" t="s">
+        <v>478</v>
+      </c>
+      <c r="J110" t="s">
+        <v>422</v>
+      </c>
+      <c r="M110" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="111" spans="4:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D111" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E111" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F111" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="G111" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="H111" t="s">
+        <v>149</v>
+      </c>
+      <c r="I111" t="s">
+        <v>479</v>
+      </c>
+      <c r="M111" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="112" spans="4:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D112" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E112" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G112" t="s">
+        <v>296</v>
+      </c>
+      <c r="I112" t="s">
+        <v>480</v>
+      </c>
+      <c r="K112" t="s">
+        <v>232</v>
+      </c>
+      <c r="M112" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="113" spans="4:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D113" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E113" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="G113" t="s">
+        <v>295</v>
+      </c>
+      <c r="I113" t="s">
+        <v>481</v>
+      </c>
+      <c r="M113" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="114" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D114" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E114" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F114" s="9"/>
+      <c r="G114" s="9"/>
+      <c r="I114" t="s">
+        <v>482</v>
+      </c>
+      <c r="M114" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="115" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D115" s="2"/>
+      <c r="E115" s="3"/>
+      <c r="H115" t="s">
+        <v>338</v>
+      </c>
+      <c r="I115" t="s">
+        <v>483</v>
+      </c>
+      <c r="M115" s="3"/>
+    </row>
+    <row r="116" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D116" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E116" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F116" t="s">
         <v>131</v>
       </c>
-      <c r="G86" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="J86" t="s">
-        <v>222</v>
-      </c>
-      <c r="L86" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="M86" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="87" spans="4:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D87" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E87" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F87" s="9" t="s">
+      <c r="G116" t="s">
+        <v>142</v>
+      </c>
+      <c r="H116" t="s">
+        <v>337</v>
+      </c>
+      <c r="I116" t="s">
+        <v>484</v>
+      </c>
+      <c r="J116" t="s">
+        <v>197</v>
+      </c>
+      <c r="K116" t="s">
+        <v>246</v>
+      </c>
+      <c r="M116" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="117" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D117" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E117" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="H117" t="s">
+        <v>339</v>
+      </c>
+      <c r="I117" t="s">
+        <v>485</v>
+      </c>
+      <c r="M117" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="118" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D118" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E118" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="I118" t="s">
+        <v>486</v>
+      </c>
+      <c r="J118" t="s">
+        <v>198</v>
+      </c>
+      <c r="K118" t="s">
+        <v>233</v>
+      </c>
+      <c r="M118" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="119" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D119" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E119" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F119" t="s">
+        <v>271</v>
+      </c>
+      <c r="H119" t="s">
+        <v>340</v>
+      </c>
+      <c r="J119" t="s">
+        <v>199</v>
+      </c>
+      <c r="K119" t="s">
+        <v>234</v>
+      </c>
+      <c r="L119" t="s">
+        <v>264</v>
+      </c>
+      <c r="M119" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="120" spans="4:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D120" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E120" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="H120" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="I120" t="s">
+        <v>487</v>
+      </c>
+      <c r="M120" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="121" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D121" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E121" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="H121" t="s">
+        <v>342</v>
+      </c>
+      <c r="I121" t="s">
+        <v>488</v>
+      </c>
+      <c r="J121" t="s">
+        <v>200</v>
+      </c>
+      <c r="M121" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="122" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D122" s="2"/>
+      <c r="E122" s="3"/>
+      <c r="I122" t="s">
+        <v>489</v>
+      </c>
+      <c r="M122" s="3"/>
+    </row>
+    <row r="123" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D123" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E123" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I123" t="s">
+        <v>490</v>
+      </c>
+      <c r="M123" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="124" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D124" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E124" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F124" t="s">
+        <v>245</v>
+      </c>
+      <c r="G124" t="s">
+        <v>298</v>
+      </c>
+      <c r="H124" t="s">
+        <v>343</v>
+      </c>
+      <c r="I124" t="s">
+        <v>491</v>
+      </c>
+      <c r="J124" t="s">
+        <v>201</v>
+      </c>
+      <c r="K124" t="s">
+        <v>235</v>
+      </c>
+      <c r="L124" t="s">
+        <v>267</v>
+      </c>
+      <c r="M124" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="125" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D125" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E125" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F125" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="G125" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="I125" t="s">
+        <v>492</v>
+      </c>
+      <c r="J125" t="s">
+        <v>202</v>
+      </c>
+      <c r="K125" t="s">
+        <v>236</v>
+      </c>
+      <c r="L125" t="s">
+        <v>265</v>
+      </c>
+      <c r="M125" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="126" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D126" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E126" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="H126" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="I126" s="9" t="s">
+        <v>493</v>
+      </c>
+      <c r="J126" t="s">
+        <v>203</v>
+      </c>
+      <c r="K126" t="s">
+        <v>237</v>
+      </c>
+      <c r="M126" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="127" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D127" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E127" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F127" t="s">
         <v>132</v>
       </c>
-      <c r="G87" s="9"/>
-      <c r="J87" t="s">
-        <v>223</v>
-      </c>
-      <c r="L87" t="s">
-        <v>296</v>
-      </c>
-      <c r="M87" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="88" spans="4:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D88" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E88" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="F88" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="G88" s="9"/>
-      <c r="H88" t="s">
+      <c r="H127" t="s">
+        <v>345</v>
+      </c>
+      <c r="I127" s="9" t="s">
+        <v>494</v>
+      </c>
+      <c r="K127" t="s">
+        <v>238</v>
+      </c>
+      <c r="L127" t="s">
+        <v>266</v>
+      </c>
+      <c r="M127" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="128" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="L128" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="129" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F129" t="s">
+        <v>288</v>
+      </c>
+      <c r="H129" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="130" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="J130" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="132" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="J132" t="s">
+        <v>318</v>
+      </c>
+      <c r="K132" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="133" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="J133" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="134" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="J134" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="135" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="J135" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="136" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="J136" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="137" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="J137" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="138" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="I138" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="139" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="I139" t="s">
         <v>155</v>
       </c>
-      <c r="I88" s="9" t="s">
-        <v>277</v>
-      </c>
-      <c r="J88" t="s">
-        <v>311</v>
-      </c>
-      <c r="M88" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="89" spans="4:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D89" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E89" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F89" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="G89" s="9" t="s">
-        <v>331</v>
-      </c>
-      <c r="H89" t="s">
+    </row>
+    <row r="141" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="I141" t="s">
         <v>156</v>
       </c>
-      <c r="J89" t="s">
-        <v>224</v>
-      </c>
-      <c r="L89" t="s">
-        <v>297</v>
-      </c>
-      <c r="M89" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="90" spans="4:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D90" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E90" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F90" t="s">
-        <v>135</v>
-      </c>
-      <c r="G90" t="s">
-        <v>330</v>
-      </c>
-      <c r="I90" t="s">
-        <v>178</v>
-      </c>
-      <c r="J90" t="s">
-        <v>225</v>
-      </c>
-      <c r="K90" t="s">
-        <v>263</v>
-      </c>
-      <c r="M90" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="91" spans="4:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D91" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E91" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F91" t="s">
-        <v>136</v>
-      </c>
-      <c r="G91" t="s">
-        <v>329</v>
-      </c>
-      <c r="I91" t="s">
-        <v>179</v>
-      </c>
-      <c r="J91" t="s">
-        <v>226</v>
-      </c>
-      <c r="M91" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="92" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D92" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E92" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="F92" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="G92" s="9"/>
-      <c r="I92" t="s">
-        <v>180</v>
-      </c>
-      <c r="J92" t="s">
-        <v>227</v>
-      </c>
-      <c r="M92" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="93" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D93" s="2"/>
-      <c r="E93" s="3"/>
-      <c r="H93" t="s">
-        <v>372</v>
-      </c>
-      <c r="I93" t="s">
-        <v>279</v>
-      </c>
-      <c r="M93" s="3"/>
-    </row>
-    <row r="94" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D94" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E94" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="F94" t="s">
-        <v>138</v>
-      </c>
-      <c r="G94" t="s">
-        <v>149</v>
-      </c>
-      <c r="H94" t="s">
-        <v>371</v>
-      </c>
-      <c r="I94" t="s">
-        <v>181</v>
-      </c>
-      <c r="J94" t="s">
-        <v>228</v>
-      </c>
-      <c r="K94" t="s">
-        <v>278</v>
-      </c>
-      <c r="M94" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="95" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D95" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E95" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="H95" t="s">
-        <v>373</v>
-      </c>
-      <c r="M95" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="96" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D96" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E96" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="I96" t="s">
-        <v>182</v>
-      </c>
-      <c r="J96" t="s">
-        <v>229</v>
-      </c>
-      <c r="K96" t="s">
-        <v>264</v>
-      </c>
-      <c r="M96" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="97" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D97" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E97" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="F97" t="s">
-        <v>305</v>
-      </c>
-      <c r="H97" t="s">
-        <v>374</v>
-      </c>
-      <c r="I97" t="s">
-        <v>183</v>
-      </c>
-      <c r="J97" t="s">
-        <v>230</v>
-      </c>
-      <c r="K97" t="s">
-        <v>265</v>
-      </c>
-      <c r="L97" t="s">
-        <v>298</v>
-      </c>
-      <c r="M97" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="98" spans="4:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D98" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E98" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="H98" s="9" t="s">
-        <v>375</v>
-      </c>
-      <c r="M98" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="99" spans="4:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D99" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E99" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="H99" t="s">
-        <v>376</v>
-      </c>
-      <c r="I99" t="s">
-        <v>184</v>
-      </c>
-      <c r="J99" t="s">
-        <v>231</v>
-      </c>
-      <c r="M99" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="100" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D100" s="2"/>
-      <c r="E100" s="3"/>
-      <c r="I100" t="s">
-        <v>314</v>
-      </c>
-      <c r="M100" s="3"/>
-    </row>
-    <row r="101" spans="4:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D101" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="E101" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="M101" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="102" spans="4:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D102" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="E102" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="F102" t="s">
-        <v>276</v>
-      </c>
-      <c r="G102" t="s">
-        <v>332</v>
-      </c>
-      <c r="H102" t="s">
-        <v>377</v>
-      </c>
-      <c r="J102" t="s">
-        <v>232</v>
-      </c>
-      <c r="K102" t="s">
-        <v>266</v>
-      </c>
-      <c r="L102" t="s">
-        <v>301</v>
-      </c>
-      <c r="M102" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="103" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D103" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="E103" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="F103" s="9" t="s">
-        <v>275</v>
-      </c>
-      <c r="G103" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="J103" t="s">
-        <v>233</v>
-      </c>
-      <c r="K103" t="s">
-        <v>267</v>
-      </c>
-      <c r="L103" t="s">
-        <v>299</v>
-      </c>
-      <c r="M103" s="5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="104" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D104" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="E104" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="H104" s="9" t="s">
-        <v>378</v>
-      </c>
-      <c r="I104" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="J104" t="s">
-        <v>234</v>
-      </c>
-      <c r="K104" t="s">
-        <v>268</v>
-      </c>
-      <c r="M104" s="5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="105" spans="4:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D105" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="E105" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="F105" t="s">
-        <v>139</v>
-      </c>
-      <c r="H105" t="s">
-        <v>379</v>
-      </c>
-      <c r="I105" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="K105" t="s">
-        <v>269</v>
-      </c>
-      <c r="L105" t="s">
-        <v>300</v>
-      </c>
-      <c r="M105" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="106" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="L106" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="107" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="F107" t="s">
-        <v>322</v>
-      </c>
-      <c r="H107" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="108" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="J108" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="110" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="J110" t="s">
-        <v>352</v>
-      </c>
-      <c r="K110" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="111" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="J111" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="112" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="J112" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="113" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J113" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="114" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J114" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="115" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J115" t="s">
-        <v>357</v>
+    </row>
+    <row r="142" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="I142" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="146" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I146" s="9" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="147" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I147" s="9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="152" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I152" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="153" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I153" t="s">
+        <v>496</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F89" r:id="rId1" xr:uid="{271D87EF-FE75-4435-92F0-B7C42F80D97B}"/>
-    <hyperlink ref="F92" r:id="rId2" xr:uid="{D1B3712C-9998-452C-A666-F08A0C006BA6}"/>
-    <hyperlink ref="F12" r:id="rId3" xr:uid="{D2F7C913-C7F7-4312-8F91-1AA5D7271530}"/>
-    <hyperlink ref="F11" r:id="rId4" xr:uid="{2A4AF34E-315F-4EDD-8729-D0E1F5DF7C57}"/>
-    <hyperlink ref="F22" r:id="rId5" xr:uid="{942D8DE3-DFD7-46BC-976E-6F2F4FCC9D02}"/>
-    <hyperlink ref="F27" r:id="rId6" xr:uid="{3FB93EA1-EE6D-4F02-9FD5-A05F7DDDB7D1}"/>
-    <hyperlink ref="F32" r:id="rId7" xr:uid="{25D4F6C4-B46F-497B-BF24-33C9AC171B81}"/>
-    <hyperlink ref="F34" r:id="rId8" xr:uid="{39833C68-0968-45C8-8399-2B41E42C29A0}"/>
-    <hyperlink ref="F39" r:id="rId9" xr:uid="{7D306272-7814-4438-BA51-7EC4EC0A0263}"/>
-    <hyperlink ref="F40" r:id="rId10" xr:uid="{1708FE19-42CF-439F-A054-74076BDCFB31}"/>
-    <hyperlink ref="F41" r:id="rId11" xr:uid="{6EC2A991-B639-4F28-B084-7FD868EBC97B}"/>
-    <hyperlink ref="F44" r:id="rId12" xr:uid="{C660C1FA-F167-4FFA-BD40-731399EAEFE3}"/>
-    <hyperlink ref="F47" r:id="rId13" xr:uid="{BDD0178F-0648-4572-A133-A5E735F9A719}"/>
-    <hyperlink ref="F49" r:id="rId14" xr:uid="{A6E53AAA-1E50-4090-B34B-9F87DB2CE138}"/>
-    <hyperlink ref="F50" r:id="rId15" xr:uid="{F1340F25-1CE1-4A96-AB21-10821F8050FA}"/>
-    <hyperlink ref="F57" r:id="rId16" xr:uid="{B87BED42-9B54-4B78-9DEB-BD28B530DA1B}"/>
-    <hyperlink ref="F61" r:id="rId17" xr:uid="{9D4DB46C-D914-46AE-8B8E-CC1C300FDA98}"/>
-    <hyperlink ref="F86" r:id="rId18" xr:uid="{AC0778F0-1F7B-41B3-813B-1245E10BFE52}"/>
-    <hyperlink ref="F7" r:id="rId19" xr:uid="{387C584A-278C-450E-820B-6D592CD9B542}"/>
-    <hyperlink ref="F8" r:id="rId20" xr:uid="{231440AF-B43B-4790-9E97-F51A5021CA9A}"/>
-    <hyperlink ref="F9" r:id="rId21" xr:uid="{75397D25-F535-4596-87C1-6CE4AF75CB9C}"/>
-    <hyperlink ref="F88" r:id="rId22" xr:uid="{AE505ADC-5D84-4887-8B45-D1B047108302}"/>
-    <hyperlink ref="F87" r:id="rId23" xr:uid="{4B851A94-480D-4562-A61A-EB57C6B36F7F}"/>
-    <hyperlink ref="I71" r:id="rId24" display="https://www.ozon.ru/product/makfa-lyubitelskaya-vermishel-dlinnaya-spagetti-500-g-140800360/?asb=PiXAxdUD%252Fb8Q6qcfNBYgYZSa74CfvsYST7VXIKCqsI4%253D&amp;asb2=oFSDihkMWoB8nWmHdebLJHz0vIatpYbUNfq2HRXzEndDi0EfZLepBYnsQxQRgmua&amp;ectx=1&amp;keywords=%D0%BC%D0%B0%D0%BA%D1%84%D0%B0&amp;miniapp=supermarket&amp;sh=K5xV8WIg-g" xr:uid="{E76EC934-5688-487D-8CEB-7EECD8297302}"/>
-    <hyperlink ref="I9" r:id="rId25" display="https://www.ozon.ru/product/pelmeni-imperator-tsezar-zamorozhennye-800-g-360092984/?asb=qjxJOzyaP5eiIp3dFFhocI2vC%252B0BwHzNexEcZ6ME9vI%253D&amp;asb2=kIq6DZcBFl2HVot5SyrOtbinVyUMRC8Yhi57ws0_MSIKiAv1lBgKMWLbe0sKN4G1&amp;ectx=1&amp;keywords=%D1%86%D0%B5%D0%B7%D0%B0%D1%80%D1%8C&amp;miniapp=supermarket&amp;sh=K5xV8Uep1Q" xr:uid="{2ECD4382-FE90-4913-80D1-5C2CD19FDA74}"/>
-    <hyperlink ref="I10" r:id="rId26" xr:uid="{715D8978-E09F-4537-A640-856992E7F8CB}"/>
-    <hyperlink ref="I105" r:id="rId27" display="https://www.ozon.ru/product/syr-brest-litovsk-klassicheskiy-45-150-g-152141663/?asb=Tdv9tczfDa0PTKhltcp1Q6PBJg4kEMxiQyThzh5iKbU%253D&amp;asb2=gf9xWzcVUAeRvGgIa54q929unGEPpy48EadGcnul4r-wPb6gcWYx1GFdDzqUI3ln&amp;ectx=1&amp;keywords=%D0%91%D1%80%D0%B5%D1%81%D1%82+%D0%9B%D0%B8%D1%82%D0%BE%D0%B2%D1%81%D0%BA&amp;miniapp=supermarket&amp;sh=K5xV8Y4_HQ" xr:uid="{EA030594-B44A-4F70-BE65-1EAA753D15CB}"/>
-    <hyperlink ref="I104" r:id="rId28" display="https://www.ozon.ru/product/brest-litovsk-maslo-sladko-slivochnoe-nesolenoe-82-5-180-g-145923184/?asb=jIkcWaZ8F2DraHiq9EkWSqHPHpJGeby2dptq6D3zZMw%253D&amp;asb2=jU54E3oIkNKIgSViutQjlT_4Mgd1c3ms7hb00oP7TOiu8wiJapREib7WfJBxMz2F&amp;ectx=1&amp;keywords=%D0%91%D1%80%D0%B5%D1%81%D1%82+%D0%9B%D0%B8%D1%82%D0%BE%D0%B2%D1%81%D0%BA&amp;miniapp=supermarket&amp;sh=K5xV8Xe3Fg" xr:uid="{B8E2B196-F6B7-4B8D-B1DC-360FE9199845}"/>
-    <hyperlink ref="H9" r:id="rId29" xr:uid="{018BC0E8-7D36-4FDC-B01F-961CF1BAB866}"/>
-    <hyperlink ref="G7" r:id="rId30" display="https://lavka.yandex.ru/213/good/b01a29d7997948658686098667c64a1e000300010000?searchQuery=%D0%A6%D0%B5%D0%B7%D0%B0%D1%80%D1%8C%20%D0%B3%D0%BE%D1%81%D1%83%D0%B4%D0%B0%D1%80%D1%8C%20%D0%B8%D0%BC%D0%BF%D0%B5%D1%80%D0%B0%D1%82%D0%BE%D1%80%20800%20%D0%B3&amp;searchPosition=-1" xr:uid="{E1D5F1F2-7D41-4892-BB76-421E3FAE8527}"/>
-    <hyperlink ref="G12" r:id="rId31" xr:uid="{AF577DF4-4728-48AF-A65A-2285548B425E}"/>
-    <hyperlink ref="J43" r:id="rId32" xr:uid="{7B711258-2660-4291-8B28-70B42D0DCF9C}"/>
-    <hyperlink ref="J51" r:id="rId33" xr:uid="{C121E486-6DC5-4AB8-BDD6-D4F32794A3A4}"/>
-    <hyperlink ref="J70" r:id="rId34" xr:uid="{7F316388-2C20-4908-B372-14903C2E8EAA}"/>
-    <hyperlink ref="J74" r:id="rId35" xr:uid="{851CBC7D-F6E3-4C94-816D-5E4B54BC54F2}"/>
-    <hyperlink ref="K12" r:id="rId36" xr:uid="{06AD9E37-3909-452B-AF07-1A08C94977D7}"/>
-    <hyperlink ref="K47" r:id="rId37" xr:uid="{96CAC567-3F0E-49CA-8DEC-F36C45823856}"/>
-    <hyperlink ref="J61" r:id="rId38" xr:uid="{159BA102-A07E-4CCA-B39C-0649E37DABAB}"/>
-    <hyperlink ref="F64" r:id="rId39" xr:uid="{02308EB3-0D4F-43E5-B4E2-B6F6C09AEFBB}"/>
-    <hyperlink ref="K7" r:id="rId40" xr:uid="{12963AA2-BE9C-48F6-ADD3-656C6E23B39C}"/>
-    <hyperlink ref="H49" r:id="rId41" xr:uid="{8E5E12B2-C9E3-4CE9-A709-1339EBF59243}"/>
-    <hyperlink ref="K10" r:id="rId42" xr:uid="{A00C7BE9-6CBD-4A4B-AB12-2C62A70BE084}"/>
-    <hyperlink ref="K59" r:id="rId43" xr:uid="{7593D602-EECA-4B89-A6ED-6CF677EB1C0D}"/>
-    <hyperlink ref="K73" r:id="rId44" xr:uid="{46977EFB-3B7E-4A69-822A-E021388A83CE}"/>
-    <hyperlink ref="L64" r:id="rId45" xr:uid="{A6E2704C-7779-416A-BF8F-0168747F4B17}"/>
-    <hyperlink ref="J9" r:id="rId46" xr:uid="{008C7D2B-E38E-4E27-B175-93EF66E5BA88}"/>
-    <hyperlink ref="J69" r:id="rId47" xr:uid="{4039C487-EB12-4F7C-9DE7-06EA042FFD2D}"/>
-    <hyperlink ref="J78" r:id="rId48" xr:uid="{6B7D29C3-52C4-4049-AA04-92C5CACA0D6B}"/>
-    <hyperlink ref="H98" r:id="rId49" xr:uid="{43050494-654D-45F2-AE59-7C5313A00FC2}"/>
-    <hyperlink ref="H104" r:id="rId50" xr:uid="{E230078A-0B3B-4E54-9A65-52FAB8048042}"/>
-    <hyperlink ref="L7" r:id="rId51" xr:uid="{3F898277-AC53-489C-B199-74F51F108BD6}"/>
-    <hyperlink ref="L86" r:id="rId52" xr:uid="{32241EFA-8502-4F0D-9CC4-A1E387DB2156}"/>
-    <hyperlink ref="G8" r:id="rId53" xr:uid="{325A37C3-627C-4F5D-B64E-A86B62410868}"/>
-    <hyperlink ref="G14" r:id="rId54" xr:uid="{CCF9626F-2EE9-4956-84D6-5829E2F596AE}"/>
+    <hyperlink ref="F12" r:id="rId1" xr:uid="{D2F7C913-C7F7-4312-8F91-1AA5D7271530}"/>
+    <hyperlink ref="F11" r:id="rId2" xr:uid="{2A4AF34E-315F-4EDD-8729-D0E1F5DF7C57}"/>
+    <hyperlink ref="F22" r:id="rId3" xr:uid="{942D8DE3-DFD7-46BC-976E-6F2F4FCC9D02}"/>
+    <hyperlink ref="F27" r:id="rId4" xr:uid="{3FB93EA1-EE6D-4F02-9FD5-A05F7DDDB7D1}"/>
+    <hyperlink ref="F32" r:id="rId5" xr:uid="{25D4F6C4-B46F-497B-BF24-33C9AC171B81}"/>
+    <hyperlink ref="F34" r:id="rId6" xr:uid="{39833C68-0968-45C8-8399-2B41E42C29A0}"/>
+    <hyperlink ref="F39" r:id="rId7" xr:uid="{7D306272-7814-4438-BA51-7EC4EC0A0263}"/>
+    <hyperlink ref="F40" r:id="rId8" xr:uid="{1708FE19-42CF-439F-A054-74076BDCFB31}"/>
+    <hyperlink ref="F41" r:id="rId9" xr:uid="{6EC2A991-B639-4F28-B084-7FD868EBC97B}"/>
+    <hyperlink ref="F44" r:id="rId10" xr:uid="{C660C1FA-F167-4FFA-BD40-731399EAEFE3}"/>
+    <hyperlink ref="F47" r:id="rId11" xr:uid="{BDD0178F-0648-4572-A133-A5E735F9A719}"/>
+    <hyperlink ref="F49" r:id="rId12" xr:uid="{A6E53AAA-1E50-4090-B34B-9F87DB2CE138}"/>
+    <hyperlink ref="F50" r:id="rId13" xr:uid="{F1340F25-1CE1-4A96-AB21-10821F8050FA}"/>
+    <hyperlink ref="F57" r:id="rId14" xr:uid="{B87BED42-9B54-4B78-9DEB-BD28B530DA1B}"/>
+    <hyperlink ref="F61" r:id="rId15" xr:uid="{9D4DB46C-D914-46AE-8B8E-CC1C300FDA98}"/>
+    <hyperlink ref="F7" r:id="rId16" xr:uid="{387C584A-278C-450E-820B-6D592CD9B542}"/>
+    <hyperlink ref="F8" r:id="rId17" xr:uid="{231440AF-B43B-4790-9E97-F51A5021CA9A}"/>
+    <hyperlink ref="F9" r:id="rId18" xr:uid="{75397D25-F535-4596-87C1-6CE4AF75CB9C}"/>
+    <hyperlink ref="I9" r:id="rId19" display="https://www.ozon.ru/product/pelmeni-imperator-tsezar-zamorozhennye-800-g-360092984/?asb=qjxJOzyaP5eiIp3dFFhocI2vC%252B0BwHzNexEcZ6ME9vI%253D&amp;asb2=kIq6DZcBFl2HVot5SyrOtbinVyUMRC8Yhi57ws0_MSIKiAv1lBgKMWLbe0sKN4G1&amp;ectx=1&amp;keywords=%D1%86%D0%B5%D0%B7%D0%B0%D1%80%D1%8C&amp;miniapp=supermarket&amp;sh=K5xV8Uep1Q" xr:uid="{2ECD4382-FE90-4913-80D1-5C2CD19FDA74}"/>
+    <hyperlink ref="H9" r:id="rId20" xr:uid="{018BC0E8-7D36-4FDC-B01F-961CF1BAB866}"/>
+    <hyperlink ref="G7" r:id="rId21" display="https://lavka.yandex.ru/213/good/b01a29d7997948658686098667c64a1e000300010000?searchQuery=%D0%A6%D0%B5%D0%B7%D0%B0%D1%80%D1%8C%20%D0%B3%D0%BE%D1%81%D1%83%D0%B4%D0%B0%D1%80%D1%8C%20%D0%B8%D0%BC%D0%BF%D0%B5%D1%80%D0%B0%D1%82%D0%BE%D1%80%20800%20%D0%B3&amp;searchPosition=-1" xr:uid="{E1D5F1F2-7D41-4892-BB76-421E3FAE8527}"/>
+    <hyperlink ref="G12" r:id="rId22" xr:uid="{AF577DF4-4728-48AF-A65A-2285548B425E}"/>
+    <hyperlink ref="J43" r:id="rId23" xr:uid="{7B711258-2660-4291-8B28-70B42D0DCF9C}"/>
+    <hyperlink ref="J51" r:id="rId24" xr:uid="{C121E486-6DC5-4AB8-BDD6-D4F32794A3A4}"/>
+    <hyperlink ref="J70" r:id="rId25" xr:uid="{7F316388-2C20-4908-B372-14903C2E8EAA}"/>
+    <hyperlink ref="J74" r:id="rId26" xr:uid="{851CBC7D-F6E3-4C94-816D-5E4B54BC54F2}"/>
+    <hyperlink ref="K12" r:id="rId27" xr:uid="{06AD9E37-3909-452B-AF07-1A08C94977D7}"/>
+    <hyperlink ref="K47" r:id="rId28" xr:uid="{96CAC567-3F0E-49CA-8DEC-F36C45823856}"/>
+    <hyperlink ref="J61" r:id="rId29" xr:uid="{159BA102-A07E-4CCA-B39C-0649E37DABAB}"/>
+    <hyperlink ref="F64" r:id="rId30" xr:uid="{02308EB3-0D4F-43E5-B4E2-B6F6C09AEFBB}"/>
+    <hyperlink ref="K7" r:id="rId31" xr:uid="{12963AA2-BE9C-48F6-ADD3-656C6E23B39C}"/>
+    <hyperlink ref="H49" r:id="rId32" xr:uid="{8E5E12B2-C9E3-4CE9-A709-1339EBF59243}"/>
+    <hyperlink ref="K10" r:id="rId33" xr:uid="{A00C7BE9-6CBD-4A4B-AB12-2C62A70BE084}"/>
+    <hyperlink ref="K59" r:id="rId34" xr:uid="{7593D602-EECA-4B89-A6ED-6CF677EB1C0D}"/>
+    <hyperlink ref="K73" r:id="rId35" xr:uid="{46977EFB-3B7E-4A69-822A-E021388A83CE}"/>
+    <hyperlink ref="L64" r:id="rId36" xr:uid="{A6E2704C-7779-416A-BF8F-0168747F4B17}"/>
+    <hyperlink ref="J9" r:id="rId37" xr:uid="{008C7D2B-E38E-4E27-B175-93EF66E5BA88}"/>
+    <hyperlink ref="J69" r:id="rId38" xr:uid="{4039C487-EB12-4F7C-9DE7-06EA042FFD2D}"/>
+    <hyperlink ref="J78" r:id="rId39" xr:uid="{6B7D29C3-52C4-4049-AA04-92C5CACA0D6B}"/>
+    <hyperlink ref="H120" r:id="rId40" xr:uid="{43050494-654D-45F2-AE59-7C5313A00FC2}"/>
+    <hyperlink ref="H126" r:id="rId41" xr:uid="{E230078A-0B3B-4E54-9A65-52FAB8048042}"/>
+    <hyperlink ref="L7" r:id="rId42" xr:uid="{3F898277-AC53-489C-B199-74F51F108BD6}"/>
+    <hyperlink ref="G8" r:id="rId43" xr:uid="{325A37C3-627C-4F5D-B64E-A86B62410868}"/>
+    <hyperlink ref="G14" r:id="rId44" xr:uid="{CCF9626F-2EE9-4956-84D6-5829E2F596AE}"/>
+    <hyperlink ref="F98" r:id="rId45" xr:uid="{ADF34D2C-186D-4EF7-8C0F-3899A4CACEB7}"/>
+    <hyperlink ref="I147" r:id="rId46" display="https://www.ozon.ru/product/syr-brest-litovsk-klassicheskiy-45-150-g-152141663/?asb=Tdv9tczfDa0PTKhltcp1Q6PBJg4kEMxiQyThzh5iKbU%253D&amp;asb2=gf9xWzcVUAeRvGgIa54q929unGEPpy48EadGcnul4r-wPb6gcWYx1GFdDzqUI3ln&amp;ectx=1&amp;keywords=%D0%91%D1%80%D0%B5%D1%81%D1%82+%D0%9B%D0%B8%D1%82%D0%BE%D0%B2%D1%81%D0%BA&amp;miniapp=supermarket&amp;sh=K5xV8Y4_HQ" xr:uid="{07F26A86-F6D3-445F-8E13-AF46AB30C0A2}"/>
+    <hyperlink ref="I10" r:id="rId47" display="https://www.ozon.ru/product/testo-sloenoe-bezdrozhzhevoe-morozko-400-g-483915621/?asb=lS%252FDdgWY7qcQ8QLDKyjchUkhgLK7ishgApYHBHjA0WU%253D&amp;asb2=bSo5EOa9Q-T0hzu9qCojO1Gx50VQ8tY40e5Gcy43d_L0B-Nr45fAevSLKm9iueIi&amp;ectx=1&amp;keywords=%D0%BC%D0%BE%D1%80%D0%BE%D0%B7%D0%BA%D0%BE+%D1%82%D0%B5%D1%81%D1%82%D0%BE&amp;miniapp=supermarket&amp;sh=K5xV8SetZA" xr:uid="{60FC73D1-007F-4DE0-9F0A-9DECB05956F5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId55"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId48"/>
 </worksheet>
 </file>
</xml_diff>